<commit_message>
Added us core v8.0.0 requirements. In the processes, noted some necessary changes to the v7.0.0 and v6.1.0 requirements. Updated these, regenerated the csv file, and regenerated the coverage file.
</commit_message>
<xml_diff>
--- a/lib/us_core_test_kit/requirements/hl7.fhir.us.core_6.1.0_reqs.xlsx
+++ b/lib/us_core_test_kit/requirements/hl7.fhir.us.core_6.1.0_reqs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/knaden/Documents/Inferno/source/us-core-test-kit/lib/us_core_test_kit/requirements/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/edeyoung/Documents/inferno/us-core-test-kit/lib/us_core_test_kit/requirements/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B26E4571-9F78-E84A-88DC-63B5BFA7F593}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9938CB48-E2A5-3A4B-A7F0-7485136FD2D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1780" yWindow="760" windowWidth="27360" windowHeight="20180" firstSheet="1" activeTab="2" xr2:uid="{D251129A-65BB-5042-909C-749E11B8C0B0}"/>
+    <workbookView xWindow="1780" yWindow="760" windowWidth="27360" windowHeight="18880" firstSheet="1" activeTab="1" xr2:uid="{D251129A-65BB-5042-909C-749E11B8C0B0}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="9" r:id="rId1"/>
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -99,7 +99,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3047" uniqueCount="1060">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3044" uniqueCount="1061">
   <si>
     <r>
       <rPr>
@@ -4085,43 +4085,16 @@
     <t>https://hl7.org/fhir/us/core/STU6.1/StructureDefinition-us-core-patient.html#mandatory-and-must-support-data-elements, https://hl7.org/fhir/us/core/STU6.1/StructureDefinition-us-core-race.html#profile-specific-implementation-guidance</t>
   </si>
   <si>
-    <t>[Organizations participating in the ONC Health IT certrification program,] must support at least one category code from OMB Race [category for the [US Core Race Extension] (https://hl7.org/fhir/us/core/STU7/StructureDefinition-us-core-race.html)]</t>
-  </si>
-  <si>
-    <t>For organizations participating in ONC certification, when using the US Core Race Extension</t>
-  </si>
-  <si>
     <t>Deprecating as this is not in US 6.1,</t>
   </si>
   <si>
     <t>https://hl7.org/fhir/us/core/STU6.1/StructureDefinition-us-core-patient.html#mandatory-and-must-support-data-elements, https://hl7.org/fhir/us/core/STU6.1/StructureDefinition-us-core-ethnicity.html#profile-specific-implementation-guidance</t>
   </si>
   <si>
-    <t>[Organizations participating in the ONC Health IT certrification program,] must support at least one category code from OMB … Ethnicity [category for the [US Core Ethnicity Extension] (https://hl7.org/fhir/us/core/STU7/StructureDefinition-us-core-ethnicity.html)]</t>
-  </si>
-  <si>
-    <t>For organizations participating in ONC certification, When using the US Core Ethnicity Extension</t>
-  </si>
-  <si>
-    <t>[Organizations participating in the ONC Health IT certrification program,] MAY include additional detailed codes from CDC Race … codes [when using the [US Core Race Extension] (https://hl7.org/fhir/us/core/STU7/StructureDefinition-us-core-race.html)]</t>
-  </si>
-  <si>
-    <t>For organizations participating in ONC certification, When using the US Core Race Extension</t>
-  </si>
-  <si>
-    <t>[Organizations participating in the ONC Health IT certrification program,] SHALL include a text description [of category codes when using the [US Core Ethnicity Extension] (https://hl7.org/fhir/us/core/STU7/StructureDefinition-us-core-ethnicity.html)]</t>
-  </si>
-  <si>
     <t>Unknown</t>
   </si>
   <si>
     <t>https://hl7.org/fhir/us/core/STU6.1/StructureDefinition-us-core-patient.html#mandatory-and-must-support-data-elements</t>
-  </si>
-  <si>
-    <t>[For Organizations participating in the ONC Health IT certrification program,] Although Patient.deceased[x] is marked as additional USCDI, certifying systems are not required to support both [boolean and dateTime data types], but SHALL support [at] least Patient.deceasedDateTime</t>
-  </si>
-  <si>
-    <t xml:space="preserve">For organizations participating in ONC certification, </t>
   </si>
   <si>
     <t>Previous name is represented by setting Patient.name.use to “old” or providing an end date in Patient.name.period or doing both</t>
@@ -4872,12 +4845,42 @@
   <si>
     <t>hl7.fhir.us.core_6.1.0</t>
   </si>
+  <si>
+    <t>Marked DEPRECATED because this is an example.</t>
+  </si>
+  <si>
+    <t>Duplicate of 254</t>
+  </si>
+  <si>
+    <t>Duplicate of requirement 260</t>
+  </si>
+  <si>
+    <t>The Complex [Extension] for Race ... allow[s] for one or more codes of which must support at least one category code from OMB Race [category for the [US Core Race Extension] (https://hl7.org/fhir/us/core/STU7/StructureDefinition-us-core-race.html)]</t>
+  </si>
+  <si>
+    <t>The Complex [Extension] for ... Ethnicity allow[s] for one or more codes of which must support at least one category code from OMB … Ethnicity [category for the [US Core Ethnicity Extension] (https://hl7.org/fhir/us/core/STU7/StructureDefinition-us-core-ethnicity.html)]</t>
+  </si>
+  <si>
+    <t>The Complex [Extension] for Race ... allow[s] for one or more codes of which MAY include additional detailed codes from CDC Race … codes [when using the [US Core Race Extension] (https://hl7.org/fhir/us/core/STU7/StructureDefinition-us-core-race.html)]</t>
+  </si>
+  <si>
+    <t>The Complex [Extension] for Race ... allow[s] for one or more codes of which SHALL include a text description [of category codes when using the [US Core Race Extension] (https://hl7.org/fhir/us/core/STU7/StructureDefinition-us-core-race.html)]</t>
+  </si>
+  <si>
+    <t>The Complex [Extension] for ... Ethnicity allow[s] for one or more codes of which MAY include additional detailed codes from CDC Race … codes [when using the [US Core Race Extension] (https://hl7.org/fhir/us/core/STU7/StructureDefinition-us-core-race.html)]</t>
+  </si>
+  <si>
+    <t>The Complex [Extension] for ... Ethnicity allow[s] for one or more codes of which SHALL include a text description [of category codes when using the [US Core Ethnicity Extension] (https://hl7.org/fhir/us/core/STU7/StructureDefinition-us-core-ethnicity.html)]</t>
+  </si>
+  <si>
+    <t>Although Patient.deceased[x] is marked as additional USCDI, certifying systems are not required to support both [boolean and dateTime data types], but SHALL support [at] least Patient.deceasedDateTime</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -5041,8 +5044,15 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -5103,8 +5113,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE2EFDA"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="22">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -5359,12 +5375,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFD0CECE"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFD0CECE"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFD0CECE"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFD0CECE"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5523,6 +5554,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="11" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -5958,11 +5992,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0272D98A-080C-3945-A7E0-CB54FB3A65A9}">
   <dimension ref="A1:V597"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="8" ySplit="1" topLeftCell="S2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="8" ySplit="1" topLeftCell="T460" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="S1" sqref="S1:T1048576"/>
+      <selection pane="bottomRight" activeCell="U473" sqref="U473"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9905,8 +9939,8 @@
       <c r="A94" s="7">
         <v>87</v>
       </c>
-      <c r="B94" s="7" t="s">
-        <v>195</v>
+      <c r="B94" s="23" t="s">
+        <v>209</v>
       </c>
       <c r="C94" s="8" t="s">
         <v>207</v>
@@ -9926,7 +9960,7 @@
       </c>
       <c r="N94" s="9" t="str" cm="1">
         <f t="array" ref="N94">SECTION_NAME(B94)</f>
-        <v>additional-uscdi-requirements</v>
+        <v>defined-pattern-elements</v>
       </c>
       <c r="O94" s="10" t="str">
         <f t="shared" si="4"/>
@@ -9952,7 +9986,7 @@
         <v>210</v>
       </c>
       <c r="D95" s="7" t="s">
-        <v>32</v>
+        <v>87</v>
       </c>
       <c r="E95" s="7" t="s">
         <v>33</v>
@@ -9979,6 +10013,9 @@
         <f t="shared" si="3"/>
         <v>Server</v>
       </c>
+      <c r="T95" s="13" t="s">
+        <v>1051</v>
+      </c>
       <c r="U95" s="63"/>
     </row>
     <row r="96" spans="1:21" ht="187" x14ac:dyDescent="0.2">
@@ -9992,7 +10029,7 @@
         <v>212</v>
       </c>
       <c r="D96" s="7" t="s">
-        <v>32</v>
+        <v>87</v>
       </c>
       <c r="E96" s="7" t="s">
         <v>79</v>
@@ -10018,6 +10055,9 @@
       <c r="P96" s="10" t="str">
         <f t="shared" si="3"/>
         <v>Client</v>
+      </c>
+      <c r="T96" s="13" t="s">
+        <v>1051</v>
       </c>
       <c r="U96" s="63"/>
     </row>
@@ -16764,7 +16804,7 @@
         <v>513</v>
       </c>
       <c r="D263" s="7" t="s">
-        <v>32</v>
+        <v>87</v>
       </c>
       <c r="E263" s="7" t="s">
         <v>33</v>
@@ -16791,6 +16831,9 @@
       <c r="Q263" s="10" t="s">
         <v>514</v>
       </c>
+      <c r="T263" s="56" t="s">
+        <v>1052</v>
+      </c>
       <c r="U263" s="63"/>
     </row>
     <row r="264" spans="1:21" ht="306" x14ac:dyDescent="0.2">
@@ -16967,7 +17010,7 @@
         <v>33</v>
       </c>
       <c r="G268" s="7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M268" s="9" t="str" cm="1">
         <f t="array" ref="M268">PAGE_NAME(B268)</f>
@@ -17001,7 +17044,7 @@
         <v>521</v>
       </c>
       <c r="D269" s="7" t="s">
-        <v>32</v>
+        <v>87</v>
       </c>
       <c r="E269" s="7" t="s">
         <v>33</v>
@@ -17028,6 +17071,9 @@
       <c r="Q269" s="10" t="s">
         <v>522</v>
       </c>
+      <c r="T269" s="71" t="s">
+        <v>1053</v>
+      </c>
       <c r="U269" s="63"/>
     </row>
     <row r="270" spans="1:21" ht="238" x14ac:dyDescent="0.2">
@@ -24626,7 +24672,7 @@
         <v>867</v>
       </c>
       <c r="C467" s="8" t="s">
-        <v>868</v>
+        <v>1054</v>
       </c>
       <c r="D467" s="7" t="s">
         <v>87</v>
@@ -24636,9 +24682,6 @@
       </c>
       <c r="G467" s="7" t="b">
         <v>1</v>
-      </c>
-      <c r="H467" s="13" t="s">
-        <v>869</v>
       </c>
       <c r="M467" s="9" t="str" cm="1">
         <f t="array" ref="M467">PAGE_NAME(B467)</f>
@@ -24657,7 +24700,7 @@
         <v/>
       </c>
       <c r="U467" s="13" t="s">
-        <v>870</v>
+        <v>868</v>
       </c>
     </row>
     <row r="468" spans="1:21" ht="102" x14ac:dyDescent="0.2">
@@ -24665,10 +24708,10 @@
         <v>460</v>
       </c>
       <c r="B468" s="23" t="s">
-        <v>871</v>
+        <v>869</v>
       </c>
       <c r="C468" s="8" t="s">
-        <v>872</v>
+        <v>1055</v>
       </c>
       <c r="D468" s="7" t="s">
         <v>87</v>
@@ -24678,9 +24721,6 @@
       </c>
       <c r="G468" s="7" t="b">
         <v>1</v>
-      </c>
-      <c r="H468" s="13" t="s">
-        <v>873</v>
       </c>
       <c r="M468" s="9" t="str" cm="1">
         <f t="array" ref="M468">PAGE_NAME(B468)</f>
@@ -24699,7 +24739,7 @@
         <v/>
       </c>
       <c r="U468" s="13" t="s">
-        <v>870</v>
+        <v>868</v>
       </c>
     </row>
     <row r="469" spans="1:21" ht="102" x14ac:dyDescent="0.2">
@@ -24710,7 +24750,7 @@
         <v>867</v>
       </c>
       <c r="C469" s="8" t="s">
-        <v>874</v>
+        <v>1056</v>
       </c>
       <c r="D469" s="7" t="s">
         <v>87</v>
@@ -24720,9 +24760,6 @@
       </c>
       <c r="G469" s="7" t="b">
         <v>1</v>
-      </c>
-      <c r="H469" s="13" t="s">
-        <v>875</v>
       </c>
       <c r="M469" s="9" t="str" cm="1">
         <f t="array" ref="M469">PAGE_NAME(B469)</f>
@@ -24741,7 +24778,7 @@
         <v/>
       </c>
       <c r="U469" s="13" t="s">
-        <v>870</v>
+        <v>868</v>
       </c>
     </row>
     <row r="470" spans="1:21" ht="102" x14ac:dyDescent="0.2">
@@ -24749,10 +24786,10 @@
         <v>462</v>
       </c>
       <c r="B470" s="23" t="s">
-        <v>871</v>
+        <v>869</v>
       </c>
       <c r="C470" s="8" t="s">
-        <v>876</v>
+        <v>1057</v>
       </c>
       <c r="D470" s="7" t="s">
         <v>87</v>
@@ -24762,9 +24799,6 @@
       </c>
       <c r="G470" s="7" t="b">
         <v>1</v>
-      </c>
-      <c r="H470" s="13" t="s">
-        <v>873</v>
       </c>
       <c r="M470" s="9" t="str" cm="1">
         <f t="array" ref="M470">PAGE_NAME(B470)</f>
@@ -24783,7 +24817,7 @@
         <v/>
       </c>
       <c r="U470" s="13" t="s">
-        <v>870</v>
+        <v>868</v>
       </c>
     </row>
     <row r="471" spans="1:21" ht="102" x14ac:dyDescent="0.2">
@@ -24794,7 +24828,7 @@
         <v>867</v>
       </c>
       <c r="C471" s="8" t="s">
-        <v>874</v>
+        <v>1058</v>
       </c>
       <c r="D471" s="7" t="s">
         <v>87</v>
@@ -24804,9 +24838,6 @@
       </c>
       <c r="G471" s="7" t="b">
         <v>1</v>
-      </c>
-      <c r="H471" s="13" t="s">
-        <v>875</v>
       </c>
       <c r="M471" s="9" t="str" cm="1">
         <f t="array" ref="M471">PAGE_NAME(B471)</f>
@@ -24825,7 +24856,7 @@
         <v/>
       </c>
       <c r="U471" s="13" t="s">
-        <v>870</v>
+        <v>868</v>
       </c>
     </row>
     <row r="472" spans="1:21" ht="102" x14ac:dyDescent="0.2">
@@ -24833,10 +24864,10 @@
         <v>464</v>
       </c>
       <c r="B472" s="23" t="s">
-        <v>871</v>
+        <v>869</v>
       </c>
       <c r="C472" s="8" t="s">
-        <v>876</v>
+        <v>1059</v>
       </c>
       <c r="D472" s="7" t="s">
         <v>87</v>
@@ -24846,9 +24877,6 @@
       </c>
       <c r="G472" s="7" t="b">
         <v>1</v>
-      </c>
-      <c r="H472" s="13" t="s">
-        <v>873</v>
       </c>
       <c r="M472" s="9" t="str" cm="1">
         <f t="array" ref="M472">PAGE_NAME(B472)</f>
@@ -24867,27 +24895,24 @@
         <v/>
       </c>
       <c r="U472" s="13" t="s">
-        <v>870</v>
-      </c>
-    </row>
-    <row r="473" spans="1:21" ht="119" x14ac:dyDescent="0.2">
+        <v>868</v>
+      </c>
+    </row>
+    <row r="473" spans="1:21" ht="85" x14ac:dyDescent="0.2">
       <c r="A473" s="7">
         <v>465</v>
       </c>
       <c r="B473" s="23" t="s">
-        <v>878</v>
+        <v>871</v>
       </c>
       <c r="C473" s="8" t="s">
-        <v>879</v>
+        <v>1060</v>
       </c>
       <c r="D473" s="7" t="s">
         <v>87</v>
       </c>
       <c r="E473" s="7" t="s">
         <v>33</v>
-      </c>
-      <c r="H473" s="13" t="s">
-        <v>880</v>
       </c>
       <c r="M473" s="9" t="str" cm="1">
         <f t="array" ref="M473">PAGE_NAME(B473)</f>
@@ -24906,7 +24931,7 @@
         <v/>
       </c>
       <c r="U473" s="13" t="s">
-        <v>870</v>
+        <v>868</v>
       </c>
     </row>
     <row r="474" spans="1:21" ht="85" x14ac:dyDescent="0.2">
@@ -24914,10 +24939,10 @@
         <v>466</v>
       </c>
       <c r="B474" s="23" t="s">
-        <v>878</v>
+        <v>871</v>
       </c>
       <c r="C474" s="8" t="s">
-        <v>881</v>
+        <v>872</v>
       </c>
       <c r="D474" s="7" t="s">
         <v>37</v>
@@ -24929,7 +24954,7 @@
         <v>1</v>
       </c>
       <c r="H474" s="13" t="s">
-        <v>882</v>
+        <v>873</v>
       </c>
       <c r="O474" s="10" t="str">
         <f t="shared" si="23"/>
@@ -24945,10 +24970,10 @@
         <v>467</v>
       </c>
       <c r="B475" s="23" t="s">
-        <v>878</v>
+        <v>871</v>
       </c>
       <c r="C475" s="8" t="s">
-        <v>883</v>
+        <v>874</v>
       </c>
       <c r="D475" s="7" t="s">
         <v>37</v>
@@ -24960,7 +24985,7 @@
         <v>1</v>
       </c>
       <c r="H475" s="13" t="s">
-        <v>884</v>
+        <v>875</v>
       </c>
       <c r="M475" s="9" t="str" cm="1">
         <f t="array" ref="M475">PAGE_NAME(B475)</f>
@@ -24984,10 +25009,10 @@
         <v>468</v>
       </c>
       <c r="B476" s="23" t="s">
-        <v>878</v>
+        <v>871</v>
       </c>
       <c r="C476" s="8" t="s">
-        <v>885</v>
+        <v>876</v>
       </c>
       <c r="D476" s="7" t="s">
         <v>41</v>
@@ -25020,10 +25045,10 @@
         <v>469</v>
       </c>
       <c r="B477" s="23" t="s">
-        <v>878</v>
+        <v>871</v>
       </c>
       <c r="C477" s="8" t="s">
-        <v>886</v>
+        <v>877</v>
       </c>
       <c r="D477" s="7" t="s">
         <v>87</v>
@@ -25059,10 +25084,10 @@
         <v>470</v>
       </c>
       <c r="B478" s="23" t="s">
+        <v>871</v>
+      </c>
+      <c r="C478" s="8" t="s">
         <v>878</v>
-      </c>
-      <c r="C478" s="8" t="s">
-        <v>887</v>
       </c>
       <c r="D478" s="7" t="s">
         <v>87</v>
@@ -25098,10 +25123,10 @@
         <v>471</v>
       </c>
       <c r="B479" s="23" t="s">
-        <v>878</v>
+        <v>871</v>
       </c>
       <c r="C479" s="8" t="s">
-        <v>888</v>
+        <v>879</v>
       </c>
       <c r="D479" s="7" t="s">
         <v>87</v>
@@ -25113,7 +25138,7 @@
         <v>1</v>
       </c>
       <c r="H479" s="13" t="s">
-        <v>889</v>
+        <v>880</v>
       </c>
       <c r="M479" s="9" t="str" cm="1">
         <f t="array" ref="M479">PAGE_NAME(B479)</f>
@@ -25140,10 +25165,10 @@
         <v>472</v>
       </c>
       <c r="B480" s="23" t="s">
-        <v>878</v>
+        <v>871</v>
       </c>
       <c r="C480" s="8" t="s">
-        <v>890</v>
+        <v>881</v>
       </c>
       <c r="D480" s="7" t="s">
         <v>112</v>
@@ -25176,10 +25201,10 @@
         <v>473</v>
       </c>
       <c r="B481" s="23" t="s">
-        <v>891</v>
+        <v>882</v>
       </c>
       <c r="C481" s="8" t="s">
-        <v>892</v>
+        <v>883</v>
       </c>
       <c r="D481" s="7" t="s">
         <v>32</v>
@@ -25191,7 +25216,7 @@
         <v>1</v>
       </c>
       <c r="H481" s="13" t="s">
-        <v>893</v>
+        <v>884</v>
       </c>
       <c r="M481" s="9" t="str" cm="1">
         <f t="array" ref="M481">PAGE_NAME(B481)</f>
@@ -25215,10 +25240,10 @@
         <v>474</v>
       </c>
       <c r="B482" s="23" t="s">
-        <v>891</v>
+        <v>882</v>
       </c>
       <c r="C482" s="8" t="s">
-        <v>894</v>
+        <v>885</v>
       </c>
       <c r="D482" s="7" t="s">
         <v>87</v>
@@ -25230,7 +25255,7 @@
         <v>1</v>
       </c>
       <c r="H482" s="13" t="s">
-        <v>895</v>
+        <v>886</v>
       </c>
       <c r="M482" s="9" t="str" cm="1">
         <f t="array" ref="M482">PAGE_NAME(B482)</f>
@@ -25249,7 +25274,7 @@
         <v>Server</v>
       </c>
       <c r="U482" s="13" t="s">
-        <v>870</v>
+        <v>868</v>
       </c>
     </row>
     <row r="483" spans="1:21" ht="68" x14ac:dyDescent="0.2">
@@ -25257,10 +25282,10 @@
         <v>475</v>
       </c>
       <c r="B483" s="23" t="s">
-        <v>891</v>
+        <v>882</v>
       </c>
       <c r="C483" s="8" t="s">
-        <v>896</v>
+        <v>887</v>
       </c>
       <c r="D483" s="7" t="s">
         <v>87</v>
@@ -25272,7 +25297,7 @@
         <v>1</v>
       </c>
       <c r="H483" s="13" t="s">
-        <v>897</v>
+        <v>888</v>
       </c>
       <c r="M483" s="9" t="str" cm="1">
         <f t="array" ref="M483">PAGE_NAME(B483)</f>
@@ -25291,7 +25316,7 @@
         <v>Server</v>
       </c>
       <c r="U483" s="13" t="s">
-        <v>870</v>
+        <v>868</v>
       </c>
     </row>
     <row r="484" spans="1:21" ht="51" x14ac:dyDescent="0.2">
@@ -25299,10 +25324,10 @@
         <v>476</v>
       </c>
       <c r="B484" s="23" t="s">
-        <v>891</v>
+        <v>882</v>
       </c>
       <c r="C484" s="8" t="s">
-        <v>898</v>
+        <v>889</v>
       </c>
       <c r="D484" s="7" t="s">
         <v>87</v>
@@ -25327,7 +25352,7 @@
         <v>Client</v>
       </c>
       <c r="U484" s="13" t="s">
-        <v>899</v>
+        <v>890</v>
       </c>
     </row>
     <row r="485" spans="1:21" ht="51" x14ac:dyDescent="0.2">
@@ -25335,10 +25360,10 @@
         <v>477</v>
       </c>
       <c r="B485" s="23" t="s">
+        <v>882</v>
+      </c>
+      <c r="C485" s="8" t="s">
         <v>891</v>
-      </c>
-      <c r="C485" s="8" t="s">
-        <v>900</v>
       </c>
       <c r="D485" s="7" t="s">
         <v>37</v>
@@ -25371,10 +25396,10 @@
         <v>478</v>
       </c>
       <c r="B486" s="23" t="s">
-        <v>891</v>
+        <v>882</v>
       </c>
       <c r="C486" s="8" t="s">
-        <v>901</v>
+        <v>892</v>
       </c>
       <c r="D486" s="7" t="s">
         <v>87</v>
@@ -25410,10 +25435,10 @@
         <v>479</v>
       </c>
       <c r="B487" s="23" t="s">
-        <v>902</v>
+        <v>893</v>
       </c>
       <c r="C487" s="8" t="s">
-        <v>903</v>
+        <v>894</v>
       </c>
       <c r="D487" s="7" t="s">
         <v>41</v>
@@ -25446,10 +25471,10 @@
         <v>480</v>
       </c>
       <c r="B488" s="23" t="s">
-        <v>902</v>
+        <v>893</v>
       </c>
       <c r="C488" s="8" t="s">
-        <v>904</v>
+        <v>895</v>
       </c>
       <c r="D488" s="7" t="s">
         <v>37</v>
@@ -25461,7 +25486,7 @@
         <v>1</v>
       </c>
       <c r="H488" s="13" t="s">
-        <v>905</v>
+        <v>896</v>
       </c>
       <c r="M488" s="9" t="str" cm="1">
         <f t="array" ref="M488">PAGE_NAME(B488)</f>
@@ -25485,10 +25510,10 @@
         <v>481</v>
       </c>
       <c r="B489" s="23" t="s">
-        <v>902</v>
+        <v>893</v>
       </c>
       <c r="C489" s="8" t="s">
-        <v>906</v>
+        <v>897</v>
       </c>
       <c r="D489" s="7" t="s">
         <v>37</v>
@@ -25521,10 +25546,10 @@
         <v>482</v>
       </c>
       <c r="B490" s="23" t="s">
-        <v>902</v>
+        <v>893</v>
       </c>
       <c r="C490" s="8" t="s">
-        <v>907</v>
+        <v>898</v>
       </c>
       <c r="D490" s="7" t="s">
         <v>87</v>
@@ -25536,7 +25561,7 @@
         <v>1</v>
       </c>
       <c r="H490" s="13" t="s">
-        <v>908</v>
+        <v>899</v>
       </c>
       <c r="M490" s="9" t="str" cm="1">
         <f t="array" ref="M490">PAGE_NAME(B490)</f>
@@ -25555,7 +25580,7 @@
         <v>Server</v>
       </c>
       <c r="U490" s="13" t="s">
-        <v>899</v>
+        <v>890</v>
       </c>
     </row>
     <row r="491" spans="1:21" ht="85" x14ac:dyDescent="0.2">
@@ -25563,10 +25588,10 @@
         <v>483</v>
       </c>
       <c r="B491" s="23" t="s">
-        <v>902</v>
+        <v>893</v>
       </c>
       <c r="C491" s="8" t="s">
-        <v>909</v>
+        <v>900</v>
       </c>
       <c r="D491" s="7" t="s">
         <v>87</v>
@@ -25578,7 +25603,7 @@
         <v>1</v>
       </c>
       <c r="H491" s="13" t="s">
-        <v>908</v>
+        <v>899</v>
       </c>
       <c r="M491" s="9" t="str" cm="1">
         <f t="array" ref="M491">PAGE_NAME(B491)</f>
@@ -25597,7 +25622,7 @@
         <v>Client</v>
       </c>
       <c r="U491" s="13" t="s">
-        <v>899</v>
+        <v>890</v>
       </c>
     </row>
     <row r="492" spans="1:21" ht="119" x14ac:dyDescent="0.2">
@@ -25605,10 +25630,10 @@
         <v>484</v>
       </c>
       <c r="B492" s="23" t="s">
-        <v>902</v>
+        <v>893</v>
       </c>
       <c r="C492" s="8" t="s">
-        <v>910</v>
+        <v>901</v>
       </c>
       <c r="D492" s="7" t="s">
         <v>87</v>
@@ -25620,7 +25645,7 @@
         <v>1</v>
       </c>
       <c r="H492" s="13" t="s">
-        <v>911</v>
+        <v>902</v>
       </c>
       <c r="M492" s="9" t="str" cm="1">
         <f t="array" ref="M492">PAGE_NAME(B492)</f>
@@ -25639,7 +25664,7 @@
         <v>Server</v>
       </c>
       <c r="U492" s="13" t="s">
-        <v>899</v>
+        <v>890</v>
       </c>
     </row>
     <row r="493" spans="1:21" ht="85" x14ac:dyDescent="0.2">
@@ -25647,10 +25672,10 @@
         <v>485</v>
       </c>
       <c r="B493" s="23" t="s">
-        <v>902</v>
+        <v>893</v>
       </c>
       <c r="C493" s="8" t="s">
-        <v>912</v>
+        <v>903</v>
       </c>
       <c r="D493" s="7" t="s">
         <v>87</v>
@@ -25662,7 +25687,7 @@
         <v>1</v>
       </c>
       <c r="H493" s="13" t="s">
-        <v>908</v>
+        <v>899</v>
       </c>
       <c r="M493" s="9" t="str" cm="1">
         <f t="array" ref="M493">PAGE_NAME(B493)</f>
@@ -25681,7 +25706,7 @@
         <v>Client</v>
       </c>
       <c r="U493" s="13" t="s">
-        <v>899</v>
+        <v>890</v>
       </c>
     </row>
     <row r="494" spans="1:21" ht="85" x14ac:dyDescent="0.2">
@@ -25689,10 +25714,10 @@
         <v>486</v>
       </c>
       <c r="B494" s="23" t="s">
-        <v>902</v>
+        <v>893</v>
       </c>
       <c r="C494" s="8" t="s">
-        <v>913</v>
+        <v>904</v>
       </c>
       <c r="D494" s="7" t="s">
         <v>87</v>
@@ -25704,7 +25729,7 @@
         <v>1</v>
       </c>
       <c r="H494" s="13" t="s">
-        <v>914</v>
+        <v>905</v>
       </c>
       <c r="M494" s="9" t="str" cm="1">
         <f t="array" ref="M494">PAGE_NAME(B494)</f>
@@ -25723,7 +25748,7 @@
         <v>Server</v>
       </c>
       <c r="U494" s="13" t="s">
-        <v>899</v>
+        <v>890</v>
       </c>
     </row>
     <row r="495" spans="1:21" ht="85" x14ac:dyDescent="0.2">
@@ -25731,10 +25756,10 @@
         <v>487</v>
       </c>
       <c r="B495" s="23" t="s">
-        <v>902</v>
+        <v>893</v>
       </c>
       <c r="C495" s="8" t="s">
-        <v>915</v>
+        <v>906</v>
       </c>
       <c r="D495" s="7" t="s">
         <v>87</v>
@@ -25746,7 +25771,7 @@
         <v>1</v>
       </c>
       <c r="H495" s="13" t="s">
-        <v>914</v>
+        <v>905</v>
       </c>
       <c r="M495" s="9" t="str" cm="1">
         <f t="array" ref="M495">PAGE_NAME(B495)</f>
@@ -25765,7 +25790,7 @@
         <v>Client</v>
       </c>
       <c r="U495" s="13" t="s">
-        <v>899</v>
+        <v>890</v>
       </c>
     </row>
     <row r="496" spans="1:21" ht="119" x14ac:dyDescent="0.2">
@@ -25773,10 +25798,10 @@
         <v>488</v>
       </c>
       <c r="B496" s="23" t="s">
-        <v>902</v>
+        <v>893</v>
       </c>
       <c r="C496" s="8" t="s">
-        <v>916</v>
+        <v>907</v>
       </c>
       <c r="D496" s="7" t="s">
         <v>87</v>
@@ -25788,7 +25813,7 @@
         <v>1</v>
       </c>
       <c r="H496" s="13" t="s">
-        <v>914</v>
+        <v>905</v>
       </c>
       <c r="M496" s="9" t="str" cm="1">
         <f t="array" ref="M496">PAGE_NAME(B496)</f>
@@ -25807,7 +25832,7 @@
         <v/>
       </c>
       <c r="U496" s="13" t="s">
-        <v>899</v>
+        <v>890</v>
       </c>
     </row>
     <row r="497" spans="1:16" ht="51" x14ac:dyDescent="0.2">
@@ -25815,10 +25840,10 @@
         <v>489</v>
       </c>
       <c r="B497" s="23" t="s">
-        <v>917</v>
+        <v>908</v>
       </c>
       <c r="C497" s="8" t="s">
-        <v>918</v>
+        <v>909</v>
       </c>
       <c r="D497" s="7" t="s">
         <v>32</v>
@@ -25851,10 +25876,10 @@
         <v>490</v>
       </c>
       <c r="B498" s="23" t="s">
-        <v>917</v>
+        <v>908</v>
       </c>
       <c r="C498" s="8" t="s">
-        <v>919</v>
+        <v>910</v>
       </c>
       <c r="D498" s="7" t="s">
         <v>32</v>
@@ -25887,10 +25912,10 @@
         <v>491</v>
       </c>
       <c r="B499" s="23" t="s">
-        <v>917</v>
+        <v>908</v>
       </c>
       <c r="C499" s="8" t="s">
-        <v>920</v>
+        <v>911</v>
       </c>
       <c r="D499" s="7" t="s">
         <v>32</v>
@@ -25923,10 +25948,10 @@
         <v>492</v>
       </c>
       <c r="B500" s="23" t="s">
-        <v>917</v>
+        <v>908</v>
       </c>
       <c r="C500" s="8" t="s">
-        <v>921</v>
+        <v>912</v>
       </c>
       <c r="D500" s="7" t="s">
         <v>32</v>
@@ -25959,10 +25984,10 @@
         <v>493</v>
       </c>
       <c r="B501" s="23" t="s">
-        <v>917</v>
+        <v>908</v>
       </c>
       <c r="C501" s="8" t="s">
-        <v>922</v>
+        <v>913</v>
       </c>
       <c r="D501" s="7" t="s">
         <v>32</v>
@@ -25995,10 +26020,10 @@
         <v>494</v>
       </c>
       <c r="B502" s="23" t="s">
-        <v>917</v>
+        <v>908</v>
       </c>
       <c r="C502" s="8" t="s">
-        <v>923</v>
+        <v>914</v>
       </c>
       <c r="D502" s="7" t="s">
         <v>32</v>
@@ -26031,10 +26056,10 @@
         <v>495</v>
       </c>
       <c r="B503" s="23" t="s">
-        <v>917</v>
+        <v>908</v>
       </c>
       <c r="C503" s="8" t="s">
-        <v>924</v>
+        <v>915</v>
       </c>
       <c r="D503" s="7" t="s">
         <v>32</v>
@@ -26067,10 +26092,10 @@
         <v>496</v>
       </c>
       <c r="B504" s="23" t="s">
-        <v>917</v>
+        <v>908</v>
       </c>
       <c r="C504" s="8" t="s">
-        <v>925</v>
+        <v>916</v>
       </c>
       <c r="D504" s="7" t="s">
         <v>32</v>
@@ -26103,10 +26128,10 @@
         <v>497</v>
       </c>
       <c r="B505" s="23" t="s">
+        <v>908</v>
+      </c>
+      <c r="C505" s="8" t="s">
         <v>917</v>
-      </c>
-      <c r="C505" s="8" t="s">
-        <v>926</v>
       </c>
       <c r="D505" s="7" t="s">
         <v>32</v>
@@ -26139,10 +26164,10 @@
         <v>498</v>
       </c>
       <c r="B506" s="23" t="s">
-        <v>917</v>
+        <v>908</v>
       </c>
       <c r="C506" s="8" t="s">
-        <v>927</v>
+        <v>918</v>
       </c>
       <c r="D506" s="7" t="s">
         <v>32</v>
@@ -26175,10 +26200,10 @@
         <v>499</v>
       </c>
       <c r="B507" s="23" t="s">
-        <v>917</v>
+        <v>908</v>
       </c>
       <c r="C507" s="8" t="s">
-        <v>928</v>
+        <v>919</v>
       </c>
       <c r="D507" s="7" t="s">
         <v>32</v>
@@ -26211,10 +26236,10 @@
         <v>500</v>
       </c>
       <c r="B508" s="23" t="s">
-        <v>917</v>
+        <v>908</v>
       </c>
       <c r="C508" s="8" t="s">
-        <v>929</v>
+        <v>920</v>
       </c>
       <c r="D508" s="7" t="s">
         <v>32</v>
@@ -26247,10 +26272,10 @@
         <v>501</v>
       </c>
       <c r="B509" s="23" t="s">
-        <v>917</v>
+        <v>908</v>
       </c>
       <c r="C509" s="8" t="s">
-        <v>930</v>
+        <v>921</v>
       </c>
       <c r="D509" s="7" t="s">
         <v>32</v>
@@ -26283,10 +26308,10 @@
         <v>502</v>
       </c>
       <c r="B510" s="23" t="s">
-        <v>917</v>
+        <v>908</v>
       </c>
       <c r="C510" s="8" t="s">
-        <v>931</v>
+        <v>922</v>
       </c>
       <c r="D510" s="7" t="s">
         <v>32</v>
@@ -26319,10 +26344,10 @@
         <v>503</v>
       </c>
       <c r="B511" s="23" t="s">
-        <v>917</v>
+        <v>908</v>
       </c>
       <c r="C511" s="8" t="s">
-        <v>932</v>
+        <v>923</v>
       </c>
       <c r="D511" s="7" t="s">
         <v>32</v>
@@ -26355,10 +26380,10 @@
         <v>504</v>
       </c>
       <c r="B512" s="23" t="s">
-        <v>917</v>
+        <v>908</v>
       </c>
       <c r="C512" s="8" t="s">
-        <v>933</v>
+        <v>924</v>
       </c>
       <c r="D512" s="7" t="s">
         <v>32</v>
@@ -26391,10 +26416,10 @@
         <v>505</v>
       </c>
       <c r="B513" s="23" t="s">
-        <v>917</v>
+        <v>908</v>
       </c>
       <c r="C513" s="8" t="s">
-        <v>934</v>
+        <v>925</v>
       </c>
       <c r="D513" s="7" t="s">
         <v>32</v>
@@ -26427,10 +26452,10 @@
         <v>506</v>
       </c>
       <c r="B514" s="23" t="s">
-        <v>917</v>
+        <v>908</v>
       </c>
       <c r="C514" s="8" t="s">
-        <v>935</v>
+        <v>926</v>
       </c>
       <c r="D514" s="7" t="s">
         <v>32</v>
@@ -26463,10 +26488,10 @@
         <v>507</v>
       </c>
       <c r="B515" s="23" t="s">
-        <v>917</v>
+        <v>908</v>
       </c>
       <c r="C515" s="8" t="s">
-        <v>936</v>
+        <v>927</v>
       </c>
       <c r="D515" s="7" t="s">
         <v>32</v>
@@ -26499,10 +26524,10 @@
         <v>508</v>
       </c>
       <c r="B516" s="23" t="s">
-        <v>917</v>
+        <v>908</v>
       </c>
       <c r="C516" s="8" t="s">
-        <v>937</v>
+        <v>928</v>
       </c>
       <c r="D516" s="7" t="s">
         <v>32</v>
@@ -26514,7 +26539,7 @@
         <v>1</v>
       </c>
       <c r="H516" s="13" t="s">
-        <v>938</v>
+        <v>929</v>
       </c>
       <c r="M516" s="9" t="str" cm="1">
         <f t="array" ref="M516">PAGE_NAME(B516)</f>
@@ -26538,10 +26563,10 @@
         <v>509</v>
       </c>
       <c r="B517" s="23" t="s">
-        <v>917</v>
+        <v>908</v>
       </c>
       <c r="C517" s="8" t="s">
-        <v>939</v>
+        <v>930</v>
       </c>
       <c r="D517" s="7" t="s">
         <v>41</v>
@@ -26553,7 +26578,7 @@
         <v>1</v>
       </c>
       <c r="H517" s="13" t="s">
-        <v>940</v>
+        <v>931</v>
       </c>
       <c r="M517" s="9" t="str" cm="1">
         <f t="array" ref="M517">PAGE_NAME(B517)</f>
@@ -26577,10 +26602,10 @@
         <v>510</v>
       </c>
       <c r="B518" s="23" t="s">
-        <v>917</v>
+        <v>908</v>
       </c>
       <c r="C518" s="8" t="s">
-        <v>941</v>
+        <v>932</v>
       </c>
       <c r="D518" s="7" t="s">
         <v>37</v>
@@ -26613,10 +26638,10 @@
         <v>511</v>
       </c>
       <c r="B519" s="23" t="s">
-        <v>942</v>
+        <v>933</v>
       </c>
       <c r="C519" s="8" t="s">
-        <v>943</v>
+        <v>934</v>
       </c>
       <c r="D519" s="7" t="s">
         <v>32</v>
@@ -26628,7 +26653,7 @@
         <v>1</v>
       </c>
       <c r="H519" s="13" t="s">
-        <v>944</v>
+        <v>935</v>
       </c>
       <c r="M519" s="9" t="str" cm="1">
         <f t="array" ref="M519">PAGE_NAME(B519)</f>
@@ -26652,10 +26677,10 @@
         <v>512</v>
       </c>
       <c r="B520" s="23" t="s">
-        <v>942</v>
+        <v>933</v>
       </c>
       <c r="C520" s="8" t="s">
-        <v>945</v>
+        <v>936</v>
       </c>
       <c r="D520" s="7" t="s">
         <v>41</v>
@@ -26667,7 +26692,7 @@
         <v>1</v>
       </c>
       <c r="H520" s="13" t="s">
-        <v>944</v>
+        <v>935</v>
       </c>
       <c r="M520" s="9" t="str" cm="1">
         <f t="array" ref="M520">PAGE_NAME(B520)</f>
@@ -26691,10 +26716,10 @@
         <v>513</v>
       </c>
       <c r="B521" s="23" t="s">
-        <v>946</v>
+        <v>937</v>
       </c>
       <c r="C521" s="8" t="s">
-        <v>947</v>
+        <v>938</v>
       </c>
       <c r="D521" s="7" t="s">
         <v>87</v>
@@ -26730,10 +26755,10 @@
         <v>514</v>
       </c>
       <c r="B522" s="23" t="s">
-        <v>948</v>
+        <v>939</v>
       </c>
       <c r="C522" s="8" t="s">
-        <v>949</v>
+        <v>940</v>
       </c>
       <c r="D522" s="7" t="s">
         <v>41</v>
@@ -26766,10 +26791,10 @@
         <v>515</v>
       </c>
       <c r="B523" s="23" t="s">
-        <v>948</v>
+        <v>939</v>
       </c>
       <c r="C523" s="8" t="s">
-        <v>950</v>
+        <v>941</v>
       </c>
       <c r="D523" s="7" t="s">
         <v>37</v>
@@ -26802,10 +26827,10 @@
         <v>516</v>
       </c>
       <c r="B524" s="53" t="s">
-        <v>948</v>
+        <v>939</v>
       </c>
       <c r="C524" s="8" t="s">
-        <v>951</v>
+        <v>942</v>
       </c>
       <c r="D524" s="7" t="s">
         <v>87</v>
@@ -26817,7 +26842,7 @@
         <v>1</v>
       </c>
       <c r="H524" s="13" t="s">
-        <v>908</v>
+        <v>899</v>
       </c>
       <c r="M524" s="9" t="str" cm="1">
         <f t="array" ref="M524">PAGE_NAME(B524)</f>
@@ -26836,7 +26861,7 @@
         <v>Server</v>
       </c>
       <c r="U524" s="13" t="s">
-        <v>899</v>
+        <v>890</v>
       </c>
     </row>
     <row r="525" spans="1:21" ht="85" x14ac:dyDescent="0.2">
@@ -26844,10 +26869,10 @@
         <v>517</v>
       </c>
       <c r="B525" s="23" t="s">
-        <v>948</v>
+        <v>939</v>
       </c>
       <c r="C525" s="8" t="s">
-        <v>952</v>
+        <v>943</v>
       </c>
       <c r="D525" s="7" t="s">
         <v>87</v>
@@ -26859,7 +26884,7 @@
         <v>1</v>
       </c>
       <c r="H525" s="13" t="s">
-        <v>908</v>
+        <v>899</v>
       </c>
       <c r="M525" s="9" t="str" cm="1">
         <f t="array" ref="M525">PAGE_NAME(B525)</f>
@@ -26878,7 +26903,7 @@
         <v>Client</v>
       </c>
       <c r="U525" s="13" t="s">
-        <v>899</v>
+        <v>890</v>
       </c>
     </row>
     <row r="526" spans="1:21" ht="119" x14ac:dyDescent="0.2">
@@ -26886,10 +26911,10 @@
         <v>518</v>
       </c>
       <c r="B526" s="23" t="s">
-        <v>948</v>
+        <v>939</v>
       </c>
       <c r="C526" s="8" t="s">
-        <v>953</v>
+        <v>944</v>
       </c>
       <c r="D526" s="7" t="s">
         <v>87</v>
@@ -26901,7 +26926,7 @@
         <v>1</v>
       </c>
       <c r="H526" s="13" t="s">
-        <v>911</v>
+        <v>902</v>
       </c>
       <c r="M526" s="9" t="str" cm="1">
         <f t="array" ref="M526">PAGE_NAME(B526)</f>
@@ -26920,7 +26945,7 @@
         <v>Server</v>
       </c>
       <c r="U526" s="13" t="s">
-        <v>899</v>
+        <v>890</v>
       </c>
     </row>
     <row r="527" spans="1:21" ht="85" x14ac:dyDescent="0.2">
@@ -26928,10 +26953,10 @@
         <v>519</v>
       </c>
       <c r="B527" s="23" t="s">
-        <v>948</v>
+        <v>939</v>
       </c>
       <c r="C527" s="8" t="s">
-        <v>954</v>
+        <v>945</v>
       </c>
       <c r="D527" s="7" t="s">
         <v>87</v>
@@ -26943,7 +26968,7 @@
         <v>1</v>
       </c>
       <c r="H527" s="13" t="s">
-        <v>908</v>
+        <v>899</v>
       </c>
       <c r="M527" s="9" t="str" cm="1">
         <f t="array" ref="M527">PAGE_NAME(B527)</f>
@@ -26962,7 +26987,7 @@
         <v>Client</v>
       </c>
       <c r="U527" s="13" t="s">
-        <v>899</v>
+        <v>890</v>
       </c>
     </row>
     <row r="528" spans="1:21" ht="85" x14ac:dyDescent="0.2">
@@ -26970,10 +26995,10 @@
         <v>520</v>
       </c>
       <c r="B528" s="23" t="s">
-        <v>948</v>
+        <v>939</v>
       </c>
       <c r="C528" s="8" t="s">
-        <v>955</v>
+        <v>946</v>
       </c>
       <c r="D528" s="7" t="s">
         <v>87</v>
@@ -26985,7 +27010,7 @@
         <v>1</v>
       </c>
       <c r="H528" s="13" t="s">
-        <v>914</v>
+        <v>905</v>
       </c>
       <c r="M528" s="9" t="str" cm="1">
         <f t="array" ref="M528">PAGE_NAME(B528)</f>
@@ -27004,7 +27029,7 @@
         <v>Server</v>
       </c>
       <c r="U528" s="13" t="s">
-        <v>899</v>
+        <v>890</v>
       </c>
     </row>
     <row r="529" spans="1:21" ht="85" x14ac:dyDescent="0.2">
@@ -27012,10 +27037,10 @@
         <v>521</v>
       </c>
       <c r="B529" s="53" t="s">
-        <v>948</v>
+        <v>939</v>
       </c>
       <c r="C529" s="8" t="s">
-        <v>956</v>
+        <v>947</v>
       </c>
       <c r="D529" s="7" t="s">
         <v>87</v>
@@ -27027,7 +27052,7 @@
         <v>1</v>
       </c>
       <c r="H529" s="13" t="s">
-        <v>914</v>
+        <v>905</v>
       </c>
       <c r="M529" s="9" t="str" cm="1">
         <f t="array" ref="M529">PAGE_NAME(B529)</f>
@@ -27046,7 +27071,7 @@
         <v>Client</v>
       </c>
       <c r="U529" s="13" t="s">
-        <v>899</v>
+        <v>890</v>
       </c>
     </row>
     <row r="530" spans="1:21" ht="102" x14ac:dyDescent="0.2">
@@ -27054,10 +27079,10 @@
         <v>522</v>
       </c>
       <c r="B530" s="23" t="s">
+        <v>939</v>
+      </c>
+      <c r="C530" s="8" t="s">
         <v>948</v>
-      </c>
-      <c r="C530" s="8" t="s">
-        <v>957</v>
       </c>
       <c r="D530" s="7" t="s">
         <v>37</v>
@@ -27085,7 +27110,7 @@
         <v/>
       </c>
       <c r="U530" s="13" t="s">
-        <v>958</v>
+        <v>949</v>
       </c>
     </row>
     <row r="531" spans="1:21" ht="68" x14ac:dyDescent="0.2">
@@ -27093,10 +27118,10 @@
         <v>523</v>
       </c>
       <c r="B531" s="23" t="s">
-        <v>959</v>
+        <v>950</v>
       </c>
       <c r="C531" s="8" t="s">
-        <v>960</v>
+        <v>951</v>
       </c>
       <c r="D531" s="7" t="s">
         <v>41</v>
@@ -27129,10 +27154,10 @@
         <v>524</v>
       </c>
       <c r="B532" s="23" t="s">
-        <v>959</v>
+        <v>950</v>
       </c>
       <c r="C532" s="8" t="s">
-        <v>961</v>
+        <v>952</v>
       </c>
       <c r="D532" s="7" t="s">
         <v>87</v>
@@ -27144,7 +27169,7 @@
         <v>1</v>
       </c>
       <c r="H532" s="13" t="s">
-        <v>962</v>
+        <v>953</v>
       </c>
       <c r="M532" s="9" t="str" cm="1">
         <f t="array" ref="M532">PAGE_NAME(B532)</f>
@@ -27163,7 +27188,7 @@
         <v>Server</v>
       </c>
       <c r="U532" s="13" t="s">
-        <v>899</v>
+        <v>890</v>
       </c>
     </row>
     <row r="533" spans="1:21" ht="51" x14ac:dyDescent="0.2">
@@ -27171,10 +27196,10 @@
         <v>525</v>
       </c>
       <c r="B533" s="23" t="s">
-        <v>959</v>
+        <v>950</v>
       </c>
       <c r="C533" s="8" t="s">
-        <v>963</v>
+        <v>954</v>
       </c>
       <c r="D533" s="7" t="s">
         <v>87</v>
@@ -27202,7 +27227,7 @@
         <v>Client</v>
       </c>
       <c r="U533" s="13" t="s">
-        <v>899</v>
+        <v>890</v>
       </c>
     </row>
     <row r="534" spans="1:21" ht="51" x14ac:dyDescent="0.2">
@@ -27210,10 +27235,10 @@
         <v>526</v>
       </c>
       <c r="B534" s="23" t="s">
-        <v>959</v>
+        <v>950</v>
       </c>
       <c r="C534" s="8" t="s">
-        <v>964</v>
+        <v>955</v>
       </c>
       <c r="D534" s="7" t="s">
         <v>41</v>
@@ -27246,10 +27271,10 @@
         <v>527</v>
       </c>
       <c r="B535" s="23" t="s">
-        <v>965</v>
+        <v>956</v>
       </c>
       <c r="C535" s="8" t="s">
-        <v>966</v>
+        <v>957</v>
       </c>
       <c r="D535" s="7" t="s">
         <v>37</v>
@@ -27277,7 +27302,7 @@
         <v>Client</v>
       </c>
       <c r="U535" s="13" t="s">
-        <v>967</v>
+        <v>958</v>
       </c>
     </row>
     <row r="536" spans="1:21" ht="34" x14ac:dyDescent="0.2">
@@ -27285,10 +27310,10 @@
         <v>528</v>
       </c>
       <c r="B536" s="23" t="s">
-        <v>968</v>
+        <v>959</v>
       </c>
       <c r="C536" s="8" t="s">
-        <v>969</v>
+        <v>960</v>
       </c>
       <c r="D536" s="7" t="s">
         <v>41</v>
@@ -27321,10 +27346,10 @@
         <v>529</v>
       </c>
       <c r="B537" s="23" t="s">
-        <v>968</v>
+        <v>959</v>
       </c>
       <c r="C537" s="8" t="s">
-        <v>970</v>
+        <v>961</v>
       </c>
       <c r="D537" s="7" t="s">
         <v>41</v>
@@ -27357,10 +27382,10 @@
         <v>530</v>
       </c>
       <c r="B538" s="23" t="s">
-        <v>968</v>
+        <v>959</v>
       </c>
       <c r="C538" s="8" t="s">
-        <v>971</v>
+        <v>962</v>
       </c>
       <c r="D538" s="7" t="s">
         <v>41</v>
@@ -27393,10 +27418,10 @@
         <v>531</v>
       </c>
       <c r="B539" s="23" t="s">
-        <v>968</v>
+        <v>959</v>
       </c>
       <c r="C539" s="8" t="s">
-        <v>972</v>
+        <v>963</v>
       </c>
       <c r="D539" s="7" t="s">
         <v>41</v>
@@ -27429,10 +27454,10 @@
         <v>532</v>
       </c>
       <c r="B540" s="23" t="s">
-        <v>973</v>
+        <v>964</v>
       </c>
       <c r="C540" s="8" t="s">
-        <v>974</v>
+        <v>965</v>
       </c>
       <c r="D540" s="7" t="s">
         <v>37</v>
@@ -27460,7 +27485,7 @@
         <v>Server</v>
       </c>
       <c r="U540" s="13" t="s">
-        <v>975</v>
+        <v>966</v>
       </c>
     </row>
     <row r="541" spans="1:21" ht="34" x14ac:dyDescent="0.2">
@@ -27468,10 +27493,10 @@
         <v>533</v>
       </c>
       <c r="B541" s="23" t="s">
-        <v>976</v>
+        <v>967</v>
       </c>
       <c r="C541" s="8" t="s">
-        <v>977</v>
+        <v>968</v>
       </c>
       <c r="D541" s="7" t="s">
         <v>32</v>
@@ -27504,10 +27529,10 @@
         <v>534</v>
       </c>
       <c r="B542" s="23" t="s">
-        <v>976</v>
+        <v>967</v>
       </c>
       <c r="C542" s="8" t="s">
-        <v>978</v>
+        <v>969</v>
       </c>
       <c r="D542" s="7" t="s">
         <v>32</v>
@@ -27540,10 +27565,10 @@
         <v>535</v>
       </c>
       <c r="B543" s="23" t="s">
-        <v>976</v>
+        <v>967</v>
       </c>
       <c r="C543" s="8" t="s">
-        <v>979</v>
+        <v>970</v>
       </c>
       <c r="D543" s="7" t="s">
         <v>32</v>
@@ -27576,10 +27601,10 @@
         <v>536</v>
       </c>
       <c r="B544" s="23" t="s">
-        <v>976</v>
+        <v>967</v>
       </c>
       <c r="C544" s="8" t="s">
-        <v>980</v>
+        <v>971</v>
       </c>
       <c r="D544" s="7" t="s">
         <v>32</v>
@@ -27612,10 +27637,10 @@
         <v>537</v>
       </c>
       <c r="B545" s="23" t="s">
-        <v>976</v>
+        <v>967</v>
       </c>
       <c r="C545" s="8" t="s">
-        <v>981</v>
+        <v>972</v>
       </c>
       <c r="D545" s="7" t="s">
         <v>32</v>
@@ -27648,10 +27673,10 @@
         <v>538</v>
       </c>
       <c r="B546" s="23" t="s">
-        <v>976</v>
+        <v>967</v>
       </c>
       <c r="C546" s="8" t="s">
-        <v>982</v>
+        <v>973</v>
       </c>
       <c r="D546" s="7" t="s">
         <v>32</v>
@@ -27684,10 +27709,10 @@
         <v>539</v>
       </c>
       <c r="B547" s="23" t="s">
-        <v>976</v>
+        <v>967</v>
       </c>
       <c r="C547" s="8" t="s">
-        <v>983</v>
+        <v>974</v>
       </c>
       <c r="D547" s="7" t="s">
         <v>32</v>
@@ -27720,10 +27745,10 @@
         <v>540</v>
       </c>
       <c r="B548" s="23" t="s">
-        <v>976</v>
+        <v>967</v>
       </c>
       <c r="C548" s="8" t="s">
-        <v>984</v>
+        <v>975</v>
       </c>
       <c r="D548" s="7" t="s">
         <v>32</v>
@@ -27756,10 +27781,10 @@
         <v>541</v>
       </c>
       <c r="B549" s="23" t="s">
+        <v>967</v>
+      </c>
+      <c r="C549" s="8" t="s">
         <v>976</v>
-      </c>
-      <c r="C549" s="8" t="s">
-        <v>985</v>
       </c>
       <c r="D549" s="7" t="s">
         <v>37</v>
@@ -27792,10 +27817,10 @@
         <v>542</v>
       </c>
       <c r="B550" s="23" t="s">
-        <v>976</v>
+        <v>967</v>
       </c>
       <c r="C550" s="8" t="s">
-        <v>986</v>
+        <v>977</v>
       </c>
       <c r="D550" s="7" t="s">
         <v>37</v>
@@ -27828,10 +27853,10 @@
         <v>543</v>
       </c>
       <c r="B551" s="23" t="s">
-        <v>976</v>
+        <v>967</v>
       </c>
       <c r="C551" s="8" t="s">
-        <v>987</v>
+        <v>978</v>
       </c>
       <c r="D551" s="7" t="s">
         <v>32</v>
@@ -27843,7 +27868,7 @@
         <v>1</v>
       </c>
       <c r="H551" s="13" t="s">
-        <v>988</v>
+        <v>979</v>
       </c>
       <c r="M551" s="9" t="str" cm="1">
         <f t="array" ref="M551">PAGE_NAME(B551)</f>
@@ -27867,10 +27892,10 @@
         <v>544</v>
       </c>
       <c r="B552" s="23" t="s">
-        <v>976</v>
+        <v>967</v>
       </c>
       <c r="C552" s="8" t="s">
-        <v>989</v>
+        <v>980</v>
       </c>
       <c r="D552" s="7" t="s">
         <v>41</v>
@@ -27903,10 +27928,10 @@
         <v>545</v>
       </c>
       <c r="B553" s="23" t="s">
-        <v>976</v>
+        <v>967</v>
       </c>
       <c r="C553" s="8" t="s">
-        <v>990</v>
+        <v>981</v>
       </c>
       <c r="D553" s="7" t="s">
         <v>41</v>
@@ -27939,10 +27964,10 @@
         <v>546</v>
       </c>
       <c r="B554" s="23" t="s">
-        <v>976</v>
+        <v>967</v>
       </c>
       <c r="C554" s="8" t="s">
-        <v>991</v>
+        <v>982</v>
       </c>
       <c r="D554" s="7" t="s">
         <v>41</v>
@@ -27975,10 +28000,10 @@
         <v>547</v>
       </c>
       <c r="B555" s="23" t="s">
-        <v>976</v>
+        <v>967</v>
       </c>
       <c r="C555" s="8" t="s">
-        <v>992</v>
+        <v>983</v>
       </c>
       <c r="D555" s="7" t="s">
         <v>41</v>
@@ -28011,10 +28036,10 @@
         <v>548</v>
       </c>
       <c r="B556" s="23" t="s">
-        <v>993</v>
+        <v>984</v>
       </c>
       <c r="C556" s="8" t="s">
-        <v>994</v>
+        <v>985</v>
       </c>
       <c r="D556" s="7" t="s">
         <v>37</v>
@@ -28047,10 +28072,10 @@
         <v>549</v>
       </c>
       <c r="B557" s="23" t="s">
-        <v>993</v>
+        <v>984</v>
       </c>
       <c r="C557" s="8" t="s">
-        <v>995</v>
+        <v>986</v>
       </c>
       <c r="D557" s="7" t="s">
         <v>37</v>
@@ -28062,7 +28087,7 @@
         <v>1</v>
       </c>
       <c r="H557" s="13" t="s">
-        <v>996</v>
+        <v>987</v>
       </c>
       <c r="M557" s="9" t="str" cm="1">
         <f t="array" ref="M557">PAGE_NAME(B557)</f>
@@ -28086,10 +28111,10 @@
         <v>550</v>
       </c>
       <c r="B558" s="23" t="s">
-        <v>997</v>
+        <v>988</v>
       </c>
       <c r="C558" s="8" t="s">
-        <v>998</v>
+        <v>989</v>
       </c>
       <c r="D558" s="7" t="s">
         <v>32</v>
@@ -28122,10 +28147,10 @@
         <v>551</v>
       </c>
       <c r="B559" s="23" t="s">
-        <v>997</v>
+        <v>988</v>
       </c>
       <c r="C559" s="8" t="s">
-        <v>998</v>
+        <v>989</v>
       </c>
       <c r="D559" s="7" t="s">
         <v>32</v>
@@ -28158,10 +28183,10 @@
         <v>552</v>
       </c>
       <c r="B560" s="23" t="s">
-        <v>997</v>
+        <v>988</v>
       </c>
       <c r="C560" s="8" t="s">
-        <v>999</v>
+        <v>990</v>
       </c>
       <c r="D560" s="7" t="s">
         <v>37</v>
@@ -28194,10 +28219,10 @@
         <v>553</v>
       </c>
       <c r="B561" s="23" t="s">
-        <v>997</v>
+        <v>988</v>
       </c>
       <c r="C561" s="8" t="s">
-        <v>999</v>
+        <v>990</v>
       </c>
       <c r="D561" s="7" t="s">
         <v>37</v>
@@ -28230,10 +28255,10 @@
         <v>554</v>
       </c>
       <c r="B562" s="23" t="s">
-        <v>997</v>
+        <v>988</v>
       </c>
       <c r="C562" s="8" t="s">
-        <v>1000</v>
+        <v>991</v>
       </c>
       <c r="D562" s="7" t="s">
         <v>37</v>
@@ -28266,10 +28291,10 @@
         <v>555</v>
       </c>
       <c r="B563" s="23" t="s">
-        <v>997</v>
+        <v>988</v>
       </c>
       <c r="C563" s="8" t="s">
-        <v>1000</v>
+        <v>991</v>
       </c>
       <c r="D563" s="7" t="s">
         <v>37</v>
@@ -28302,10 +28327,10 @@
         <v>556</v>
       </c>
       <c r="B564" s="23" t="s">
-        <v>997</v>
+        <v>988</v>
       </c>
       <c r="C564" s="8" t="s">
-        <v>1001</v>
+        <v>992</v>
       </c>
       <c r="D564" s="7" t="s">
         <v>37</v>
@@ -28338,10 +28363,10 @@
         <v>557</v>
       </c>
       <c r="B565" s="23" t="s">
-        <v>997</v>
+        <v>988</v>
       </c>
       <c r="C565" s="8" t="s">
-        <v>1001</v>
+        <v>992</v>
       </c>
       <c r="D565" s="7" t="s">
         <v>37</v>
@@ -28374,10 +28399,10 @@
         <v>558</v>
       </c>
       <c r="B566" s="23" t="s">
-        <v>997</v>
+        <v>988</v>
       </c>
       <c r="C566" s="8" t="s">
-        <v>1002</v>
+        <v>993</v>
       </c>
       <c r="D566" s="7" t="s">
         <v>32</v>
@@ -28410,10 +28435,10 @@
         <v>559</v>
       </c>
       <c r="B567" s="23" t="s">
-        <v>997</v>
+        <v>988</v>
       </c>
       <c r="C567" s="8" t="s">
-        <v>1002</v>
+        <v>993</v>
       </c>
       <c r="D567" s="7" t="s">
         <v>32</v>
@@ -28446,10 +28471,10 @@
         <v>560</v>
       </c>
       <c r="B568" s="23" t="s">
-        <v>997</v>
+        <v>988</v>
       </c>
       <c r="C568" s="8" t="s">
-        <v>1003</v>
+        <v>994</v>
       </c>
       <c r="D568" s="7" t="s">
         <v>37</v>
@@ -28482,10 +28507,10 @@
         <v>561</v>
       </c>
       <c r="B569" s="23" t="s">
-        <v>997</v>
+        <v>988</v>
       </c>
       <c r="C569" s="8" t="s">
-        <v>1003</v>
+        <v>994</v>
       </c>
       <c r="D569" s="7" t="s">
         <v>37</v>
@@ -28518,10 +28543,10 @@
         <v>562</v>
       </c>
       <c r="B570" s="23" t="s">
-        <v>997</v>
+        <v>988</v>
       </c>
       <c r="C570" s="8" t="s">
-        <v>1004</v>
+        <v>995</v>
       </c>
       <c r="D570" s="7" t="s">
         <v>32</v>
@@ -28554,10 +28579,10 @@
         <v>563</v>
       </c>
       <c r="B571" s="23" t="s">
-        <v>997</v>
+        <v>988</v>
       </c>
       <c r="C571" s="8" t="s">
-        <v>1004</v>
+        <v>995</v>
       </c>
       <c r="D571" s="7" t="s">
         <v>32</v>
@@ -28590,10 +28615,10 @@
         <v>564</v>
       </c>
       <c r="B572" s="23" t="s">
-        <v>997</v>
+        <v>988</v>
       </c>
       <c r="C572" s="8" t="s">
-        <v>1005</v>
+        <v>996</v>
       </c>
       <c r="D572" s="7" t="s">
         <v>32</v>
@@ -28626,10 +28651,10 @@
         <v>565</v>
       </c>
       <c r="B573" s="23" t="s">
-        <v>997</v>
+        <v>988</v>
       </c>
       <c r="C573" s="8" t="s">
-        <v>1005</v>
+        <v>996</v>
       </c>
       <c r="D573" s="7" t="s">
         <v>32</v>
@@ -28662,10 +28687,10 @@
         <v>566</v>
       </c>
       <c r="B574" s="23" t="s">
+        <v>988</v>
+      </c>
+      <c r="C574" s="8" t="s">
         <v>997</v>
-      </c>
-      <c r="C574" s="8" t="s">
-        <v>1006</v>
       </c>
       <c r="D574" s="7" t="s">
         <v>37</v>
@@ -28698,10 +28723,10 @@
         <v>567</v>
       </c>
       <c r="B575" s="23" t="s">
+        <v>988</v>
+      </c>
+      <c r="C575" s="8" t="s">
         <v>997</v>
-      </c>
-      <c r="C575" s="8" t="s">
-        <v>1006</v>
       </c>
       <c r="D575" s="7" t="s">
         <v>37</v>
@@ -28734,10 +28759,10 @@
         <v>568</v>
       </c>
       <c r="B576" s="23" t="s">
-        <v>997</v>
+        <v>988</v>
       </c>
       <c r="C576" s="8" t="s">
-        <v>1007</v>
+        <v>998</v>
       </c>
       <c r="D576" s="7" t="s">
         <v>32</v>
@@ -28770,10 +28795,10 @@
         <v>569</v>
       </c>
       <c r="B577" s="23" t="s">
-        <v>997</v>
+        <v>988</v>
       </c>
       <c r="C577" s="8" t="s">
-        <v>1007</v>
+        <v>998</v>
       </c>
       <c r="D577" s="7" t="s">
         <v>32</v>
@@ -28806,10 +28831,10 @@
         <v>570</v>
       </c>
       <c r="B578" s="23" t="s">
-        <v>997</v>
+        <v>988</v>
       </c>
       <c r="C578" s="8" t="s">
-        <v>1008</v>
+        <v>999</v>
       </c>
       <c r="D578" s="7" t="s">
         <v>32</v>
@@ -28842,10 +28867,10 @@
         <v>571</v>
       </c>
       <c r="B579" s="23" t="s">
-        <v>997</v>
+        <v>988</v>
       </c>
       <c r="C579" s="8" t="s">
-        <v>1008</v>
+        <v>999</v>
       </c>
       <c r="D579" s="7" t="s">
         <v>32</v>
@@ -28878,10 +28903,10 @@
         <v>572</v>
       </c>
       <c r="B580" s="23" t="s">
-        <v>997</v>
+        <v>988</v>
       </c>
       <c r="C580" s="8" t="s">
-        <v>1009</v>
+        <v>1000</v>
       </c>
       <c r="D580" s="7" t="s">
         <v>32</v>
@@ -28914,10 +28939,10 @@
         <v>573</v>
       </c>
       <c r="B581" s="23" t="s">
-        <v>997</v>
+        <v>988</v>
       </c>
       <c r="C581" s="8" t="s">
-        <v>1009</v>
+        <v>1000</v>
       </c>
       <c r="D581" s="7" t="s">
         <v>32</v>
@@ -28950,10 +28975,10 @@
         <v>574</v>
       </c>
       <c r="B582" s="23" t="s">
-        <v>997</v>
+        <v>988</v>
       </c>
       <c r="C582" s="8" t="s">
-        <v>1010</v>
+        <v>1001</v>
       </c>
       <c r="D582" s="7" t="s">
         <v>37</v>
@@ -28986,10 +29011,10 @@
         <v>575</v>
       </c>
       <c r="B583" s="23" t="s">
-        <v>997</v>
+        <v>988</v>
       </c>
       <c r="C583" s="8" t="s">
-        <v>1010</v>
+        <v>1001</v>
       </c>
       <c r="D583" s="7" t="s">
         <v>37</v>
@@ -29022,10 +29047,10 @@
         <v>576</v>
       </c>
       <c r="B584" s="23" t="s">
-        <v>997</v>
+        <v>988</v>
       </c>
       <c r="C584" s="8" t="s">
-        <v>1011</v>
+        <v>1002</v>
       </c>
       <c r="D584" s="7" t="s">
         <v>37</v>
@@ -29058,10 +29083,10 @@
         <v>577</v>
       </c>
       <c r="B585" s="23" t="s">
-        <v>997</v>
+        <v>988</v>
       </c>
       <c r="C585" s="8" t="s">
-        <v>1012</v>
+        <v>1003</v>
       </c>
       <c r="D585" s="7" t="s">
         <v>37</v>
@@ -29094,10 +29119,10 @@
         <v>578</v>
       </c>
       <c r="B586" s="23" t="s">
-        <v>997</v>
+        <v>988</v>
       </c>
       <c r="C586" s="8" t="s">
-        <v>1013</v>
+        <v>1004</v>
       </c>
       <c r="D586" s="7" t="s">
         <v>41</v>
@@ -29130,10 +29155,10 @@
         <v>579</v>
       </c>
       <c r="B587" s="23" t="s">
-        <v>997</v>
+        <v>988</v>
       </c>
       <c r="C587" s="8" t="s">
-        <v>1013</v>
+        <v>1004</v>
       </c>
       <c r="D587" s="7" t="s">
         <v>41</v>
@@ -29166,10 +29191,10 @@
         <v>580</v>
       </c>
       <c r="B588" s="23" t="s">
-        <v>997</v>
+        <v>988</v>
       </c>
       <c r="C588" s="8" t="s">
-        <v>1014</v>
+        <v>1005</v>
       </c>
       <c r="D588" s="7" t="s">
         <v>41</v>
@@ -29202,10 +29227,10 @@
         <v>581</v>
       </c>
       <c r="B589" s="23" t="s">
-        <v>997</v>
+        <v>988</v>
       </c>
       <c r="C589" s="8" t="s">
-        <v>1014</v>
+        <v>1005</v>
       </c>
       <c r="D589" s="7" t="s">
         <v>41</v>
@@ -29238,10 +29263,10 @@
         <v>582</v>
       </c>
       <c r="B590" s="39" t="s">
-        <v>1015</v>
+        <v>1006</v>
       </c>
       <c r="C590" s="8" t="s">
-        <v>1016</v>
+        <v>1007</v>
       </c>
       <c r="D590" s="7" t="s">
         <v>87</v>
@@ -29253,7 +29278,7 @@
         <v>1</v>
       </c>
       <c r="H590" s="13" t="s">
-        <v>1017</v>
+        <v>1008</v>
       </c>
       <c r="M590" s="9" t="str" cm="1">
         <f t="array" ref="M590">PAGE_NAME(B590)</f>
@@ -29270,10 +29295,10 @@
         <v>583</v>
       </c>
       <c r="B591" s="39" t="s">
-        <v>1015</v>
+        <v>1006</v>
       </c>
       <c r="C591" s="8" t="s">
-        <v>1016</v>
+        <v>1007</v>
       </c>
       <c r="D591" s="7" t="s">
         <v>87</v>
@@ -29285,7 +29310,7 @@
         <v>1</v>
       </c>
       <c r="H591" s="13" t="s">
-        <v>1017</v>
+        <v>1008</v>
       </c>
       <c r="M591" s="9" t="str" cm="1">
         <f t="array" ref="M591">PAGE_NAME(B591)</f>
@@ -29302,10 +29327,10 @@
         <v>584</v>
       </c>
       <c r="B592" s="11" t="s">
-        <v>1018</v>
+        <v>1009</v>
       </c>
       <c r="C592" s="8" t="s">
-        <v>1019</v>
+        <v>1010</v>
       </c>
       <c r="D592" s="7" t="s">
         <v>32</v>
@@ -29317,7 +29342,7 @@
         <v>1</v>
       </c>
       <c r="H592" s="13" t="s">
-        <v>944</v>
+        <v>935</v>
       </c>
       <c r="M592" s="9" t="str" cm="1">
         <f t="array" ref="M592">PAGE_NAME(B592)</f>
@@ -29345,7 +29370,7 @@
         <v>327</v>
       </c>
       <c r="C593" s="8" t="s">
-        <v>1020</v>
+        <v>1011</v>
       </c>
       <c r="D593" s="7" t="s">
         <v>41</v>
@@ -29381,7 +29406,7 @@
         <v>327</v>
       </c>
       <c r="C594" s="8" t="s">
-        <v>1021</v>
+        <v>1012</v>
       </c>
       <c r="D594" s="7" t="s">
         <v>41</v>
@@ -29414,10 +29439,10 @@
         <v>702</v>
       </c>
       <c r="B595" s="23" t="s">
-        <v>1022</v>
+        <v>1013</v>
       </c>
       <c r="C595" s="8" t="s">
-        <v>1023</v>
+        <v>1014</v>
       </c>
       <c r="D595" s="7" t="s">
         <v>37</v>
@@ -29445,7 +29470,7 @@
         <v/>
       </c>
       <c r="U595" s="13" t="s">
-        <v>1024</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="596" spans="1:21" ht="51" x14ac:dyDescent="0.2">
@@ -29453,10 +29478,10 @@
         <v>703</v>
       </c>
       <c r="B596" s="23" t="s">
-        <v>1022</v>
+        <v>1013</v>
       </c>
       <c r="C596" s="8" t="s">
-        <v>1025</v>
+        <v>1016</v>
       </c>
       <c r="D596" s="7" t="s">
         <v>37</v>
@@ -29484,7 +29509,7 @@
         <v/>
       </c>
       <c r="U596" s="13" t="s">
-        <v>1026</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="597" spans="1:21" x14ac:dyDescent="0.2">
@@ -29541,7 +29566,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C323F474-BE25-4449-9222-E1A46A1843B5}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -29553,7 +29578,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="409.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="69" t="s">
-        <v>1027</v>
+        <v>1018</v>
       </c>
       <c r="B1" s="70"/>
     </row>
@@ -29563,84 +29588,84 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="15" t="s">
-        <v>1028</v>
+        <v>1019</v>
       </c>
       <c r="B3" t="s">
-        <v>1059</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="15" t="s">
-        <v>1029</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="15" t="s">
-        <v>1030</v>
+        <v>1021</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>1031</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="15" t="s">
-        <v>1032</v>
+        <v>1023</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>1033</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="15" t="s">
-        <v>1034</v>
+        <v>1025</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>1035</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="15" t="s">
-        <v>1036</v>
+        <v>1027</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>1037</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A9" s="15" t="s">
-        <v>1038</v>
+        <v>1029</v>
       </c>
       <c r="B9" s="31" t="s">
-        <v>1039</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="15" t="s">
-        <v>1040</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="153" x14ac:dyDescent="0.2">
       <c r="A11" s="15" t="s">
-        <v>1041</v>
+        <v>1032</v>
       </c>
       <c r="B11" s="31" t="s">
-        <v>1042</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="15" t="s">
-        <v>1043</v>
+        <v>1034</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>1044</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="15" t="s">
-        <v>1045</v>
+        <v>1036</v>
       </c>
       <c r="B13" s="32" t="s">
-        <v>1046</v>
+        <v>1037</v>
       </c>
     </row>
   </sheetData>
@@ -29671,19 +29696,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
-        <v>1030</v>
+        <v>1021</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>1047</v>
+        <v>1038</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>1048</v>
+        <v>1039</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>1049</v>
+        <v>1040</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>1050</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -29691,13 +29716,13 @@
         <v>0.1</v>
       </c>
       <c r="B2" t="s">
-        <v>1051</v>
+        <v>1042</v>
       </c>
       <c r="C2" s="44" t="s">
-        <v>1052</v>
+        <v>1043</v>
       </c>
       <c r="D2" t="s">
-        <v>1053</v>
+        <v>1044</v>
       </c>
       <c r="E2" s="45">
         <v>45618</v>
@@ -29723,13 +29748,13 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>1054</v>
+        <v>1045</v>
       </c>
       <c r="B1" t="s">
         <v>14</v>
       </c>
       <c r="C1" t="s">
-        <v>1055</v>
+        <v>1046</v>
       </c>
       <c r="D1" t="s">
         <v>16</v>
@@ -29746,7 +29771,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>1056</v>
+        <v>1047</v>
       </c>
       <c r="D2" t="s">
         <v>53</v>
@@ -29763,7 +29788,7 @@
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>1057</v>
+        <v>1048</v>
       </c>
       <c r="D3" t="s">
         <v>52</v>
@@ -29777,7 +29802,7 @@
         <v>41</v>
       </c>
       <c r="C4" t="s">
-        <v>1058</v>
+        <v>1049</v>
       </c>
       <c r="E4" t="s">
         <v>55</v>
@@ -29796,7 +29821,7 @@
         <v>75</v>
       </c>
       <c r="E6" t="s">
-        <v>877</v>
+        <v>870</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -29810,6 +29835,28 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="b5a44311-ed64-4a72-909f-c9dc6973bde2" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="eebd8b74-b9de-41b2-9247-c010c4973c2b">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <Description xmlns="eebd8b74-b9de-41b2-9247-c010c4973c2b" xsi:nil="true"/>
+    <SortOrder xmlns="eebd8b74-b9de-41b2-9247-c010c4973c2b" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EC335ED7BB179244BF94A0DFE64544DC" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d3a0f66abe5d2a0564332877ab55d3f7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="eebd8b74-b9de-41b2-9247-c010c4973c2b" xmlns:ns3="b7009bbd-f938-489b-a530-f05273710fff" xmlns:ns4="b5a44311-ed64-4a72-909f-c9dc6973bde2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ec7ca2ee893ff8a0f61d4046c6461645" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="eebd8b74-b9de-41b2-9247-c010c4973c2b"/>
@@ -30063,29 +30110,33 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19B0E317-5E0E-4728-AB3F-40F2C2B957FB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="eebd8b74-b9de-41b2-9247-c010c4973c2b"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="b7009bbd-f938-489b-a530-f05273710fff"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="b5a44311-ed64-4a72-909f-c9dc6973bde2"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="b5a44311-ed64-4a72-909f-c9dc6973bde2" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="eebd8b74-b9de-41b2-9247-c010c4973c2b">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <Description xmlns="eebd8b74-b9de-41b2-9247-c010c4973c2b" xsi:nil="true"/>
-    <SortOrder xmlns="eebd8b74-b9de-41b2-9247-c010c4973c2b" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA84097F-5807-4DCF-92C6-48C9EE26CFB8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C0B0A19-6928-4F0B-831A-5B9FDDD3F6CE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -30103,30 +30154,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA84097F-5807-4DCF-92C6-48C9EE26CFB8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19B0E317-5E0E-4728-AB3F-40F2C2B957FB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="eebd8b74-b9de-41b2-9247-c010c4973c2b"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="b7009bbd-f938-489b-a530-f05273710fff"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="b5a44311-ed64-4a72-909f-c9dc6973bde2"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
updated based on comments. made same updates in v6.1.0 and v7.0.0. regenerated csv and coverage files.
</commit_message>
<xml_diff>
--- a/lib/us_core_test_kit/requirements/hl7.fhir.us.core_6.1.0_reqs.xlsx
+++ b/lib/us_core_test_kit/requirements/hl7.fhir.us.core_6.1.0_reqs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/edeyoung/Documents/inferno/us-core-test-kit/lib/us_core_test_kit/requirements/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9938CB48-E2A5-3A4B-A7F0-7485136FD2D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF5115A0-60B2-374F-97AE-A6FAC6940F09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1780" yWindow="760" windowWidth="27360" windowHeight="18880" firstSheet="1" activeTab="1" xr2:uid="{D251129A-65BB-5042-909C-749E11B8C0B0}"/>
   </bookViews>
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -99,7 +99,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3044" uniqueCount="1061">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3045" uniqueCount="1062">
   <si>
     <r>
       <rPr>
@@ -4874,6 +4874,9 @@
   </si>
   <si>
     <t>Although Patient.deceased[x] is marked as additional USCDI, certifying systems are not required to support both [boolean and dateTime data types], but SHALL support [at] least Patient.deceasedDateTime</t>
+  </si>
+  <si>
+    <t>Duplicate to req 1</t>
   </si>
 </sst>
 </file>
@@ -5537,6 +5540,9 @@
     <xf numFmtId="0" fontId="18" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="24" fillId="11" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -5554,9 +5560,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="11" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -5931,14 +5934,14 @@
       <c r="C3" s="28"/>
     </row>
     <row r="4" spans="1:3" ht="409.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="65" t="s">
+      <c r="A4" s="66" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="47"/>
       <c r="C4" s="29"/>
     </row>
     <row r="5" spans="1:3" ht="258" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="65"/>
+      <c r="A5" s="66"/>
       <c r="B5" s="48"/>
       <c r="C5" s="28"/>
     </row>
@@ -5950,19 +5953,19 @@
       <c r="C6" s="50"/>
     </row>
     <row r="7" spans="1:3" ht="98" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="66" t="s">
+      <c r="A7" s="67" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="67"/>
+      <c r="B7" s="68"/>
       <c r="C7" s="46"/>
     </row>
     <row r="8" spans="1:3" ht="126" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="66"/>
-      <c r="B8" s="68"/>
+      <c r="A8" s="67"/>
+      <c r="B8" s="69"/>
       <c r="C8" s="46"/>
     </row>
     <row r="9" spans="1:3" ht="68" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="65"/>
+      <c r="A9" s="66"/>
       <c r="B9" s="51"/>
       <c r="C9" s="46"/>
     </row>
@@ -5993,10 +5996,10 @@
   <dimension ref="A1:V597"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="8" ySplit="1" topLeftCell="T460" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="8" ySplit="1" topLeftCell="T278" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="U473" sqref="U473"/>
+      <selection pane="bottomRight" activeCell="E280" sqref="E280"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7555,7 +7558,7 @@
         <v>106</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>32</v>
+        <v>87</v>
       </c>
       <c r="E34" s="7" t="s">
         <v>33</v>
@@ -7578,6 +7581,9 @@
       <c r="P34" s="10" t="str">
         <f t="shared" si="1"/>
         <v>Server</v>
+      </c>
+      <c r="T34" s="56" t="s">
+        <v>1061</v>
       </c>
       <c r="U34" s="63"/>
     </row>
@@ -17004,7 +17010,7 @@
         <v>521</v>
       </c>
       <c r="D268" s="7" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="E268" s="7" t="s">
         <v>33</v>
@@ -17071,7 +17077,7 @@
       <c r="Q269" s="10" t="s">
         <v>522</v>
       </c>
-      <c r="T269" s="71" t="s">
+      <c r="T269" s="65" t="s">
         <v>1053</v>
       </c>
       <c r="U269" s="63"/>
@@ -17490,7 +17496,7 @@
         <v>542</v>
       </c>
       <c r="D280" s="7" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="E280" s="7" t="s">
         <v>33</v>
@@ -29577,14 +29583,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="409.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="70" t="s">
         <v>1018</v>
       </c>
-      <c r="B1" s="70"/>
+      <c r="B1" s="71"/>
     </row>
     <row r="2" spans="1:2" ht="82.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="70"/>
-      <c r="B2" s="70"/>
+      <c r="A2" s="71"/>
+      <c r="B2" s="71"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="15" t="s">
@@ -29835,6 +29841,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="b5a44311-ed64-4a72-909f-c9dc6973bde2" xsi:nil="true"/>
@@ -29845,15 +29860,6 @@
     <SortOrder xmlns="eebd8b74-b9de-41b2-9247-c010c4973c2b" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -30111,6 +30117,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA84097F-5807-4DCF-92C6-48C9EE26CFB8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19B0E317-5E0E-4728-AB3F-40F2C2B957FB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
@@ -30124,14 +30138,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="b5a44311-ed64-4a72-909f-c9dc6973bde2"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA84097F-5807-4DCF-92C6-48C9EE26CFB8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Add us core v8.0.0 requirements. (#262)
* Added us core v8.0.0 requirements. In the processes, noted some necessary changes to the v7.0.0 and v6.1.0 requirements. Updated these, regenerated the csv file, and regenerated the coverage file.

* deleted helper column from v8 xlsx

* add some comments

* updated based on comments. made same updates in v6.1.0 and v7.0.0. regenerated csv and coverage files.

* confirm changes to 800_reqs

---------

Co-authored-by: Lizzie Charbonneau <lizzie@mitre.org>
Co-authored-by: Yunwei Wang <>
</commit_message>
<xml_diff>
--- a/lib/us_core_test_kit/requirements/hl7.fhir.us.core_6.1.0_reqs.xlsx
+++ b/lib/us_core_test_kit/requirements/hl7.fhir.us.core_6.1.0_reqs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/knaden/Documents/Inferno/source/us-core-test-kit/lib/us_core_test_kit/requirements/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/edeyoung/Documents/inferno/us-core-test-kit/lib/us_core_test_kit/requirements/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B26E4571-9F78-E84A-88DC-63B5BFA7F593}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF5115A0-60B2-374F-97AE-A6FAC6940F09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1780" yWindow="760" windowWidth="27360" windowHeight="20180" firstSheet="1" activeTab="2" xr2:uid="{D251129A-65BB-5042-909C-749E11B8C0B0}"/>
+    <workbookView xWindow="1780" yWindow="760" windowWidth="27360" windowHeight="18880" firstSheet="1" activeTab="1" xr2:uid="{D251129A-65BB-5042-909C-749E11B8C0B0}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="9" r:id="rId1"/>
@@ -99,7 +99,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3047" uniqueCount="1060">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3045" uniqueCount="1062">
   <si>
     <r>
       <rPr>
@@ -4085,43 +4085,16 @@
     <t>https://hl7.org/fhir/us/core/STU6.1/StructureDefinition-us-core-patient.html#mandatory-and-must-support-data-elements, https://hl7.org/fhir/us/core/STU6.1/StructureDefinition-us-core-race.html#profile-specific-implementation-guidance</t>
   </si>
   <si>
-    <t>[Organizations participating in the ONC Health IT certrification program,] must support at least one category code from OMB Race [category for the [US Core Race Extension] (https://hl7.org/fhir/us/core/STU7/StructureDefinition-us-core-race.html)]</t>
-  </si>
-  <si>
-    <t>For organizations participating in ONC certification, when using the US Core Race Extension</t>
-  </si>
-  <si>
     <t>Deprecating as this is not in US 6.1,</t>
   </si>
   <si>
     <t>https://hl7.org/fhir/us/core/STU6.1/StructureDefinition-us-core-patient.html#mandatory-and-must-support-data-elements, https://hl7.org/fhir/us/core/STU6.1/StructureDefinition-us-core-ethnicity.html#profile-specific-implementation-guidance</t>
   </si>
   <si>
-    <t>[Organizations participating in the ONC Health IT certrification program,] must support at least one category code from OMB … Ethnicity [category for the [US Core Ethnicity Extension] (https://hl7.org/fhir/us/core/STU7/StructureDefinition-us-core-ethnicity.html)]</t>
-  </si>
-  <si>
-    <t>For organizations participating in ONC certification, When using the US Core Ethnicity Extension</t>
-  </si>
-  <si>
-    <t>[Organizations participating in the ONC Health IT certrification program,] MAY include additional detailed codes from CDC Race … codes [when using the [US Core Race Extension] (https://hl7.org/fhir/us/core/STU7/StructureDefinition-us-core-race.html)]</t>
-  </si>
-  <si>
-    <t>For organizations participating in ONC certification, When using the US Core Race Extension</t>
-  </si>
-  <si>
-    <t>[Organizations participating in the ONC Health IT certrification program,] SHALL include a text description [of category codes when using the [US Core Ethnicity Extension] (https://hl7.org/fhir/us/core/STU7/StructureDefinition-us-core-ethnicity.html)]</t>
-  </si>
-  <si>
     <t>Unknown</t>
   </si>
   <si>
     <t>https://hl7.org/fhir/us/core/STU6.1/StructureDefinition-us-core-patient.html#mandatory-and-must-support-data-elements</t>
-  </si>
-  <si>
-    <t>[For Organizations participating in the ONC Health IT certrification program,] Although Patient.deceased[x] is marked as additional USCDI, certifying systems are not required to support both [boolean and dateTime data types], but SHALL support [at] least Patient.deceasedDateTime</t>
-  </si>
-  <si>
-    <t xml:space="preserve">For organizations participating in ONC certification, </t>
   </si>
   <si>
     <t>Previous name is represented by setting Patient.name.use to “old” or providing an end date in Patient.name.period or doing both</t>
@@ -4872,12 +4845,45 @@
   <si>
     <t>hl7.fhir.us.core_6.1.0</t>
   </si>
+  <si>
+    <t>Marked DEPRECATED because this is an example.</t>
+  </si>
+  <si>
+    <t>Duplicate of 254</t>
+  </si>
+  <si>
+    <t>Duplicate of requirement 260</t>
+  </si>
+  <si>
+    <t>The Complex [Extension] for Race ... allow[s] for one or more codes of which must support at least one category code from OMB Race [category for the [US Core Race Extension] (https://hl7.org/fhir/us/core/STU7/StructureDefinition-us-core-race.html)]</t>
+  </si>
+  <si>
+    <t>The Complex [Extension] for ... Ethnicity allow[s] for one or more codes of which must support at least one category code from OMB … Ethnicity [category for the [US Core Ethnicity Extension] (https://hl7.org/fhir/us/core/STU7/StructureDefinition-us-core-ethnicity.html)]</t>
+  </si>
+  <si>
+    <t>The Complex [Extension] for Race ... allow[s] for one or more codes of which MAY include additional detailed codes from CDC Race … codes [when using the [US Core Race Extension] (https://hl7.org/fhir/us/core/STU7/StructureDefinition-us-core-race.html)]</t>
+  </si>
+  <si>
+    <t>The Complex [Extension] for Race ... allow[s] for one or more codes of which SHALL include a text description [of category codes when using the [US Core Race Extension] (https://hl7.org/fhir/us/core/STU7/StructureDefinition-us-core-race.html)]</t>
+  </si>
+  <si>
+    <t>The Complex [Extension] for ... Ethnicity allow[s] for one or more codes of which MAY include additional detailed codes from CDC Race … codes [when using the [US Core Race Extension] (https://hl7.org/fhir/us/core/STU7/StructureDefinition-us-core-race.html)]</t>
+  </si>
+  <si>
+    <t>The Complex [Extension] for ... Ethnicity allow[s] for one or more codes of which SHALL include a text description [of category codes when using the [US Core Ethnicity Extension] (https://hl7.org/fhir/us/core/STU7/StructureDefinition-us-core-ethnicity.html)]</t>
+  </si>
+  <si>
+    <t>Although Patient.deceased[x] is marked as additional USCDI, certifying systems are not required to support both [boolean and dateTime data types], but SHALL support [at] least Patient.deceasedDateTime</t>
+  </si>
+  <si>
+    <t>Duplicate to req 1</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -5041,8 +5047,15 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -5103,8 +5116,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE2EFDA"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="22">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -5359,12 +5378,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFD0CECE"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFD0CECE"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFD0CECE"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFD0CECE"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5504,6 +5538,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="11" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5897,14 +5934,14 @@
       <c r="C3" s="28"/>
     </row>
     <row r="4" spans="1:3" ht="409.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="65" t="s">
+      <c r="A4" s="66" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="47"/>
       <c r="C4" s="29"/>
     </row>
     <row r="5" spans="1:3" ht="258" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="65"/>
+      <c r="A5" s="66"/>
       <c r="B5" s="48"/>
       <c r="C5" s="28"/>
     </row>
@@ -5916,19 +5953,19 @@
       <c r="C6" s="50"/>
     </row>
     <row r="7" spans="1:3" ht="98" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="66" t="s">
+      <c r="A7" s="67" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="67"/>
+      <c r="B7" s="68"/>
       <c r="C7" s="46"/>
     </row>
     <row r="8" spans="1:3" ht="126" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="66"/>
-      <c r="B8" s="68"/>
+      <c r="A8" s="67"/>
+      <c r="B8" s="69"/>
       <c r="C8" s="46"/>
     </row>
     <row r="9" spans="1:3" ht="68" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="65"/>
+      <c r="A9" s="66"/>
       <c r="B9" s="51"/>
       <c r="C9" s="46"/>
     </row>
@@ -5958,11 +5995,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0272D98A-080C-3945-A7E0-CB54FB3A65A9}">
   <dimension ref="A1:V597"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="8" ySplit="1" topLeftCell="S2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="8" ySplit="1" topLeftCell="T278" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="S1" sqref="S1:T1048576"/>
+      <selection pane="bottomRight" activeCell="E280" sqref="E280"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7521,7 +7558,7 @@
         <v>106</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>32</v>
+        <v>87</v>
       </c>
       <c r="E34" s="7" t="s">
         <v>33</v>
@@ -7544,6 +7581,9 @@
       <c r="P34" s="10" t="str">
         <f t="shared" si="1"/>
         <v>Server</v>
+      </c>
+      <c r="T34" s="56" t="s">
+        <v>1061</v>
       </c>
       <c r="U34" s="63"/>
     </row>
@@ -9905,8 +9945,8 @@
       <c r="A94" s="7">
         <v>87</v>
       </c>
-      <c r="B94" s="7" t="s">
-        <v>195</v>
+      <c r="B94" s="23" t="s">
+        <v>209</v>
       </c>
       <c r="C94" s="8" t="s">
         <v>207</v>
@@ -9926,7 +9966,7 @@
       </c>
       <c r="N94" s="9" t="str" cm="1">
         <f t="array" ref="N94">SECTION_NAME(B94)</f>
-        <v>additional-uscdi-requirements</v>
+        <v>defined-pattern-elements</v>
       </c>
       <c r="O94" s="10" t="str">
         <f t="shared" si="4"/>
@@ -9952,7 +9992,7 @@
         <v>210</v>
       </c>
       <c r="D95" s="7" t="s">
-        <v>32</v>
+        <v>87</v>
       </c>
       <c r="E95" s="7" t="s">
         <v>33</v>
@@ -9979,6 +10019,9 @@
         <f t="shared" si="3"/>
         <v>Server</v>
       </c>
+      <c r="T95" s="13" t="s">
+        <v>1051</v>
+      </c>
       <c r="U95" s="63"/>
     </row>
     <row r="96" spans="1:21" ht="187" x14ac:dyDescent="0.2">
@@ -9992,7 +10035,7 @@
         <v>212</v>
       </c>
       <c r="D96" s="7" t="s">
-        <v>32</v>
+        <v>87</v>
       </c>
       <c r="E96" s="7" t="s">
         <v>79</v>
@@ -10018,6 +10061,9 @@
       <c r="P96" s="10" t="str">
         <f t="shared" si="3"/>
         <v>Client</v>
+      </c>
+      <c r="T96" s="13" t="s">
+        <v>1051</v>
       </c>
       <c r="U96" s="63"/>
     </row>
@@ -16764,7 +16810,7 @@
         <v>513</v>
       </c>
       <c r="D263" s="7" t="s">
-        <v>32</v>
+        <v>87</v>
       </c>
       <c r="E263" s="7" t="s">
         <v>33</v>
@@ -16791,6 +16837,9 @@
       <c r="Q263" s="10" t="s">
         <v>514</v>
       </c>
+      <c r="T263" s="56" t="s">
+        <v>1052</v>
+      </c>
       <c r="U263" s="63"/>
     </row>
     <row r="264" spans="1:21" ht="306" x14ac:dyDescent="0.2">
@@ -16961,13 +17010,13 @@
         <v>521</v>
       </c>
       <c r="D268" s="7" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="E268" s="7" t="s">
         <v>33</v>
       </c>
       <c r="G268" s="7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M268" s="9" t="str" cm="1">
         <f t="array" ref="M268">PAGE_NAME(B268)</f>
@@ -17001,7 +17050,7 @@
         <v>521</v>
       </c>
       <c r="D269" s="7" t="s">
-        <v>32</v>
+        <v>87</v>
       </c>
       <c r="E269" s="7" t="s">
         <v>33</v>
@@ -17028,6 +17077,9 @@
       <c r="Q269" s="10" t="s">
         <v>522</v>
       </c>
+      <c r="T269" s="65" t="s">
+        <v>1053</v>
+      </c>
       <c r="U269" s="63"/>
     </row>
     <row r="270" spans="1:21" ht="238" x14ac:dyDescent="0.2">
@@ -17444,7 +17496,7 @@
         <v>542</v>
       </c>
       <c r="D280" s="7" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="E280" s="7" t="s">
         <v>33</v>
@@ -24626,7 +24678,7 @@
         <v>867</v>
       </c>
       <c r="C467" s="8" t="s">
-        <v>868</v>
+        <v>1054</v>
       </c>
       <c r="D467" s="7" t="s">
         <v>87</v>
@@ -24636,9 +24688,6 @@
       </c>
       <c r="G467" s="7" t="b">
         <v>1</v>
-      </c>
-      <c r="H467" s="13" t="s">
-        <v>869</v>
       </c>
       <c r="M467" s="9" t="str" cm="1">
         <f t="array" ref="M467">PAGE_NAME(B467)</f>
@@ -24657,7 +24706,7 @@
         <v/>
       </c>
       <c r="U467" s="13" t="s">
-        <v>870</v>
+        <v>868</v>
       </c>
     </row>
     <row r="468" spans="1:21" ht="102" x14ac:dyDescent="0.2">
@@ -24665,10 +24714,10 @@
         <v>460</v>
       </c>
       <c r="B468" s="23" t="s">
-        <v>871</v>
+        <v>869</v>
       </c>
       <c r="C468" s="8" t="s">
-        <v>872</v>
+        <v>1055</v>
       </c>
       <c r="D468" s="7" t="s">
         <v>87</v>
@@ -24678,9 +24727,6 @@
       </c>
       <c r="G468" s="7" t="b">
         <v>1</v>
-      </c>
-      <c r="H468" s="13" t="s">
-        <v>873</v>
       </c>
       <c r="M468" s="9" t="str" cm="1">
         <f t="array" ref="M468">PAGE_NAME(B468)</f>
@@ -24699,7 +24745,7 @@
         <v/>
       </c>
       <c r="U468" s="13" t="s">
-        <v>870</v>
+        <v>868</v>
       </c>
     </row>
     <row r="469" spans="1:21" ht="102" x14ac:dyDescent="0.2">
@@ -24710,7 +24756,7 @@
         <v>867</v>
       </c>
       <c r="C469" s="8" t="s">
-        <v>874</v>
+        <v>1056</v>
       </c>
       <c r="D469" s="7" t="s">
         <v>87</v>
@@ -24720,9 +24766,6 @@
       </c>
       <c r="G469" s="7" t="b">
         <v>1</v>
-      </c>
-      <c r="H469" s="13" t="s">
-        <v>875</v>
       </c>
       <c r="M469" s="9" t="str" cm="1">
         <f t="array" ref="M469">PAGE_NAME(B469)</f>
@@ -24741,7 +24784,7 @@
         <v/>
       </c>
       <c r="U469" s="13" t="s">
-        <v>870</v>
+        <v>868</v>
       </c>
     </row>
     <row r="470" spans="1:21" ht="102" x14ac:dyDescent="0.2">
@@ -24749,10 +24792,10 @@
         <v>462</v>
       </c>
       <c r="B470" s="23" t="s">
-        <v>871</v>
+        <v>869</v>
       </c>
       <c r="C470" s="8" t="s">
-        <v>876</v>
+        <v>1057</v>
       </c>
       <c r="D470" s="7" t="s">
         <v>87</v>
@@ -24762,9 +24805,6 @@
       </c>
       <c r="G470" s="7" t="b">
         <v>1</v>
-      </c>
-      <c r="H470" s="13" t="s">
-        <v>873</v>
       </c>
       <c r="M470" s="9" t="str" cm="1">
         <f t="array" ref="M470">PAGE_NAME(B470)</f>
@@ -24783,7 +24823,7 @@
         <v/>
       </c>
       <c r="U470" s="13" t="s">
-        <v>870</v>
+        <v>868</v>
       </c>
     </row>
     <row r="471" spans="1:21" ht="102" x14ac:dyDescent="0.2">
@@ -24794,7 +24834,7 @@
         <v>867</v>
       </c>
       <c r="C471" s="8" t="s">
-        <v>874</v>
+        <v>1058</v>
       </c>
       <c r="D471" s="7" t="s">
         <v>87</v>
@@ -24804,9 +24844,6 @@
       </c>
       <c r="G471" s="7" t="b">
         <v>1</v>
-      </c>
-      <c r="H471" s="13" t="s">
-        <v>875</v>
       </c>
       <c r="M471" s="9" t="str" cm="1">
         <f t="array" ref="M471">PAGE_NAME(B471)</f>
@@ -24825,7 +24862,7 @@
         <v/>
       </c>
       <c r="U471" s="13" t="s">
-        <v>870</v>
+        <v>868</v>
       </c>
     </row>
     <row r="472" spans="1:21" ht="102" x14ac:dyDescent="0.2">
@@ -24833,10 +24870,10 @@
         <v>464</v>
       </c>
       <c r="B472" s="23" t="s">
-        <v>871</v>
+        <v>869</v>
       </c>
       <c r="C472" s="8" t="s">
-        <v>876</v>
+        <v>1059</v>
       </c>
       <c r="D472" s="7" t="s">
         <v>87</v>
@@ -24846,9 +24883,6 @@
       </c>
       <c r="G472" s="7" t="b">
         <v>1</v>
-      </c>
-      <c r="H472" s="13" t="s">
-        <v>873</v>
       </c>
       <c r="M472" s="9" t="str" cm="1">
         <f t="array" ref="M472">PAGE_NAME(B472)</f>
@@ -24867,27 +24901,24 @@
         <v/>
       </c>
       <c r="U472" s="13" t="s">
-        <v>870</v>
-      </c>
-    </row>
-    <row r="473" spans="1:21" ht="119" x14ac:dyDescent="0.2">
+        <v>868</v>
+      </c>
+    </row>
+    <row r="473" spans="1:21" ht="85" x14ac:dyDescent="0.2">
       <c r="A473" s="7">
         <v>465</v>
       </c>
       <c r="B473" s="23" t="s">
-        <v>878</v>
+        <v>871</v>
       </c>
       <c r="C473" s="8" t="s">
-        <v>879</v>
+        <v>1060</v>
       </c>
       <c r="D473" s="7" t="s">
         <v>87</v>
       </c>
       <c r="E473" s="7" t="s">
         <v>33</v>
-      </c>
-      <c r="H473" s="13" t="s">
-        <v>880</v>
       </c>
       <c r="M473" s="9" t="str" cm="1">
         <f t="array" ref="M473">PAGE_NAME(B473)</f>
@@ -24906,7 +24937,7 @@
         <v/>
       </c>
       <c r="U473" s="13" t="s">
-        <v>870</v>
+        <v>868</v>
       </c>
     </row>
     <row r="474" spans="1:21" ht="85" x14ac:dyDescent="0.2">
@@ -24914,10 +24945,10 @@
         <v>466</v>
       </c>
       <c r="B474" s="23" t="s">
-        <v>878</v>
+        <v>871</v>
       </c>
       <c r="C474" s="8" t="s">
-        <v>881</v>
+        <v>872</v>
       </c>
       <c r="D474" s="7" t="s">
         <v>37</v>
@@ -24929,7 +24960,7 @@
         <v>1</v>
       </c>
       <c r="H474" s="13" t="s">
-        <v>882</v>
+        <v>873</v>
       </c>
       <c r="O474" s="10" t="str">
         <f t="shared" si="23"/>
@@ -24945,10 +24976,10 @@
         <v>467</v>
       </c>
       <c r="B475" s="23" t="s">
-        <v>878</v>
+        <v>871</v>
       </c>
       <c r="C475" s="8" t="s">
-        <v>883</v>
+        <v>874</v>
       </c>
       <c r="D475" s="7" t="s">
         <v>37</v>
@@ -24960,7 +24991,7 @@
         <v>1</v>
       </c>
       <c r="H475" s="13" t="s">
-        <v>884</v>
+        <v>875</v>
       </c>
       <c r="M475" s="9" t="str" cm="1">
         <f t="array" ref="M475">PAGE_NAME(B475)</f>
@@ -24984,10 +25015,10 @@
         <v>468</v>
       </c>
       <c r="B476" s="23" t="s">
-        <v>878</v>
+        <v>871</v>
       </c>
       <c r="C476" s="8" t="s">
-        <v>885</v>
+        <v>876</v>
       </c>
       <c r="D476" s="7" t="s">
         <v>41</v>
@@ -25020,10 +25051,10 @@
         <v>469</v>
       </c>
       <c r="B477" s="23" t="s">
-        <v>878</v>
+        <v>871</v>
       </c>
       <c r="C477" s="8" t="s">
-        <v>886</v>
+        <v>877</v>
       </c>
       <c r="D477" s="7" t="s">
         <v>87</v>
@@ -25059,10 +25090,10 @@
         <v>470</v>
       </c>
       <c r="B478" s="23" t="s">
+        <v>871</v>
+      </c>
+      <c r="C478" s="8" t="s">
         <v>878</v>
-      </c>
-      <c r="C478" s="8" t="s">
-        <v>887</v>
       </c>
       <c r="D478" s="7" t="s">
         <v>87</v>
@@ -25098,10 +25129,10 @@
         <v>471</v>
       </c>
       <c r="B479" s="23" t="s">
-        <v>878</v>
+        <v>871</v>
       </c>
       <c r="C479" s="8" t="s">
-        <v>888</v>
+        <v>879</v>
       </c>
       <c r="D479" s="7" t="s">
         <v>87</v>
@@ -25113,7 +25144,7 @@
         <v>1</v>
       </c>
       <c r="H479" s="13" t="s">
-        <v>889</v>
+        <v>880</v>
       </c>
       <c r="M479" s="9" t="str" cm="1">
         <f t="array" ref="M479">PAGE_NAME(B479)</f>
@@ -25140,10 +25171,10 @@
         <v>472</v>
       </c>
       <c r="B480" s="23" t="s">
-        <v>878</v>
+        <v>871</v>
       </c>
       <c r="C480" s="8" t="s">
-        <v>890</v>
+        <v>881</v>
       </c>
       <c r="D480" s="7" t="s">
         <v>112</v>
@@ -25176,10 +25207,10 @@
         <v>473</v>
       </c>
       <c r="B481" s="23" t="s">
-        <v>891</v>
+        <v>882</v>
       </c>
       <c r="C481" s="8" t="s">
-        <v>892</v>
+        <v>883</v>
       </c>
       <c r="D481" s="7" t="s">
         <v>32</v>
@@ -25191,7 +25222,7 @@
         <v>1</v>
       </c>
       <c r="H481" s="13" t="s">
-        <v>893</v>
+        <v>884</v>
       </c>
       <c r="M481" s="9" t="str" cm="1">
         <f t="array" ref="M481">PAGE_NAME(B481)</f>
@@ -25215,10 +25246,10 @@
         <v>474</v>
       </c>
       <c r="B482" s="23" t="s">
-        <v>891</v>
+        <v>882</v>
       </c>
       <c r="C482" s="8" t="s">
-        <v>894</v>
+        <v>885</v>
       </c>
       <c r="D482" s="7" t="s">
         <v>87</v>
@@ -25230,7 +25261,7 @@
         <v>1</v>
       </c>
       <c r="H482" s="13" t="s">
-        <v>895</v>
+        <v>886</v>
       </c>
       <c r="M482" s="9" t="str" cm="1">
         <f t="array" ref="M482">PAGE_NAME(B482)</f>
@@ -25249,7 +25280,7 @@
         <v>Server</v>
       </c>
       <c r="U482" s="13" t="s">
-        <v>870</v>
+        <v>868</v>
       </c>
     </row>
     <row r="483" spans="1:21" ht="68" x14ac:dyDescent="0.2">
@@ -25257,10 +25288,10 @@
         <v>475</v>
       </c>
       <c r="B483" s="23" t="s">
-        <v>891</v>
+        <v>882</v>
       </c>
       <c r="C483" s="8" t="s">
-        <v>896</v>
+        <v>887</v>
       </c>
       <c r="D483" s="7" t="s">
         <v>87</v>
@@ -25272,7 +25303,7 @@
         <v>1</v>
       </c>
       <c r="H483" s="13" t="s">
-        <v>897</v>
+        <v>888</v>
       </c>
       <c r="M483" s="9" t="str" cm="1">
         <f t="array" ref="M483">PAGE_NAME(B483)</f>
@@ -25291,7 +25322,7 @@
         <v>Server</v>
       </c>
       <c r="U483" s="13" t="s">
-        <v>870</v>
+        <v>868</v>
       </c>
     </row>
     <row r="484" spans="1:21" ht="51" x14ac:dyDescent="0.2">
@@ -25299,10 +25330,10 @@
         <v>476</v>
       </c>
       <c r="B484" s="23" t="s">
-        <v>891</v>
+        <v>882</v>
       </c>
       <c r="C484" s="8" t="s">
-        <v>898</v>
+        <v>889</v>
       </c>
       <c r="D484" s="7" t="s">
         <v>87</v>
@@ -25327,7 +25358,7 @@
         <v>Client</v>
       </c>
       <c r="U484" s="13" t="s">
-        <v>899</v>
+        <v>890</v>
       </c>
     </row>
     <row r="485" spans="1:21" ht="51" x14ac:dyDescent="0.2">
@@ -25335,10 +25366,10 @@
         <v>477</v>
       </c>
       <c r="B485" s="23" t="s">
+        <v>882</v>
+      </c>
+      <c r="C485" s="8" t="s">
         <v>891</v>
-      </c>
-      <c r="C485" s="8" t="s">
-        <v>900</v>
       </c>
       <c r="D485" s="7" t="s">
         <v>37</v>
@@ -25371,10 +25402,10 @@
         <v>478</v>
       </c>
       <c r="B486" s="23" t="s">
-        <v>891</v>
+        <v>882</v>
       </c>
       <c r="C486" s="8" t="s">
-        <v>901</v>
+        <v>892</v>
       </c>
       <c r="D486" s="7" t="s">
         <v>87</v>
@@ -25410,10 +25441,10 @@
         <v>479</v>
       </c>
       <c r="B487" s="23" t="s">
-        <v>902</v>
+        <v>893</v>
       </c>
       <c r="C487" s="8" t="s">
-        <v>903</v>
+        <v>894</v>
       </c>
       <c r="D487" s="7" t="s">
         <v>41</v>
@@ -25446,10 +25477,10 @@
         <v>480</v>
       </c>
       <c r="B488" s="23" t="s">
-        <v>902</v>
+        <v>893</v>
       </c>
       <c r="C488" s="8" t="s">
-        <v>904</v>
+        <v>895</v>
       </c>
       <c r="D488" s="7" t="s">
         <v>37</v>
@@ -25461,7 +25492,7 @@
         <v>1</v>
       </c>
       <c r="H488" s="13" t="s">
-        <v>905</v>
+        <v>896</v>
       </c>
       <c r="M488" s="9" t="str" cm="1">
         <f t="array" ref="M488">PAGE_NAME(B488)</f>
@@ -25485,10 +25516,10 @@
         <v>481</v>
       </c>
       <c r="B489" s="23" t="s">
-        <v>902</v>
+        <v>893</v>
       </c>
       <c r="C489" s="8" t="s">
-        <v>906</v>
+        <v>897</v>
       </c>
       <c r="D489" s="7" t="s">
         <v>37</v>
@@ -25521,10 +25552,10 @@
         <v>482</v>
       </c>
       <c r="B490" s="23" t="s">
-        <v>902</v>
+        <v>893</v>
       </c>
       <c r="C490" s="8" t="s">
-        <v>907</v>
+        <v>898</v>
       </c>
       <c r="D490" s="7" t="s">
         <v>87</v>
@@ -25536,7 +25567,7 @@
         <v>1</v>
       </c>
       <c r="H490" s="13" t="s">
-        <v>908</v>
+        <v>899</v>
       </c>
       <c r="M490" s="9" t="str" cm="1">
         <f t="array" ref="M490">PAGE_NAME(B490)</f>
@@ -25555,7 +25586,7 @@
         <v>Server</v>
       </c>
       <c r="U490" s="13" t="s">
-        <v>899</v>
+        <v>890</v>
       </c>
     </row>
     <row r="491" spans="1:21" ht="85" x14ac:dyDescent="0.2">
@@ -25563,10 +25594,10 @@
         <v>483</v>
       </c>
       <c r="B491" s="23" t="s">
-        <v>902</v>
+        <v>893</v>
       </c>
       <c r="C491" s="8" t="s">
-        <v>909</v>
+        <v>900</v>
       </c>
       <c r="D491" s="7" t="s">
         <v>87</v>
@@ -25578,7 +25609,7 @@
         <v>1</v>
       </c>
       <c r="H491" s="13" t="s">
-        <v>908</v>
+        <v>899</v>
       </c>
       <c r="M491" s="9" t="str" cm="1">
         <f t="array" ref="M491">PAGE_NAME(B491)</f>
@@ -25597,7 +25628,7 @@
         <v>Client</v>
       </c>
       <c r="U491" s="13" t="s">
-        <v>899</v>
+        <v>890</v>
       </c>
     </row>
     <row r="492" spans="1:21" ht="119" x14ac:dyDescent="0.2">
@@ -25605,10 +25636,10 @@
         <v>484</v>
       </c>
       <c r="B492" s="23" t="s">
-        <v>902</v>
+        <v>893</v>
       </c>
       <c r="C492" s="8" t="s">
-        <v>910</v>
+        <v>901</v>
       </c>
       <c r="D492" s="7" t="s">
         <v>87</v>
@@ -25620,7 +25651,7 @@
         <v>1</v>
       </c>
       <c r="H492" s="13" t="s">
-        <v>911</v>
+        <v>902</v>
       </c>
       <c r="M492" s="9" t="str" cm="1">
         <f t="array" ref="M492">PAGE_NAME(B492)</f>
@@ -25639,7 +25670,7 @@
         <v>Server</v>
       </c>
       <c r="U492" s="13" t="s">
-        <v>899</v>
+        <v>890</v>
       </c>
     </row>
     <row r="493" spans="1:21" ht="85" x14ac:dyDescent="0.2">
@@ -25647,10 +25678,10 @@
         <v>485</v>
       </c>
       <c r="B493" s="23" t="s">
-        <v>902</v>
+        <v>893</v>
       </c>
       <c r="C493" s="8" t="s">
-        <v>912</v>
+        <v>903</v>
       </c>
       <c r="D493" s="7" t="s">
         <v>87</v>
@@ -25662,7 +25693,7 @@
         <v>1</v>
       </c>
       <c r="H493" s="13" t="s">
-        <v>908</v>
+        <v>899</v>
       </c>
       <c r="M493" s="9" t="str" cm="1">
         <f t="array" ref="M493">PAGE_NAME(B493)</f>
@@ -25681,7 +25712,7 @@
         <v>Client</v>
       </c>
       <c r="U493" s="13" t="s">
-        <v>899</v>
+        <v>890</v>
       </c>
     </row>
     <row r="494" spans="1:21" ht="85" x14ac:dyDescent="0.2">
@@ -25689,10 +25720,10 @@
         <v>486</v>
       </c>
       <c r="B494" s="23" t="s">
-        <v>902</v>
+        <v>893</v>
       </c>
       <c r="C494" s="8" t="s">
-        <v>913</v>
+        <v>904</v>
       </c>
       <c r="D494" s="7" t="s">
         <v>87</v>
@@ -25704,7 +25735,7 @@
         <v>1</v>
       </c>
       <c r="H494" s="13" t="s">
-        <v>914</v>
+        <v>905</v>
       </c>
       <c r="M494" s="9" t="str" cm="1">
         <f t="array" ref="M494">PAGE_NAME(B494)</f>
@@ -25723,7 +25754,7 @@
         <v>Server</v>
       </c>
       <c r="U494" s="13" t="s">
-        <v>899</v>
+        <v>890</v>
       </c>
     </row>
     <row r="495" spans="1:21" ht="85" x14ac:dyDescent="0.2">
@@ -25731,10 +25762,10 @@
         <v>487</v>
       </c>
       <c r="B495" s="23" t="s">
-        <v>902</v>
+        <v>893</v>
       </c>
       <c r="C495" s="8" t="s">
-        <v>915</v>
+        <v>906</v>
       </c>
       <c r="D495" s="7" t="s">
         <v>87</v>
@@ -25746,7 +25777,7 @@
         <v>1</v>
       </c>
       <c r="H495" s="13" t="s">
-        <v>914</v>
+        <v>905</v>
       </c>
       <c r="M495" s="9" t="str" cm="1">
         <f t="array" ref="M495">PAGE_NAME(B495)</f>
@@ -25765,7 +25796,7 @@
         <v>Client</v>
       </c>
       <c r="U495" s="13" t="s">
-        <v>899</v>
+        <v>890</v>
       </c>
     </row>
     <row r="496" spans="1:21" ht="119" x14ac:dyDescent="0.2">
@@ -25773,10 +25804,10 @@
         <v>488</v>
       </c>
       <c r="B496" s="23" t="s">
-        <v>902</v>
+        <v>893</v>
       </c>
       <c r="C496" s="8" t="s">
-        <v>916</v>
+        <v>907</v>
       </c>
       <c r="D496" s="7" t="s">
         <v>87</v>
@@ -25788,7 +25819,7 @@
         <v>1</v>
       </c>
       <c r="H496" s="13" t="s">
-        <v>914</v>
+        <v>905</v>
       </c>
       <c r="M496" s="9" t="str" cm="1">
         <f t="array" ref="M496">PAGE_NAME(B496)</f>
@@ -25807,7 +25838,7 @@
         <v/>
       </c>
       <c r="U496" s="13" t="s">
-        <v>899</v>
+        <v>890</v>
       </c>
     </row>
     <row r="497" spans="1:16" ht="51" x14ac:dyDescent="0.2">
@@ -25815,10 +25846,10 @@
         <v>489</v>
       </c>
       <c r="B497" s="23" t="s">
-        <v>917</v>
+        <v>908</v>
       </c>
       <c r="C497" s="8" t="s">
-        <v>918</v>
+        <v>909</v>
       </c>
       <c r="D497" s="7" t="s">
         <v>32</v>
@@ -25851,10 +25882,10 @@
         <v>490</v>
       </c>
       <c r="B498" s="23" t="s">
-        <v>917</v>
+        <v>908</v>
       </c>
       <c r="C498" s="8" t="s">
-        <v>919</v>
+        <v>910</v>
       </c>
       <c r="D498" s="7" t="s">
         <v>32</v>
@@ -25887,10 +25918,10 @@
         <v>491</v>
       </c>
       <c r="B499" s="23" t="s">
-        <v>917</v>
+        <v>908</v>
       </c>
       <c r="C499" s="8" t="s">
-        <v>920</v>
+        <v>911</v>
       </c>
       <c r="D499" s="7" t="s">
         <v>32</v>
@@ -25923,10 +25954,10 @@
         <v>492</v>
       </c>
       <c r="B500" s="23" t="s">
-        <v>917</v>
+        <v>908</v>
       </c>
       <c r="C500" s="8" t="s">
-        <v>921</v>
+        <v>912</v>
       </c>
       <c r="D500" s="7" t="s">
         <v>32</v>
@@ -25959,10 +25990,10 @@
         <v>493</v>
       </c>
       <c r="B501" s="23" t="s">
-        <v>917</v>
+        <v>908</v>
       </c>
       <c r="C501" s="8" t="s">
-        <v>922</v>
+        <v>913</v>
       </c>
       <c r="D501" s="7" t="s">
         <v>32</v>
@@ -25995,10 +26026,10 @@
         <v>494</v>
       </c>
       <c r="B502" s="23" t="s">
-        <v>917</v>
+        <v>908</v>
       </c>
       <c r="C502" s="8" t="s">
-        <v>923</v>
+        <v>914</v>
       </c>
       <c r="D502" s="7" t="s">
         <v>32</v>
@@ -26031,10 +26062,10 @@
         <v>495</v>
       </c>
       <c r="B503" s="23" t="s">
-        <v>917</v>
+        <v>908</v>
       </c>
       <c r="C503" s="8" t="s">
-        <v>924</v>
+        <v>915</v>
       </c>
       <c r="D503" s="7" t="s">
         <v>32</v>
@@ -26067,10 +26098,10 @@
         <v>496</v>
       </c>
       <c r="B504" s="23" t="s">
-        <v>917</v>
+        <v>908</v>
       </c>
       <c r="C504" s="8" t="s">
-        <v>925</v>
+        <v>916</v>
       </c>
       <c r="D504" s="7" t="s">
         <v>32</v>
@@ -26103,10 +26134,10 @@
         <v>497</v>
       </c>
       <c r="B505" s="23" t="s">
+        <v>908</v>
+      </c>
+      <c r="C505" s="8" t="s">
         <v>917</v>
-      </c>
-      <c r="C505" s="8" t="s">
-        <v>926</v>
       </c>
       <c r="D505" s="7" t="s">
         <v>32</v>
@@ -26139,10 +26170,10 @@
         <v>498</v>
       </c>
       <c r="B506" s="23" t="s">
-        <v>917</v>
+        <v>908</v>
       </c>
       <c r="C506" s="8" t="s">
-        <v>927</v>
+        <v>918</v>
       </c>
       <c r="D506" s="7" t="s">
         <v>32</v>
@@ -26175,10 +26206,10 @@
         <v>499</v>
       </c>
       <c r="B507" s="23" t="s">
-        <v>917</v>
+        <v>908</v>
       </c>
       <c r="C507" s="8" t="s">
-        <v>928</v>
+        <v>919</v>
       </c>
       <c r="D507" s="7" t="s">
         <v>32</v>
@@ -26211,10 +26242,10 @@
         <v>500</v>
       </c>
       <c r="B508" s="23" t="s">
-        <v>917</v>
+        <v>908</v>
       </c>
       <c r="C508" s="8" t="s">
-        <v>929</v>
+        <v>920</v>
       </c>
       <c r="D508" s="7" t="s">
         <v>32</v>
@@ -26247,10 +26278,10 @@
         <v>501</v>
       </c>
       <c r="B509" s="23" t="s">
-        <v>917</v>
+        <v>908</v>
       </c>
       <c r="C509" s="8" t="s">
-        <v>930</v>
+        <v>921</v>
       </c>
       <c r="D509" s="7" t="s">
         <v>32</v>
@@ -26283,10 +26314,10 @@
         <v>502</v>
       </c>
       <c r="B510" s="23" t="s">
-        <v>917</v>
+        <v>908</v>
       </c>
       <c r="C510" s="8" t="s">
-        <v>931</v>
+        <v>922</v>
       </c>
       <c r="D510" s="7" t="s">
         <v>32</v>
@@ -26319,10 +26350,10 @@
         <v>503</v>
       </c>
       <c r="B511" s="23" t="s">
-        <v>917</v>
+        <v>908</v>
       </c>
       <c r="C511" s="8" t="s">
-        <v>932</v>
+        <v>923</v>
       </c>
       <c r="D511" s="7" t="s">
         <v>32</v>
@@ -26355,10 +26386,10 @@
         <v>504</v>
       </c>
       <c r="B512" s="23" t="s">
-        <v>917</v>
+        <v>908</v>
       </c>
       <c r="C512" s="8" t="s">
-        <v>933</v>
+        <v>924</v>
       </c>
       <c r="D512" s="7" t="s">
         <v>32</v>
@@ -26391,10 +26422,10 @@
         <v>505</v>
       </c>
       <c r="B513" s="23" t="s">
-        <v>917</v>
+        <v>908</v>
       </c>
       <c r="C513" s="8" t="s">
-        <v>934</v>
+        <v>925</v>
       </c>
       <c r="D513" s="7" t="s">
         <v>32</v>
@@ -26427,10 +26458,10 @@
         <v>506</v>
       </c>
       <c r="B514" s="23" t="s">
-        <v>917</v>
+        <v>908</v>
       </c>
       <c r="C514" s="8" t="s">
-        <v>935</v>
+        <v>926</v>
       </c>
       <c r="D514" s="7" t="s">
         <v>32</v>
@@ -26463,10 +26494,10 @@
         <v>507</v>
       </c>
       <c r="B515" s="23" t="s">
-        <v>917</v>
+        <v>908</v>
       </c>
       <c r="C515" s="8" t="s">
-        <v>936</v>
+        <v>927</v>
       </c>
       <c r="D515" s="7" t="s">
         <v>32</v>
@@ -26499,10 +26530,10 @@
         <v>508</v>
       </c>
       <c r="B516" s="23" t="s">
-        <v>917</v>
+        <v>908</v>
       </c>
       <c r="C516" s="8" t="s">
-        <v>937</v>
+        <v>928</v>
       </c>
       <c r="D516" s="7" t="s">
         <v>32</v>
@@ -26514,7 +26545,7 @@
         <v>1</v>
       </c>
       <c r="H516" s="13" t="s">
-        <v>938</v>
+        <v>929</v>
       </c>
       <c r="M516" s="9" t="str" cm="1">
         <f t="array" ref="M516">PAGE_NAME(B516)</f>
@@ -26538,10 +26569,10 @@
         <v>509</v>
       </c>
       <c r="B517" s="23" t="s">
-        <v>917</v>
+        <v>908</v>
       </c>
       <c r="C517" s="8" t="s">
-        <v>939</v>
+        <v>930</v>
       </c>
       <c r="D517" s="7" t="s">
         <v>41</v>
@@ -26553,7 +26584,7 @@
         <v>1</v>
       </c>
       <c r="H517" s="13" t="s">
-        <v>940</v>
+        <v>931</v>
       </c>
       <c r="M517" s="9" t="str" cm="1">
         <f t="array" ref="M517">PAGE_NAME(B517)</f>
@@ -26577,10 +26608,10 @@
         <v>510</v>
       </c>
       <c r="B518" s="23" t="s">
-        <v>917</v>
+        <v>908</v>
       </c>
       <c r="C518" s="8" t="s">
-        <v>941</v>
+        <v>932</v>
       </c>
       <c r="D518" s="7" t="s">
         <v>37</v>
@@ -26613,10 +26644,10 @@
         <v>511</v>
       </c>
       <c r="B519" s="23" t="s">
-        <v>942</v>
+        <v>933</v>
       </c>
       <c r="C519" s="8" t="s">
-        <v>943</v>
+        <v>934</v>
       </c>
       <c r="D519" s="7" t="s">
         <v>32</v>
@@ -26628,7 +26659,7 @@
         <v>1</v>
       </c>
       <c r="H519" s="13" t="s">
-        <v>944</v>
+        <v>935</v>
       </c>
       <c r="M519" s="9" t="str" cm="1">
         <f t="array" ref="M519">PAGE_NAME(B519)</f>
@@ -26652,10 +26683,10 @@
         <v>512</v>
       </c>
       <c r="B520" s="23" t="s">
-        <v>942</v>
+        <v>933</v>
       </c>
       <c r="C520" s="8" t="s">
-        <v>945</v>
+        <v>936</v>
       </c>
       <c r="D520" s="7" t="s">
         <v>41</v>
@@ -26667,7 +26698,7 @@
         <v>1</v>
       </c>
       <c r="H520" s="13" t="s">
-        <v>944</v>
+        <v>935</v>
       </c>
       <c r="M520" s="9" t="str" cm="1">
         <f t="array" ref="M520">PAGE_NAME(B520)</f>
@@ -26691,10 +26722,10 @@
         <v>513</v>
       </c>
       <c r="B521" s="23" t="s">
-        <v>946</v>
+        <v>937</v>
       </c>
       <c r="C521" s="8" t="s">
-        <v>947</v>
+        <v>938</v>
       </c>
       <c r="D521" s="7" t="s">
         <v>87</v>
@@ -26730,10 +26761,10 @@
         <v>514</v>
       </c>
       <c r="B522" s="23" t="s">
-        <v>948</v>
+        <v>939</v>
       </c>
       <c r="C522" s="8" t="s">
-        <v>949</v>
+        <v>940</v>
       </c>
       <c r="D522" s="7" t="s">
         <v>41</v>
@@ -26766,10 +26797,10 @@
         <v>515</v>
       </c>
       <c r="B523" s="23" t="s">
-        <v>948</v>
+        <v>939</v>
       </c>
       <c r="C523" s="8" t="s">
-        <v>950</v>
+        <v>941</v>
       </c>
       <c r="D523" s="7" t="s">
         <v>37</v>
@@ -26802,10 +26833,10 @@
         <v>516</v>
       </c>
       <c r="B524" s="53" t="s">
-        <v>948</v>
+        <v>939</v>
       </c>
       <c r="C524" s="8" t="s">
-        <v>951</v>
+        <v>942</v>
       </c>
       <c r="D524" s="7" t="s">
         <v>87</v>
@@ -26817,7 +26848,7 @@
         <v>1</v>
       </c>
       <c r="H524" s="13" t="s">
-        <v>908</v>
+        <v>899</v>
       </c>
       <c r="M524" s="9" t="str" cm="1">
         <f t="array" ref="M524">PAGE_NAME(B524)</f>
@@ -26836,7 +26867,7 @@
         <v>Server</v>
       </c>
       <c r="U524" s="13" t="s">
-        <v>899</v>
+        <v>890</v>
       </c>
     </row>
     <row r="525" spans="1:21" ht="85" x14ac:dyDescent="0.2">
@@ -26844,10 +26875,10 @@
         <v>517</v>
       </c>
       <c r="B525" s="23" t="s">
-        <v>948</v>
+        <v>939</v>
       </c>
       <c r="C525" s="8" t="s">
-        <v>952</v>
+        <v>943</v>
       </c>
       <c r="D525" s="7" t="s">
         <v>87</v>
@@ -26859,7 +26890,7 @@
         <v>1</v>
       </c>
       <c r="H525" s="13" t="s">
-        <v>908</v>
+        <v>899</v>
       </c>
       <c r="M525" s="9" t="str" cm="1">
         <f t="array" ref="M525">PAGE_NAME(B525)</f>
@@ -26878,7 +26909,7 @@
         <v>Client</v>
       </c>
       <c r="U525" s="13" t="s">
-        <v>899</v>
+        <v>890</v>
       </c>
     </row>
     <row r="526" spans="1:21" ht="119" x14ac:dyDescent="0.2">
@@ -26886,10 +26917,10 @@
         <v>518</v>
       </c>
       <c r="B526" s="23" t="s">
-        <v>948</v>
+        <v>939</v>
       </c>
       <c r="C526" s="8" t="s">
-        <v>953</v>
+        <v>944</v>
       </c>
       <c r="D526" s="7" t="s">
         <v>87</v>
@@ -26901,7 +26932,7 @@
         <v>1</v>
       </c>
       <c r="H526" s="13" t="s">
-        <v>911</v>
+        <v>902</v>
       </c>
       <c r="M526" s="9" t="str" cm="1">
         <f t="array" ref="M526">PAGE_NAME(B526)</f>
@@ -26920,7 +26951,7 @@
         <v>Server</v>
       </c>
       <c r="U526" s="13" t="s">
-        <v>899</v>
+        <v>890</v>
       </c>
     </row>
     <row r="527" spans="1:21" ht="85" x14ac:dyDescent="0.2">
@@ -26928,10 +26959,10 @@
         <v>519</v>
       </c>
       <c r="B527" s="23" t="s">
-        <v>948</v>
+        <v>939</v>
       </c>
       <c r="C527" s="8" t="s">
-        <v>954</v>
+        <v>945</v>
       </c>
       <c r="D527" s="7" t="s">
         <v>87</v>
@@ -26943,7 +26974,7 @@
         <v>1</v>
       </c>
       <c r="H527" s="13" t="s">
-        <v>908</v>
+        <v>899</v>
       </c>
       <c r="M527" s="9" t="str" cm="1">
         <f t="array" ref="M527">PAGE_NAME(B527)</f>
@@ -26962,7 +26993,7 @@
         <v>Client</v>
       </c>
       <c r="U527" s="13" t="s">
-        <v>899</v>
+        <v>890</v>
       </c>
     </row>
     <row r="528" spans="1:21" ht="85" x14ac:dyDescent="0.2">
@@ -26970,10 +27001,10 @@
         <v>520</v>
       </c>
       <c r="B528" s="23" t="s">
-        <v>948</v>
+        <v>939</v>
       </c>
       <c r="C528" s="8" t="s">
-        <v>955</v>
+        <v>946</v>
       </c>
       <c r="D528" s="7" t="s">
         <v>87</v>
@@ -26985,7 +27016,7 @@
         <v>1</v>
       </c>
       <c r="H528" s="13" t="s">
-        <v>914</v>
+        <v>905</v>
       </c>
       <c r="M528" s="9" t="str" cm="1">
         <f t="array" ref="M528">PAGE_NAME(B528)</f>
@@ -27004,7 +27035,7 @@
         <v>Server</v>
       </c>
       <c r="U528" s="13" t="s">
-        <v>899</v>
+        <v>890</v>
       </c>
     </row>
     <row r="529" spans="1:21" ht="85" x14ac:dyDescent="0.2">
@@ -27012,10 +27043,10 @@
         <v>521</v>
       </c>
       <c r="B529" s="53" t="s">
-        <v>948</v>
+        <v>939</v>
       </c>
       <c r="C529" s="8" t="s">
-        <v>956</v>
+        <v>947</v>
       </c>
       <c r="D529" s="7" t="s">
         <v>87</v>
@@ -27027,7 +27058,7 @@
         <v>1</v>
       </c>
       <c r="H529" s="13" t="s">
-        <v>914</v>
+        <v>905</v>
       </c>
       <c r="M529" s="9" t="str" cm="1">
         <f t="array" ref="M529">PAGE_NAME(B529)</f>
@@ -27046,7 +27077,7 @@
         <v>Client</v>
       </c>
       <c r="U529" s="13" t="s">
-        <v>899</v>
+        <v>890</v>
       </c>
     </row>
     <row r="530" spans="1:21" ht="102" x14ac:dyDescent="0.2">
@@ -27054,10 +27085,10 @@
         <v>522</v>
       </c>
       <c r="B530" s="23" t="s">
+        <v>939</v>
+      </c>
+      <c r="C530" s="8" t="s">
         <v>948</v>
-      </c>
-      <c r="C530" s="8" t="s">
-        <v>957</v>
       </c>
       <c r="D530" s="7" t="s">
         <v>37</v>
@@ -27085,7 +27116,7 @@
         <v/>
       </c>
       <c r="U530" s="13" t="s">
-        <v>958</v>
+        <v>949</v>
       </c>
     </row>
     <row r="531" spans="1:21" ht="68" x14ac:dyDescent="0.2">
@@ -27093,10 +27124,10 @@
         <v>523</v>
       </c>
       <c r="B531" s="23" t="s">
-        <v>959</v>
+        <v>950</v>
       </c>
       <c r="C531" s="8" t="s">
-        <v>960</v>
+        <v>951</v>
       </c>
       <c r="D531" s="7" t="s">
         <v>41</v>
@@ -27129,10 +27160,10 @@
         <v>524</v>
       </c>
       <c r="B532" s="23" t="s">
-        <v>959</v>
+        <v>950</v>
       </c>
       <c r="C532" s="8" t="s">
-        <v>961</v>
+        <v>952</v>
       </c>
       <c r="D532" s="7" t="s">
         <v>87</v>
@@ -27144,7 +27175,7 @@
         <v>1</v>
       </c>
       <c r="H532" s="13" t="s">
-        <v>962</v>
+        <v>953</v>
       </c>
       <c r="M532" s="9" t="str" cm="1">
         <f t="array" ref="M532">PAGE_NAME(B532)</f>
@@ -27163,7 +27194,7 @@
         <v>Server</v>
       </c>
       <c r="U532" s="13" t="s">
-        <v>899</v>
+        <v>890</v>
       </c>
     </row>
     <row r="533" spans="1:21" ht="51" x14ac:dyDescent="0.2">
@@ -27171,10 +27202,10 @@
         <v>525</v>
       </c>
       <c r="B533" s="23" t="s">
-        <v>959</v>
+        <v>950</v>
       </c>
       <c r="C533" s="8" t="s">
-        <v>963</v>
+        <v>954</v>
       </c>
       <c r="D533" s="7" t="s">
         <v>87</v>
@@ -27202,7 +27233,7 @@
         <v>Client</v>
       </c>
       <c r="U533" s="13" t="s">
-        <v>899</v>
+        <v>890</v>
       </c>
     </row>
     <row r="534" spans="1:21" ht="51" x14ac:dyDescent="0.2">
@@ -27210,10 +27241,10 @@
         <v>526</v>
       </c>
       <c r="B534" s="23" t="s">
-        <v>959</v>
+        <v>950</v>
       </c>
       <c r="C534" s="8" t="s">
-        <v>964</v>
+        <v>955</v>
       </c>
       <c r="D534" s="7" t="s">
         <v>41</v>
@@ -27246,10 +27277,10 @@
         <v>527</v>
       </c>
       <c r="B535" s="23" t="s">
-        <v>965</v>
+        <v>956</v>
       </c>
       <c r="C535" s="8" t="s">
-        <v>966</v>
+        <v>957</v>
       </c>
       <c r="D535" s="7" t="s">
         <v>37</v>
@@ -27277,7 +27308,7 @@
         <v>Client</v>
       </c>
       <c r="U535" s="13" t="s">
-        <v>967</v>
+        <v>958</v>
       </c>
     </row>
     <row r="536" spans="1:21" ht="34" x14ac:dyDescent="0.2">
@@ -27285,10 +27316,10 @@
         <v>528</v>
       </c>
       <c r="B536" s="23" t="s">
-        <v>968</v>
+        <v>959</v>
       </c>
       <c r="C536" s="8" t="s">
-        <v>969</v>
+        <v>960</v>
       </c>
       <c r="D536" s="7" t="s">
         <v>41</v>
@@ -27321,10 +27352,10 @@
         <v>529</v>
       </c>
       <c r="B537" s="23" t="s">
-        <v>968</v>
+        <v>959</v>
       </c>
       <c r="C537" s="8" t="s">
-        <v>970</v>
+        <v>961</v>
       </c>
       <c r="D537" s="7" t="s">
         <v>41</v>
@@ -27357,10 +27388,10 @@
         <v>530</v>
       </c>
       <c r="B538" s="23" t="s">
-        <v>968</v>
+        <v>959</v>
       </c>
       <c r="C538" s="8" t="s">
-        <v>971</v>
+        <v>962</v>
       </c>
       <c r="D538" s="7" t="s">
         <v>41</v>
@@ -27393,10 +27424,10 @@
         <v>531</v>
       </c>
       <c r="B539" s="23" t="s">
-        <v>968</v>
+        <v>959</v>
       </c>
       <c r="C539" s="8" t="s">
-        <v>972</v>
+        <v>963</v>
       </c>
       <c r="D539" s="7" t="s">
         <v>41</v>
@@ -27429,10 +27460,10 @@
         <v>532</v>
       </c>
       <c r="B540" s="23" t="s">
-        <v>973</v>
+        <v>964</v>
       </c>
       <c r="C540" s="8" t="s">
-        <v>974</v>
+        <v>965</v>
       </c>
       <c r="D540" s="7" t="s">
         <v>37</v>
@@ -27460,7 +27491,7 @@
         <v>Server</v>
       </c>
       <c r="U540" s="13" t="s">
-        <v>975</v>
+        <v>966</v>
       </c>
     </row>
     <row r="541" spans="1:21" ht="34" x14ac:dyDescent="0.2">
@@ -27468,10 +27499,10 @@
         <v>533</v>
       </c>
       <c r="B541" s="23" t="s">
-        <v>976</v>
+        <v>967</v>
       </c>
       <c r="C541" s="8" t="s">
-        <v>977</v>
+        <v>968</v>
       </c>
       <c r="D541" s="7" t="s">
         <v>32</v>
@@ -27504,10 +27535,10 @@
         <v>534</v>
       </c>
       <c r="B542" s="23" t="s">
-        <v>976</v>
+        <v>967</v>
       </c>
       <c r="C542" s="8" t="s">
-        <v>978</v>
+        <v>969</v>
       </c>
       <c r="D542" s="7" t="s">
         <v>32</v>
@@ -27540,10 +27571,10 @@
         <v>535</v>
       </c>
       <c r="B543" s="23" t="s">
-        <v>976</v>
+        <v>967</v>
       </c>
       <c r="C543" s="8" t="s">
-        <v>979</v>
+        <v>970</v>
       </c>
       <c r="D543" s="7" t="s">
         <v>32</v>
@@ -27576,10 +27607,10 @@
         <v>536</v>
       </c>
       <c r="B544" s="23" t="s">
-        <v>976</v>
+        <v>967</v>
       </c>
       <c r="C544" s="8" t="s">
-        <v>980</v>
+        <v>971</v>
       </c>
       <c r="D544" s="7" t="s">
         <v>32</v>
@@ -27612,10 +27643,10 @@
         <v>537</v>
       </c>
       <c r="B545" s="23" t="s">
-        <v>976</v>
+        <v>967</v>
       </c>
       <c r="C545" s="8" t="s">
-        <v>981</v>
+        <v>972</v>
       </c>
       <c r="D545" s="7" t="s">
         <v>32</v>
@@ -27648,10 +27679,10 @@
         <v>538</v>
       </c>
       <c r="B546" s="23" t="s">
-        <v>976</v>
+        <v>967</v>
       </c>
       <c r="C546" s="8" t="s">
-        <v>982</v>
+        <v>973</v>
       </c>
       <c r="D546" s="7" t="s">
         <v>32</v>
@@ -27684,10 +27715,10 @@
         <v>539</v>
       </c>
       <c r="B547" s="23" t="s">
-        <v>976</v>
+        <v>967</v>
       </c>
       <c r="C547" s="8" t="s">
-        <v>983</v>
+        <v>974</v>
       </c>
       <c r="D547" s="7" t="s">
         <v>32</v>
@@ -27720,10 +27751,10 @@
         <v>540</v>
       </c>
       <c r="B548" s="23" t="s">
-        <v>976</v>
+        <v>967</v>
       </c>
       <c r="C548" s="8" t="s">
-        <v>984</v>
+        <v>975</v>
       </c>
       <c r="D548" s="7" t="s">
         <v>32</v>
@@ -27756,10 +27787,10 @@
         <v>541</v>
       </c>
       <c r="B549" s="23" t="s">
+        <v>967</v>
+      </c>
+      <c r="C549" s="8" t="s">
         <v>976</v>
-      </c>
-      <c r="C549" s="8" t="s">
-        <v>985</v>
       </c>
       <c r="D549" s="7" t="s">
         <v>37</v>
@@ -27792,10 +27823,10 @@
         <v>542</v>
       </c>
       <c r="B550" s="23" t="s">
-        <v>976</v>
+        <v>967</v>
       </c>
       <c r="C550" s="8" t="s">
-        <v>986</v>
+        <v>977</v>
       </c>
       <c r="D550" s="7" t="s">
         <v>37</v>
@@ -27828,10 +27859,10 @@
         <v>543</v>
       </c>
       <c r="B551" s="23" t="s">
-        <v>976</v>
+        <v>967</v>
       </c>
       <c r="C551" s="8" t="s">
-        <v>987</v>
+        <v>978</v>
       </c>
       <c r="D551" s="7" t="s">
         <v>32</v>
@@ -27843,7 +27874,7 @@
         <v>1</v>
       </c>
       <c r="H551" s="13" t="s">
-        <v>988</v>
+        <v>979</v>
       </c>
       <c r="M551" s="9" t="str" cm="1">
         <f t="array" ref="M551">PAGE_NAME(B551)</f>
@@ -27867,10 +27898,10 @@
         <v>544</v>
       </c>
       <c r="B552" s="23" t="s">
-        <v>976</v>
+        <v>967</v>
       </c>
       <c r="C552" s="8" t="s">
-        <v>989</v>
+        <v>980</v>
       </c>
       <c r="D552" s="7" t="s">
         <v>41</v>
@@ -27903,10 +27934,10 @@
         <v>545</v>
       </c>
       <c r="B553" s="23" t="s">
-        <v>976</v>
+        <v>967</v>
       </c>
       <c r="C553" s="8" t="s">
-        <v>990</v>
+        <v>981</v>
       </c>
       <c r="D553" s="7" t="s">
         <v>41</v>
@@ -27939,10 +27970,10 @@
         <v>546</v>
       </c>
       <c r="B554" s="23" t="s">
-        <v>976</v>
+        <v>967</v>
       </c>
       <c r="C554" s="8" t="s">
-        <v>991</v>
+        <v>982</v>
       </c>
       <c r="D554" s="7" t="s">
         <v>41</v>
@@ -27975,10 +28006,10 @@
         <v>547</v>
       </c>
       <c r="B555" s="23" t="s">
-        <v>976</v>
+        <v>967</v>
       </c>
       <c r="C555" s="8" t="s">
-        <v>992</v>
+        <v>983</v>
       </c>
       <c r="D555" s="7" t="s">
         <v>41</v>
@@ -28011,10 +28042,10 @@
         <v>548</v>
       </c>
       <c r="B556" s="23" t="s">
-        <v>993</v>
+        <v>984</v>
       </c>
       <c r="C556" s="8" t="s">
-        <v>994</v>
+        <v>985</v>
       </c>
       <c r="D556" s="7" t="s">
         <v>37</v>
@@ -28047,10 +28078,10 @@
         <v>549</v>
       </c>
       <c r="B557" s="23" t="s">
-        <v>993</v>
+        <v>984</v>
       </c>
       <c r="C557" s="8" t="s">
-        <v>995</v>
+        <v>986</v>
       </c>
       <c r="D557" s="7" t="s">
         <v>37</v>
@@ -28062,7 +28093,7 @@
         <v>1</v>
       </c>
       <c r="H557" s="13" t="s">
-        <v>996</v>
+        <v>987</v>
       </c>
       <c r="M557" s="9" t="str" cm="1">
         <f t="array" ref="M557">PAGE_NAME(B557)</f>
@@ -28086,10 +28117,10 @@
         <v>550</v>
       </c>
       <c r="B558" s="23" t="s">
-        <v>997</v>
+        <v>988</v>
       </c>
       <c r="C558" s="8" t="s">
-        <v>998</v>
+        <v>989</v>
       </c>
       <c r="D558" s="7" t="s">
         <v>32</v>
@@ -28122,10 +28153,10 @@
         <v>551</v>
       </c>
       <c r="B559" s="23" t="s">
-        <v>997</v>
+        <v>988</v>
       </c>
       <c r="C559" s="8" t="s">
-        <v>998</v>
+        <v>989</v>
       </c>
       <c r="D559" s="7" t="s">
         <v>32</v>
@@ -28158,10 +28189,10 @@
         <v>552</v>
       </c>
       <c r="B560" s="23" t="s">
-        <v>997</v>
+        <v>988</v>
       </c>
       <c r="C560" s="8" t="s">
-        <v>999</v>
+        <v>990</v>
       </c>
       <c r="D560" s="7" t="s">
         <v>37</v>
@@ -28194,10 +28225,10 @@
         <v>553</v>
       </c>
       <c r="B561" s="23" t="s">
-        <v>997</v>
+        <v>988</v>
       </c>
       <c r="C561" s="8" t="s">
-        <v>999</v>
+        <v>990</v>
       </c>
       <c r="D561" s="7" t="s">
         <v>37</v>
@@ -28230,10 +28261,10 @@
         <v>554</v>
       </c>
       <c r="B562" s="23" t="s">
-        <v>997</v>
+        <v>988</v>
       </c>
       <c r="C562" s="8" t="s">
-        <v>1000</v>
+        <v>991</v>
       </c>
       <c r="D562" s="7" t="s">
         <v>37</v>
@@ -28266,10 +28297,10 @@
         <v>555</v>
       </c>
       <c r="B563" s="23" t="s">
-        <v>997</v>
+        <v>988</v>
       </c>
       <c r="C563" s="8" t="s">
-        <v>1000</v>
+        <v>991</v>
       </c>
       <c r="D563" s="7" t="s">
         <v>37</v>
@@ -28302,10 +28333,10 @@
         <v>556</v>
       </c>
       <c r="B564" s="23" t="s">
-        <v>997</v>
+        <v>988</v>
       </c>
       <c r="C564" s="8" t="s">
-        <v>1001</v>
+        <v>992</v>
       </c>
       <c r="D564" s="7" t="s">
         <v>37</v>
@@ -28338,10 +28369,10 @@
         <v>557</v>
       </c>
       <c r="B565" s="23" t="s">
-        <v>997</v>
+        <v>988</v>
       </c>
       <c r="C565" s="8" t="s">
-        <v>1001</v>
+        <v>992</v>
       </c>
       <c r="D565" s="7" t="s">
         <v>37</v>
@@ -28374,10 +28405,10 @@
         <v>558</v>
       </c>
       <c r="B566" s="23" t="s">
-        <v>997</v>
+        <v>988</v>
       </c>
       <c r="C566" s="8" t="s">
-        <v>1002</v>
+        <v>993</v>
       </c>
       <c r="D566" s="7" t="s">
         <v>32</v>
@@ -28410,10 +28441,10 @@
         <v>559</v>
       </c>
       <c r="B567" s="23" t="s">
-        <v>997</v>
+        <v>988</v>
       </c>
       <c r="C567" s="8" t="s">
-        <v>1002</v>
+        <v>993</v>
       </c>
       <c r="D567" s="7" t="s">
         <v>32</v>
@@ -28446,10 +28477,10 @@
         <v>560</v>
       </c>
       <c r="B568" s="23" t="s">
-        <v>997</v>
+        <v>988</v>
       </c>
       <c r="C568" s="8" t="s">
-        <v>1003</v>
+        <v>994</v>
       </c>
       <c r="D568" s="7" t="s">
         <v>37</v>
@@ -28482,10 +28513,10 @@
         <v>561</v>
       </c>
       <c r="B569" s="23" t="s">
-        <v>997</v>
+        <v>988</v>
       </c>
       <c r="C569" s="8" t="s">
-        <v>1003</v>
+        <v>994</v>
       </c>
       <c r="D569" s="7" t="s">
         <v>37</v>
@@ -28518,10 +28549,10 @@
         <v>562</v>
       </c>
       <c r="B570" s="23" t="s">
-        <v>997</v>
+        <v>988</v>
       </c>
       <c r="C570" s="8" t="s">
-        <v>1004</v>
+        <v>995</v>
       </c>
       <c r="D570" s="7" t="s">
         <v>32</v>
@@ -28554,10 +28585,10 @@
         <v>563</v>
       </c>
       <c r="B571" s="23" t="s">
-        <v>997</v>
+        <v>988</v>
       </c>
       <c r="C571" s="8" t="s">
-        <v>1004</v>
+        <v>995</v>
       </c>
       <c r="D571" s="7" t="s">
         <v>32</v>
@@ -28590,10 +28621,10 @@
         <v>564</v>
       </c>
       <c r="B572" s="23" t="s">
-        <v>997</v>
+        <v>988</v>
       </c>
       <c r="C572" s="8" t="s">
-        <v>1005</v>
+        <v>996</v>
       </c>
       <c r="D572" s="7" t="s">
         <v>32</v>
@@ -28626,10 +28657,10 @@
         <v>565</v>
       </c>
       <c r="B573" s="23" t="s">
-        <v>997</v>
+        <v>988</v>
       </c>
       <c r="C573" s="8" t="s">
-        <v>1005</v>
+        <v>996</v>
       </c>
       <c r="D573" s="7" t="s">
         <v>32</v>
@@ -28662,10 +28693,10 @@
         <v>566</v>
       </c>
       <c r="B574" s="23" t="s">
+        <v>988</v>
+      </c>
+      <c r="C574" s="8" t="s">
         <v>997</v>
-      </c>
-      <c r="C574" s="8" t="s">
-        <v>1006</v>
       </c>
       <c r="D574" s="7" t="s">
         <v>37</v>
@@ -28698,10 +28729,10 @@
         <v>567</v>
       </c>
       <c r="B575" s="23" t="s">
+        <v>988</v>
+      </c>
+      <c r="C575" s="8" t="s">
         <v>997</v>
-      </c>
-      <c r="C575" s="8" t="s">
-        <v>1006</v>
       </c>
       <c r="D575" s="7" t="s">
         <v>37</v>
@@ -28734,10 +28765,10 @@
         <v>568</v>
       </c>
       <c r="B576" s="23" t="s">
-        <v>997</v>
+        <v>988</v>
       </c>
       <c r="C576" s="8" t="s">
-        <v>1007</v>
+        <v>998</v>
       </c>
       <c r="D576" s="7" t="s">
         <v>32</v>
@@ -28770,10 +28801,10 @@
         <v>569</v>
       </c>
       <c r="B577" s="23" t="s">
-        <v>997</v>
+        <v>988</v>
       </c>
       <c r="C577" s="8" t="s">
-        <v>1007</v>
+        <v>998</v>
       </c>
       <c r="D577" s="7" t="s">
         <v>32</v>
@@ -28806,10 +28837,10 @@
         <v>570</v>
       </c>
       <c r="B578" s="23" t="s">
-        <v>997</v>
+        <v>988</v>
       </c>
       <c r="C578" s="8" t="s">
-        <v>1008</v>
+        <v>999</v>
       </c>
       <c r="D578" s="7" t="s">
         <v>32</v>
@@ -28842,10 +28873,10 @@
         <v>571</v>
       </c>
       <c r="B579" s="23" t="s">
-        <v>997</v>
+        <v>988</v>
       </c>
       <c r="C579" s="8" t="s">
-        <v>1008</v>
+        <v>999</v>
       </c>
       <c r="D579" s="7" t="s">
         <v>32</v>
@@ -28878,10 +28909,10 @@
         <v>572</v>
       </c>
       <c r="B580" s="23" t="s">
-        <v>997</v>
+        <v>988</v>
       </c>
       <c r="C580" s="8" t="s">
-        <v>1009</v>
+        <v>1000</v>
       </c>
       <c r="D580" s="7" t="s">
         <v>32</v>
@@ -28914,10 +28945,10 @@
         <v>573</v>
       </c>
       <c r="B581" s="23" t="s">
-        <v>997</v>
+        <v>988</v>
       </c>
       <c r="C581" s="8" t="s">
-        <v>1009</v>
+        <v>1000</v>
       </c>
       <c r="D581" s="7" t="s">
         <v>32</v>
@@ -28950,10 +28981,10 @@
         <v>574</v>
       </c>
       <c r="B582" s="23" t="s">
-        <v>997</v>
+        <v>988</v>
       </c>
       <c r="C582" s="8" t="s">
-        <v>1010</v>
+        <v>1001</v>
       </c>
       <c r="D582" s="7" t="s">
         <v>37</v>
@@ -28986,10 +29017,10 @@
         <v>575</v>
       </c>
       <c r="B583" s="23" t="s">
-        <v>997</v>
+        <v>988</v>
       </c>
       <c r="C583" s="8" t="s">
-        <v>1010</v>
+        <v>1001</v>
       </c>
       <c r="D583" s="7" t="s">
         <v>37</v>
@@ -29022,10 +29053,10 @@
         <v>576</v>
       </c>
       <c r="B584" s="23" t="s">
-        <v>997</v>
+        <v>988</v>
       </c>
       <c r="C584" s="8" t="s">
-        <v>1011</v>
+        <v>1002</v>
       </c>
       <c r="D584" s="7" t="s">
         <v>37</v>
@@ -29058,10 +29089,10 @@
         <v>577</v>
       </c>
       <c r="B585" s="23" t="s">
-        <v>997</v>
+        <v>988</v>
       </c>
       <c r="C585" s="8" t="s">
-        <v>1012</v>
+        <v>1003</v>
       </c>
       <c r="D585" s="7" t="s">
         <v>37</v>
@@ -29094,10 +29125,10 @@
         <v>578</v>
       </c>
       <c r="B586" s="23" t="s">
-        <v>997</v>
+        <v>988</v>
       </c>
       <c r="C586" s="8" t="s">
-        <v>1013</v>
+        <v>1004</v>
       </c>
       <c r="D586" s="7" t="s">
         <v>41</v>
@@ -29130,10 +29161,10 @@
         <v>579</v>
       </c>
       <c r="B587" s="23" t="s">
-        <v>997</v>
+        <v>988</v>
       </c>
       <c r="C587" s="8" t="s">
-        <v>1013</v>
+        <v>1004</v>
       </c>
       <c r="D587" s="7" t="s">
         <v>41</v>
@@ -29166,10 +29197,10 @@
         <v>580</v>
       </c>
       <c r="B588" s="23" t="s">
-        <v>997</v>
+        <v>988</v>
       </c>
       <c r="C588" s="8" t="s">
-        <v>1014</v>
+        <v>1005</v>
       </c>
       <c r="D588" s="7" t="s">
         <v>41</v>
@@ -29202,10 +29233,10 @@
         <v>581</v>
       </c>
       <c r="B589" s="23" t="s">
-        <v>997</v>
+        <v>988</v>
       </c>
       <c r="C589" s="8" t="s">
-        <v>1014</v>
+        <v>1005</v>
       </c>
       <c r="D589" s="7" t="s">
         <v>41</v>
@@ -29238,10 +29269,10 @@
         <v>582</v>
       </c>
       <c r="B590" s="39" t="s">
-        <v>1015</v>
+        <v>1006</v>
       </c>
       <c r="C590" s="8" t="s">
-        <v>1016</v>
+        <v>1007</v>
       </c>
       <c r="D590" s="7" t="s">
         <v>87</v>
@@ -29253,7 +29284,7 @@
         <v>1</v>
       </c>
       <c r="H590" s="13" t="s">
-        <v>1017</v>
+        <v>1008</v>
       </c>
       <c r="M590" s="9" t="str" cm="1">
         <f t="array" ref="M590">PAGE_NAME(B590)</f>
@@ -29270,10 +29301,10 @@
         <v>583</v>
       </c>
       <c r="B591" s="39" t="s">
-        <v>1015</v>
+        <v>1006</v>
       </c>
       <c r="C591" s="8" t="s">
-        <v>1016</v>
+        <v>1007</v>
       </c>
       <c r="D591" s="7" t="s">
         <v>87</v>
@@ -29285,7 +29316,7 @@
         <v>1</v>
       </c>
       <c r="H591" s="13" t="s">
-        <v>1017</v>
+        <v>1008</v>
       </c>
       <c r="M591" s="9" t="str" cm="1">
         <f t="array" ref="M591">PAGE_NAME(B591)</f>
@@ -29302,10 +29333,10 @@
         <v>584</v>
       </c>
       <c r="B592" s="11" t="s">
-        <v>1018</v>
+        <v>1009</v>
       </c>
       <c r="C592" s="8" t="s">
-        <v>1019</v>
+        <v>1010</v>
       </c>
       <c r="D592" s="7" t="s">
         <v>32</v>
@@ -29317,7 +29348,7 @@
         <v>1</v>
       </c>
       <c r="H592" s="13" t="s">
-        <v>944</v>
+        <v>935</v>
       </c>
       <c r="M592" s="9" t="str" cm="1">
         <f t="array" ref="M592">PAGE_NAME(B592)</f>
@@ -29345,7 +29376,7 @@
         <v>327</v>
       </c>
       <c r="C593" s="8" t="s">
-        <v>1020</v>
+        <v>1011</v>
       </c>
       <c r="D593" s="7" t="s">
         <v>41</v>
@@ -29381,7 +29412,7 @@
         <v>327</v>
       </c>
       <c r="C594" s="8" t="s">
-        <v>1021</v>
+        <v>1012</v>
       </c>
       <c r="D594" s="7" t="s">
         <v>41</v>
@@ -29414,10 +29445,10 @@
         <v>702</v>
       </c>
       <c r="B595" s="23" t="s">
-        <v>1022</v>
+        <v>1013</v>
       </c>
       <c r="C595" s="8" t="s">
-        <v>1023</v>
+        <v>1014</v>
       </c>
       <c r="D595" s="7" t="s">
         <v>37</v>
@@ -29445,7 +29476,7 @@
         <v/>
       </c>
       <c r="U595" s="13" t="s">
-        <v>1024</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="596" spans="1:21" ht="51" x14ac:dyDescent="0.2">
@@ -29453,10 +29484,10 @@
         <v>703</v>
       </c>
       <c r="B596" s="23" t="s">
-        <v>1022</v>
+        <v>1013</v>
       </c>
       <c r="C596" s="8" t="s">
-        <v>1025</v>
+        <v>1016</v>
       </c>
       <c r="D596" s="7" t="s">
         <v>37</v>
@@ -29484,7 +29515,7 @@
         <v/>
       </c>
       <c r="U596" s="13" t="s">
-        <v>1026</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="597" spans="1:21" x14ac:dyDescent="0.2">
@@ -29541,7 +29572,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C323F474-BE25-4449-9222-E1A46A1843B5}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -29552,95 +29583,95 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="409.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="69" t="s">
-        <v>1027</v>
-      </c>
-      <c r="B1" s="70"/>
+      <c r="A1" s="70" t="s">
+        <v>1018</v>
+      </c>
+      <c r="B1" s="71"/>
     </row>
     <row r="2" spans="1:2" ht="82.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="70"/>
-      <c r="B2" s="70"/>
+      <c r="A2" s="71"/>
+      <c r="B2" s="71"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="15" t="s">
-        <v>1028</v>
+        <v>1019</v>
       </c>
       <c r="B3" t="s">
-        <v>1059</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="15" t="s">
-        <v>1029</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="15" t="s">
-        <v>1030</v>
+        <v>1021</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>1031</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="15" t="s">
-        <v>1032</v>
+        <v>1023</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>1033</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="15" t="s">
-        <v>1034</v>
+        <v>1025</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>1035</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="15" t="s">
-        <v>1036</v>
+        <v>1027</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>1037</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A9" s="15" t="s">
-        <v>1038</v>
+        <v>1029</v>
       </c>
       <c r="B9" s="31" t="s">
-        <v>1039</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="15" t="s">
-        <v>1040</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="153" x14ac:dyDescent="0.2">
       <c r="A11" s="15" t="s">
-        <v>1041</v>
+        <v>1032</v>
       </c>
       <c r="B11" s="31" t="s">
-        <v>1042</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="15" t="s">
-        <v>1043</v>
+        <v>1034</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>1044</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="15" t="s">
-        <v>1045</v>
+        <v>1036</v>
       </c>
       <c r="B13" s="32" t="s">
-        <v>1046</v>
+        <v>1037</v>
       </c>
     </row>
   </sheetData>
@@ -29671,19 +29702,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
-        <v>1030</v>
+        <v>1021</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>1047</v>
+        <v>1038</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>1048</v>
+        <v>1039</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>1049</v>
+        <v>1040</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>1050</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -29691,13 +29722,13 @@
         <v>0.1</v>
       </c>
       <c r="B2" t="s">
-        <v>1051</v>
+        <v>1042</v>
       </c>
       <c r="C2" s="44" t="s">
-        <v>1052</v>
+        <v>1043</v>
       </c>
       <c r="D2" t="s">
-        <v>1053</v>
+        <v>1044</v>
       </c>
       <c r="E2" s="45">
         <v>45618</v>
@@ -29723,13 +29754,13 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>1054</v>
+        <v>1045</v>
       </c>
       <c r="B1" t="s">
         <v>14</v>
       </c>
       <c r="C1" t="s">
-        <v>1055</v>
+        <v>1046</v>
       </c>
       <c r="D1" t="s">
         <v>16</v>
@@ -29746,7 +29777,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>1056</v>
+        <v>1047</v>
       </c>
       <c r="D2" t="s">
         <v>53</v>
@@ -29763,7 +29794,7 @@
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>1057</v>
+        <v>1048</v>
       </c>
       <c r="D3" t="s">
         <v>52</v>
@@ -29777,7 +29808,7 @@
         <v>41</v>
       </c>
       <c r="C4" t="s">
-        <v>1058</v>
+        <v>1049</v>
       </c>
       <c r="E4" t="s">
         <v>55</v>
@@ -29796,7 +29827,7 @@
         <v>75</v>
       </c>
       <c r="E6" t="s">
-        <v>877</v>
+        <v>870</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -29810,6 +29841,28 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="b5a44311-ed64-4a72-909f-c9dc6973bde2" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="eebd8b74-b9de-41b2-9247-c010c4973c2b">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <Description xmlns="eebd8b74-b9de-41b2-9247-c010c4973c2b" xsi:nil="true"/>
+    <SortOrder xmlns="eebd8b74-b9de-41b2-9247-c010c4973c2b" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EC335ED7BB179244BF94A0DFE64544DC" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d3a0f66abe5d2a0564332877ab55d3f7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="eebd8b74-b9de-41b2-9247-c010c4973c2b" xmlns:ns3="b7009bbd-f938-489b-a530-f05273710fff" xmlns:ns4="b5a44311-ed64-4a72-909f-c9dc6973bde2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ec7ca2ee893ff8a0f61d4046c6461645" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="eebd8b74-b9de-41b2-9247-c010c4973c2b"/>
@@ -30063,29 +30116,33 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA84097F-5807-4DCF-92C6-48C9EE26CFB8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="b5a44311-ed64-4a72-909f-c9dc6973bde2" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="eebd8b74-b9de-41b2-9247-c010c4973c2b">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <Description xmlns="eebd8b74-b9de-41b2-9247-c010c4973c2b" xsi:nil="true"/>
-    <SortOrder xmlns="eebd8b74-b9de-41b2-9247-c010c4973c2b" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19B0E317-5E0E-4728-AB3F-40F2C2B957FB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="eebd8b74-b9de-41b2-9247-c010c4973c2b"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="b7009bbd-f938-489b-a530-f05273710fff"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="b5a44311-ed64-4a72-909f-c9dc6973bde2"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C0B0A19-6928-4F0B-831A-5B9FDDD3F6CE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -30103,30 +30160,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA84097F-5807-4DCF-92C6-48C9EE26CFB8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19B0E317-5E0E-4728-AB3F-40F2C2B957FB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="eebd8b74-b9de-41b2-9247-c010c4973c2b"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="b7009bbd-f938-489b-a530-f05273710fff"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="b5a44311-ed64-4a72-909f-c9dc6973bde2"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
template and requirements changes based off of review comments
</commit_message>
<xml_diff>
--- a/lib/us_core_test_kit/requirements/hl7.fhir.us.core_6.1.0_reqs.xlsx
+++ b/lib/us_core_test_kit/requirements/hl7.fhir.us.core_6.1.0_reqs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/edeyoung/Documents/inferno/us-core-test-kit/lib/us_core_test_kit/requirements/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF5115A0-60B2-374F-97AE-A6FAC6940F09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{821C9270-6E16-7046-850B-C2AF8D885195}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1780" yWindow="760" windowWidth="27360" windowHeight="18880" firstSheet="1" activeTab="1" xr2:uid="{D251129A-65BB-5042-909C-749E11B8C0B0}"/>
   </bookViews>
@@ -20,8 +20,8 @@
     <sheet name="Column Data" sheetId="7" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Requirements!$A$1:$U$597</definedName>
-    <definedName name="bottom" localSheetId="1">Requirements!$U$698</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Requirements!$A$1:$U$601</definedName>
+    <definedName name="bottom" localSheetId="1">Requirements!$U$702</definedName>
     <definedName name="EXPLODE" localSheetId="0">_xlfn.LAMBDA(_xlpm.string,_xlfn.MAKEARRAY(1,LEN(_xlpm.string),_xlfn.LAMBDA(_xlpm.r,_xlpm.c,MID(_xlpm.string,_xlpm.c,1))))</definedName>
     <definedName name="EXPLODE">_xlfn.LAMBDA(_xlpm.string,_xlfn.MAKEARRAY(1,LEN(_xlpm.string),_xlfn.LAMBDA(_xlpm.r,_xlpm.c,MID(_xlpm.string,_xlpm.c,1))))</definedName>
     <definedName name="FIND_DUPLICATES" localSheetId="0">_xlfn.LAMBDA(_xlpm.test_word,_xlpm.test_key,_xlpm.words,_xlpm.keys,_xlpm.threshold, _xlfn.LET(_xlpm.duplist,_xlfn._xlws.FILTER(_xlpm.keys,_xlfn.BYROW(_xlpm.words, _xlfn.LAMBDA(_xlpm.word, Info!HAMDIST(INDEX(_xlpm.word,1,1), _xlpm.test_word)&lt;_xlpm.threshold))),_xlfn.SINGLE(_xlfn._xlws.FILTER(_xlpm.duplist,_xlpm.duplist&lt;&gt;_xlpm.test_key,""))))</definedName>
@@ -40,21 +40,21 @@
     <definedName name="root" localSheetId="1">Requirements!$U$551</definedName>
     <definedName name="SECTION_NAME" localSheetId="0">_xlfn.LAMBDA(_xlpm.url,IFERROR(_xlfn.LET(_xlpm.rev_string, Info!STRREV(_xlpm.url), _xlpm.hash_index,FIND("#", _xlpm.rev_string),_xlpm.section, RIGHT(_xlpm.url, _xlpm.hash_index-1),_xlpm.section),""))</definedName>
     <definedName name="SECTION_NAME">_xlfn.LAMBDA(_xlpm.url,IFERROR(_xlfn.LET(_xlpm.rev_string, STRREV(_xlpm.url), _xlpm.hash_index,FIND("#", _xlpm.rev_string),_xlpm.section, RIGHT(_xlpm.url, _xlpm.hash_index-1),_xlpm.section),""))</definedName>
-    <definedName name="ServiceRequest" localSheetId="1">Requirements!$U$601</definedName>
-    <definedName name="ServiceRequest.authoredOn" localSheetId="1">Requirements!$U$616</definedName>
-    <definedName name="ServiceRequest.category" localSheetId="1">Requirements!$U$604</definedName>
-    <definedName name="ServiceRequest.code" localSheetId="1">Requirements!$U$609</definedName>
-    <definedName name="ServiceRequest.intent" localSheetId="1">Requirements!$U$603</definedName>
-    <definedName name="ServiceRequest.occurrence_x_" localSheetId="1">Requirements!$U$612</definedName>
-    <definedName name="ServiceRequest.reasonCode" localSheetId="1">Requirements!$U$618</definedName>
-    <definedName name="ServiceRequest.reasonReference" localSheetId="1">Requirements!$U$620</definedName>
-    <definedName name="ServiceRequest.requester" localSheetId="1">Requirements!$U$617</definedName>
-    <definedName name="ServiceRequest.status" localSheetId="1">Requirements!$U$602</definedName>
-    <definedName name="ServiceRequest.subject" localSheetId="1">Requirements!$U$611</definedName>
+    <definedName name="ServiceRequest" localSheetId="1">Requirements!$U$605</definedName>
+    <definedName name="ServiceRequest.authoredOn" localSheetId="1">Requirements!$U$620</definedName>
+    <definedName name="ServiceRequest.category" localSheetId="1">Requirements!$U$608</definedName>
+    <definedName name="ServiceRequest.code" localSheetId="1">Requirements!$U$613</definedName>
+    <definedName name="ServiceRequest.intent" localSheetId="1">Requirements!$U$607</definedName>
+    <definedName name="ServiceRequest.occurrence_x_" localSheetId="1">Requirements!$U$616</definedName>
+    <definedName name="ServiceRequest.reasonCode" localSheetId="1">Requirements!$U$622</definedName>
+    <definedName name="ServiceRequest.reasonReference" localSheetId="1">Requirements!$U$624</definedName>
+    <definedName name="ServiceRequest.requester" localSheetId="1">Requirements!$U$621</definedName>
+    <definedName name="ServiceRequest.status" localSheetId="1">Requirements!$U$606</definedName>
+    <definedName name="ServiceRequest.subject" localSheetId="1">Requirements!$U$615</definedName>
     <definedName name="STRREV" localSheetId="0">_xlfn.LAMBDA(_xlpm.word, _xlfn.CONCAT(MID(_xlpm.word,_xlfn.SEQUENCE(LEN(_xlpm.word),,LEN(_xlpm.word),-1),1)))</definedName>
     <definedName name="STRREV">_xlfn.LAMBDA(_xlpm.word, _xlfn.CONCAT(MID(_xlpm.word,_xlfn.SEQUENCE(LEN(_xlpm.word),,LEN(_xlpm.word),-1),1)))</definedName>
     <definedName name="top" localSheetId="1">Requirements!$U$543</definedName>
-    <definedName name="tx" localSheetId="1">Requirements!$U$622</definedName>
+    <definedName name="tx" localSheetId="1">Requirements!$U$626</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -99,7 +99,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3045" uniqueCount="1062">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3065" uniqueCount="1069">
   <si>
     <r>
       <rPr>
@@ -4878,6 +4878,27 @@
   <si>
     <t>Duplicate to req 1</t>
   </si>
+  <si>
+    <t>https://hl7.org/fhir/us/core/STU7/StructureDefinition-us-core-allergyintolerance.html#mandatory-and-must-support-data-elements</t>
+  </si>
+  <si>
+    <t>Each AllergyIntolerance Must Have: a clinical status of the allergy (e.g., active or resolved)</t>
+  </si>
+  <si>
+    <t>Each AllergyIntolerance Must Have: a code that tells you what the patient is allergic to</t>
+  </si>
+  <si>
+    <t>Each AllergyIntolerance Must Support: a verification status</t>
+  </si>
+  <si>
+    <t>StructureDefinition-us-core-allergyintolerance</t>
+  </si>
+  <si>
+    <t>mandatory-and-must-support-data-elements</t>
+  </si>
+  <si>
+    <t>Each AllergyIntolerance Must Support: a reaction manifestation</t>
+  </si>
 </sst>
 </file>
 
@@ -5055,7 +5076,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -5122,8 +5143,26 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFF2CC"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFCE4D6"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDEBF7"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="23">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -5393,12 +5432,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFD0CECE"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFD0CECE"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFD0CECE"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5561,6 +5613,22 @@
     <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="13" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="14" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -5993,13 +6061,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0272D98A-080C-3945-A7E0-CB54FB3A65A9}">
-  <dimension ref="A1:V597"/>
+  <dimension ref="A1:V601"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="8" ySplit="1" topLeftCell="T278" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="8" ySplit="1" topLeftCell="T61" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E280" sqref="E280"/>
+      <selection pane="bottomRight" activeCell="B95" sqref="B95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -29256,11 +29324,11 @@
         <v>patient-privacy-and-security</v>
       </c>
       <c r="O589" s="10" t="str">
-        <f t="shared" ref="O589:O597" si="31">IF(ISNUMBER(SEARCH("MAY", C589)), "MAY", IF(ISNUMBER(SEARCH("SHOULD", C589)), "SHOULD", IF(ISNUMBER(SEARCH("SHALL", C589)), "SHALL", IF(ISNUMBER(SEARCH("SHOULD NOT", C589)), "SHOULD NOT", IF(ISNUMBER(SEARCH("SHALL NOT", C589)), "SHALL NOT", "")))))</f>
+        <f t="shared" ref="O589:O601" si="31">IF(ISNUMBER(SEARCH("MAY", C589)), "MAY", IF(ISNUMBER(SEARCH("SHOULD", C589)), "SHOULD", IF(ISNUMBER(SEARCH("SHALL", C589)), "SHALL", IF(ISNUMBER(SEARCH("SHOULD NOT", C589)), "SHOULD NOT", IF(ISNUMBER(SEARCH("SHALL NOT", C589)), "SHALL NOT", "")))))</f>
         <v>MAY</v>
       </c>
       <c r="P589" s="10" t="str">
-        <f t="shared" ref="P589:P597" si="32">IF(ISNUMBER(SEARCH("server", C589)), "Server", IF(ISNUMBER(SEARCH("Server", C589)), "Server", IF(ISNUMBER(SEARCH("client", C589)), "Client", IF(ISNUMBER(SEARCH("Client", C589)), "Client", IF(ISNUMBER(SEARCH("US Core Responder", C589)), "Server", IF(ISNUMBER(SEARCH("US Core Requestor", C589)), "Client", ""))))))</f>
+        <f t="shared" ref="P589:P601" si="32">IF(ISNUMBER(SEARCH("server", C589)), "Server", IF(ISNUMBER(SEARCH("Server", C589)), "Server", IF(ISNUMBER(SEARCH("client", C589)), "Client", IF(ISNUMBER(SEARCH("Client", C589)), "Client", IF(ISNUMBER(SEARCH("US Core Responder", C589)), "Server", IF(ISNUMBER(SEARCH("US Core Requestor", C589)), "Client", ""))))))</f>
         <v/>
       </c>
     </row>
@@ -29359,27 +29427,27 @@
         <v>mandatory-and-must-support-data-elements</v>
       </c>
       <c r="O592" s="10" t="str">
-        <f t="shared" ref="O592" si="33">IF(ISNUMBER(SEARCH("MAY", C592)), "MAY", IF(ISNUMBER(SEARCH("SHOULD", C592)), "SHOULD", IF(ISNUMBER(SEARCH("SHALL", C592)), "SHALL", IF(ISNUMBER(SEARCH("SHOULD NOT", C592)), "SHOULD NOT", IF(ISNUMBER(SEARCH("SHALL NOT", C592)), "SHALL NOT", "")))))</f>
+        <f t="shared" ref="O592:O594" si="33">IF(ISNUMBER(SEARCH("MAY", C592)), "MAY", IF(ISNUMBER(SEARCH("SHOULD", C592)), "SHOULD", IF(ISNUMBER(SEARCH("SHALL", C592)), "SHALL", IF(ISNUMBER(SEARCH("SHOULD NOT", C592)), "SHOULD NOT", IF(ISNUMBER(SEARCH("SHALL NOT", C592)), "SHALL NOT", "")))))</f>
         <v/>
       </c>
       <c r="P592" s="10" t="str">
-        <f t="shared" ref="P592" si="34">IF(ISNUMBER(SEARCH("server", C592)), "Server", IF(ISNUMBER(SEARCH("Server", C592)), "Server", IF(ISNUMBER(SEARCH("client", C592)), "Client", IF(ISNUMBER(SEARCH("Client", C592)), "Client", IF(ISNUMBER(SEARCH("US Core Responder", C592)), "Server", IF(ISNUMBER(SEARCH("US Core Requestor", C592)), "Client", ""))))))</f>
+        <f t="shared" ref="P592:P594" si="34">IF(ISNUMBER(SEARCH("server", C592)), "Server", IF(ISNUMBER(SEARCH("Server", C592)), "Server", IF(ISNUMBER(SEARCH("client", C592)), "Client", IF(ISNUMBER(SEARCH("Client", C592)), "Client", IF(ISNUMBER(SEARCH("US Core Responder", C592)), "Server", IF(ISNUMBER(SEARCH("US Core Requestor", C592)), "Client", ""))))))</f>
         <v/>
       </c>
       <c r="U592" s="10"/>
     </row>
-    <row r="593" spans="1:21" ht="136" x14ac:dyDescent="0.2">
+    <row r="593" spans="1:22" ht="34" x14ac:dyDescent="0.2">
       <c r="A593" s="7">
-        <v>700</v>
+        <v>585</v>
       </c>
       <c r="B593" s="23" t="s">
-        <v>327</v>
+        <v>1062</v>
       </c>
       <c r="C593" s="8" t="s">
-        <v>1011</v>
+        <v>1063</v>
       </c>
       <c r="D593" s="7" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="E593" s="7" t="s">
         <v>33</v>
@@ -29389,147 +29457,303 @@
       </c>
       <c r="M593" s="9" t="str" cm="1">
         <f t="array" ref="M593">PAGE_NAME(B593)</f>
-        <v>StructureDefinition-us-core-condition-encounter-diagnosis</v>
+        <v>StructureDefinition-us-core-allergyintolerance</v>
       </c>
       <c r="N593" s="9" t="str" cm="1">
         <f t="array" ref="N593">SECTION_NAME(B593)</f>
+        <v>mandatory-and-must-support-data-elements</v>
+      </c>
+      <c r="O593" s="10" t="str">
+        <f t="shared" si="33"/>
+        <v/>
+      </c>
+      <c r="P593" s="10" t="str">
+        <f t="shared" si="34"/>
+        <v/>
+      </c>
+      <c r="T593" s="10"/>
+      <c r="V593" s="13"/>
+    </row>
+    <row r="594" spans="1:22" ht="34" x14ac:dyDescent="0.2">
+      <c r="A594" s="7">
+        <v>586</v>
+      </c>
+      <c r="B594" s="23" t="s">
+        <v>1062</v>
+      </c>
+      <c r="C594" s="8" t="s">
+        <v>1064</v>
+      </c>
+      <c r="D594" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E594" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G594" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="M594" s="9" t="str" cm="1">
+        <f t="array" ref="M594">PAGE_NAME(B594)</f>
+        <v>StructureDefinition-us-core-allergyintolerance</v>
+      </c>
+      <c r="N594" s="9" t="str" cm="1">
+        <f t="array" ref="N594">SECTION_NAME(B594)</f>
+        <v>mandatory-and-must-support-data-elements</v>
+      </c>
+      <c r="O594" s="10" t="str">
+        <f t="shared" si="33"/>
+        <v/>
+      </c>
+      <c r="P594" s="10" t="str">
+        <f t="shared" si="34"/>
+        <v/>
+      </c>
+      <c r="T594" s="10"/>
+      <c r="V594" s="13"/>
+    </row>
+    <row r="595" spans="1:22" ht="34" x14ac:dyDescent="0.2">
+      <c r="A595" s="7">
+        <v>587</v>
+      </c>
+      <c r="B595" s="72" t="s">
+        <v>1062</v>
+      </c>
+      <c r="C595" s="73" t="s">
+        <v>1065</v>
+      </c>
+      <c r="D595" s="74" t="s">
+        <v>32</v>
+      </c>
+      <c r="E595" s="74" t="s">
+        <v>33</v>
+      </c>
+      <c r="F595" s="75"/>
+      <c r="G595" s="74" t="b">
+        <v>0</v>
+      </c>
+      <c r="H595" s="76"/>
+      <c r="I595" s="77"/>
+      <c r="J595" s="77"/>
+      <c r="K595" s="77"/>
+      <c r="L595" s="77"/>
+      <c r="M595" s="78" t="s">
+        <v>1066</v>
+      </c>
+      <c r="N595" s="78" t="s">
+        <v>1067</v>
+      </c>
+      <c r="O595" s="79"/>
+      <c r="P595" s="79"/>
+      <c r="Q595" s="79"/>
+      <c r="R595" s="79"/>
+      <c r="S595" s="76"/>
+      <c r="T595" s="79"/>
+      <c r="U595" s="76"/>
+      <c r="V595" s="76"/>
+    </row>
+    <row r="596" spans="1:22" ht="34" x14ac:dyDescent="0.2">
+      <c r="A596" s="7">
+        <v>588</v>
+      </c>
+      <c r="B596" s="72" t="s">
+        <v>1062</v>
+      </c>
+      <c r="C596" s="73" t="s">
+        <v>1068</v>
+      </c>
+      <c r="D596" s="74" t="s">
+        <v>32</v>
+      </c>
+      <c r="E596" s="74" t="s">
+        <v>33</v>
+      </c>
+      <c r="F596" s="75"/>
+      <c r="G596" s="74" t="b">
+        <v>0</v>
+      </c>
+      <c r="H596" s="76"/>
+      <c r="I596" s="77"/>
+      <c r="J596" s="77"/>
+      <c r="K596" s="77"/>
+      <c r="L596" s="77"/>
+      <c r="M596" s="78" t="s">
+        <v>1066</v>
+      </c>
+      <c r="N596" s="78" t="s">
+        <v>1067</v>
+      </c>
+      <c r="O596" s="79"/>
+      <c r="P596" s="79"/>
+      <c r="Q596" s="79"/>
+      <c r="R596" s="79"/>
+      <c r="S596" s="76"/>
+      <c r="T596" s="79"/>
+      <c r="U596" s="76"/>
+      <c r="V596" s="76"/>
+    </row>
+    <row r="597" spans="1:22" ht="136" x14ac:dyDescent="0.2">
+      <c r="A597" s="7">
+        <v>700</v>
+      </c>
+      <c r="B597" s="23" t="s">
+        <v>327</v>
+      </c>
+      <c r="C597" s="8" t="s">
+        <v>1011</v>
+      </c>
+      <c r="D597" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E597" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G597" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="M597" s="9" t="str" cm="1">
+        <f t="array" ref="M597">PAGE_NAME(B597)</f>
+        <v>StructureDefinition-us-core-condition-encounter-diagnosis</v>
+      </c>
+      <c r="N597" s="9" t="str" cm="1">
+        <f t="array" ref="N597">SECTION_NAME(B597)</f>
         <v>notes</v>
       </c>
-      <c r="O593" s="10" t="str">
+      <c r="O597" s="10" t="str">
         <f t="shared" si="31"/>
         <v>MAY</v>
       </c>
-      <c r="P593" s="10" t="str">
+      <c r="P597" s="10" t="str">
         <f t="shared" si="32"/>
         <v>Server</v>
       </c>
     </row>
-    <row r="594" spans="1:21" ht="136" x14ac:dyDescent="0.2">
-      <c r="A594" s="7">
+    <row r="598" spans="1:22" ht="136" x14ac:dyDescent="0.2">
+      <c r="A598" s="7">
         <v>701</v>
       </c>
-      <c r="B594" s="23" t="s">
+      <c r="B598" s="23" t="s">
         <v>327</v>
       </c>
-      <c r="C594" s="8" t="s">
+      <c r="C598" s="8" t="s">
         <v>1012</v>
       </c>
-      <c r="D594" s="7" t="s">
+      <c r="D598" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="E594" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="G594" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="M594" s="9" t="str" cm="1">
-        <f t="array" ref="M594">PAGE_NAME(B594)</f>
+      <c r="E598" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G598" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="M598" s="9" t="str" cm="1">
+        <f t="array" ref="M598">PAGE_NAME(B598)</f>
         <v>StructureDefinition-us-core-condition-encounter-diagnosis</v>
       </c>
-      <c r="N594" s="9" t="str" cm="1">
-        <f t="array" ref="N594">SECTION_NAME(B594)</f>
+      <c r="N598" s="9" t="str" cm="1">
+        <f t="array" ref="N598">SECTION_NAME(B598)</f>
         <v>notes</v>
       </c>
-      <c r="O594" s="10" t="str">
+      <c r="O598" s="10" t="str">
         <f t="shared" si="31"/>
         <v>MAY</v>
       </c>
-      <c r="P594" s="10" t="str">
+      <c r="P598" s="10" t="str">
         <f t="shared" si="32"/>
         <v>Server</v>
       </c>
     </row>
-    <row r="595" spans="1:21" ht="51" x14ac:dyDescent="0.2">
-      <c r="A595" s="7">
+    <row r="599" spans="1:22" ht="51" x14ac:dyDescent="0.2">
+      <c r="A599" s="7">
         <v>702</v>
       </c>
-      <c r="B595" s="23" t="s">
+      <c r="B599" s="23" t="s">
         <v>1013</v>
       </c>
-      <c r="C595" s="8" t="s">
+      <c r="C599" s="8" t="s">
         <v>1014</v>
       </c>
-      <c r="D595" s="7" t="s">
+      <c r="D599" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="E595" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="G595" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="M595" s="9" t="str" cm="1">
-        <f t="array" ref="M595">PAGE_NAME(B595)</f>
+      <c r="E599" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G599" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="M599" s="9" t="str" cm="1">
+        <f t="array" ref="M599">PAGE_NAME(B599)</f>
         <v>StructureDefinition-us-core-practitionerrole</v>
       </c>
-      <c r="N595" s="9" t="str" cm="1">
-        <f t="array" ref="N595">SECTION_NAME(B595)</f>
+      <c r="N599" s="9" t="str" cm="1">
+        <f t="array" ref="N599">SECTION_NAME(B599)</f>
         <v>mandatory-and-must-support-data-elements</v>
       </c>
-      <c r="O595" s="10" t="str">
+      <c r="O599" s="10" t="str">
         <f t="shared" si="31"/>
         <v>SHOULD</v>
       </c>
-      <c r="P595" s="10" t="str">
+      <c r="P599" s="10" t="str">
         <f t="shared" si="32"/>
         <v/>
       </c>
-      <c r="U595" s="13" t="s">
+      <c r="U599" s="13" t="s">
         <v>1015</v>
       </c>
     </row>
-    <row r="596" spans="1:21" ht="51" x14ac:dyDescent="0.2">
-      <c r="A596" s="7">
+    <row r="600" spans="1:22" ht="51" x14ac:dyDescent="0.2">
+      <c r="A600" s="7">
         <v>703</v>
       </c>
-      <c r="B596" s="23" t="s">
+      <c r="B600" s="23" t="s">
         <v>1013</v>
       </c>
-      <c r="C596" s="8" t="s">
+      <c r="C600" s="8" t="s">
         <v>1016</v>
       </c>
-      <c r="D596" s="7" t="s">
+      <c r="D600" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="E596" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="G596" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="M596" s="9" t="str" cm="1">
-        <f t="array" ref="M596">PAGE_NAME(B596)</f>
+      <c r="E600" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G600" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="M600" s="9" t="str" cm="1">
+        <f t="array" ref="M600">PAGE_NAME(B600)</f>
         <v>StructureDefinition-us-core-practitionerrole</v>
       </c>
-      <c r="N596" s="9" t="str" cm="1">
-        <f t="array" ref="N596">SECTION_NAME(B596)</f>
+      <c r="N600" s="9" t="str" cm="1">
+        <f t="array" ref="N600">SECTION_NAME(B600)</f>
         <v>mandatory-and-must-support-data-elements</v>
       </c>
-      <c r="O596" s="10" t="str">
+      <c r="O600" s="10" t="str">
         <f t="shared" si="31"/>
         <v>SHOULD</v>
       </c>
-      <c r="P596" s="10" t="str">
+      <c r="P600" s="10" t="str">
         <f t="shared" si="32"/>
         <v/>
       </c>
-      <c r="U596" s="13" t="s">
+      <c r="U600" s="13" t="s">
         <v>1017</v>
       </c>
     </row>
-    <row r="597" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="O597" s="10" t="str">
+    <row r="601" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="O601" s="10" t="str">
         <f t="shared" si="31"/>
         <v/>
       </c>
-      <c r="P597" s="10" t="str">
+      <c r="P601" s="10" t="str">
         <f t="shared" si="32"/>
         <v/>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:U597" xr:uid="{0272D98A-080C-3945-A7E0-CB54FB3A65A9}"/>
+  <autoFilter ref="A1:U601" xr:uid="{0272D98A-080C-3945-A7E0-CB54FB3A65A9}"/>
   <phoneticPr fontId="19" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="B590" r:id="rId1" location="current-binding-for-coded-elements" display="https://www.hl7.org/fhir/us/core/general-requirements.html#current-binding-for-coded-elements" xr:uid="{C85EAD83-E2C6-4B4C-91F6-5EEB41B6CA95}"/>
@@ -29548,19 +29772,19 @@
           <x14:formula1>
             <xm:f>'Column Data'!$B$2:$B$3</xm:f>
           </x14:formula1>
-          <xm:sqref>G1:G257 G259:G589 G593:G1048576</xm:sqref>
+          <xm:sqref>G1:G257 G259:G589 G597:G1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F4FB27A2-804E-CB49-B85C-BBEE0C688B4F}">
           <x14:formula1>
             <xm:f>'Column Data'!$D$2:$D$4</xm:f>
           </x14:formula1>
-          <xm:sqref>I593:I1048576 I2:I589 K593:K1048576 K163:K398 K400:K412 K2:K138 K414:K418 K425:K589</xm:sqref>
+          <xm:sqref>I597:I1048576 I2:I589 K597:K1048576 K163:K398 K400:K412 K2:K138 K414:K418 K425:K589</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4866B9BF-5615-6646-965F-909D4D65F2A5}">
           <x14:formula1>
             <xm:f>'Column Data'!$A$2:$A$7</xm:f>
           </x14:formula1>
-          <xm:sqref>D2:D589 D593:D1048576</xm:sqref>
+          <xm:sqref>D2:D589 D597:D1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -29841,28 +30065,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="b5a44311-ed64-4a72-909f-c9dc6973bde2" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="eebd8b74-b9de-41b2-9247-c010c4973c2b">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <Description xmlns="eebd8b74-b9de-41b2-9247-c010c4973c2b" xsi:nil="true"/>
-    <SortOrder xmlns="eebd8b74-b9de-41b2-9247-c010c4973c2b" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EC335ED7BB179244BF94A0DFE64544DC" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d3a0f66abe5d2a0564332877ab55d3f7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="eebd8b74-b9de-41b2-9247-c010c4973c2b" xmlns:ns3="b7009bbd-f938-489b-a530-f05273710fff" xmlns:ns4="b5a44311-ed64-4a72-909f-c9dc6973bde2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ec7ca2ee893ff8a0f61d4046c6461645" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="eebd8b74-b9de-41b2-9247-c010c4973c2b"/>
@@ -30116,10 +30318,44 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="b5a44311-ed64-4a72-909f-c9dc6973bde2" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="eebd8b74-b9de-41b2-9247-c010c4973c2b">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <Description xmlns="eebd8b74-b9de-41b2-9247-c010c4973c2b" xsi:nil="true"/>
+    <SortOrder xmlns="eebd8b74-b9de-41b2-9247-c010c4973c2b" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA84097F-5807-4DCF-92C6-48C9EE26CFB8}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C0B0A19-6928-4F0B-831A-5B9FDDD3F6CE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="eebd8b74-b9de-41b2-9247-c010c4973c2b"/>
+    <ds:schemaRef ds:uri="b7009bbd-f938-489b-a530-f05273710fff"/>
+    <ds:schemaRef ds:uri="b5a44311-ed64-4a72-909f-c9dc6973bde2"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -30143,21 +30379,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C0B0A19-6928-4F0B-831A-5B9FDDD3F6CE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA84097F-5807-4DCF-92C6-48C9EE26CFB8}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="eebd8b74-b9de-41b2-9247-c010c4973c2b"/>
-    <ds:schemaRef ds:uri="b7009bbd-f938-489b-a530-f05273710fff"/>
-    <ds:schemaRef ds:uri="b5a44311-ed64-4a72-909f-c9dc6973bde2"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
deprecated 'must have' requirements for allergy intollerance as these are in the structure definition and are unnecessary to reference separately. Removed references to these requirements. Regenerated everything.
</commit_message>
<xml_diff>
--- a/lib/us_core_test_kit/requirements/hl7.fhir.us.core_6.1.0_reqs.xlsx
+++ b/lib/us_core_test_kit/requirements/hl7.fhir.us.core_6.1.0_reqs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/edeyoung/Documents/inferno/us-core-test-kit/lib/us_core_test_kit/requirements/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{821C9270-6E16-7046-850B-C2AF8D885195}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B719ED2-74F4-5244-8A3F-99FB6C6180AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1780" yWindow="760" windowWidth="27360" windowHeight="18880" firstSheet="1" activeTab="1" xr2:uid="{D251129A-65BB-5042-909C-749E11B8C0B0}"/>
   </bookViews>
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -99,7 +99,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3065" uniqueCount="1069">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3068" uniqueCount="1070">
   <si>
     <r>
       <rPr>
@@ -4898,6 +4898,9 @@
   </si>
   <si>
     <t>Each AllergyIntolerance Must Support: a reaction manifestation</t>
+  </si>
+  <si>
+    <t>Deprecated because this is in the structured definition and unnecessary as a separate requirement.</t>
   </si>
 </sst>
 </file>
@@ -5595,6 +5598,22 @@
     <xf numFmtId="0" fontId="24" fillId="11" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="13" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="14" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -5613,22 +5632,6 @@
     <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="24" fillId="12" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="12" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="12" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="13" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="14" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -6002,14 +6005,14 @@
       <c r="C3" s="28"/>
     </row>
     <row r="4" spans="1:3" ht="409.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="66" t="s">
+      <c r="A4" s="74" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="47"/>
       <c r="C4" s="29"/>
     </row>
     <row r="5" spans="1:3" ht="258" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="66"/>
+      <c r="A5" s="74"/>
       <c r="B5" s="48"/>
       <c r="C5" s="28"/>
     </row>
@@ -6021,19 +6024,19 @@
       <c r="C6" s="50"/>
     </row>
     <row r="7" spans="1:3" ht="98" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="67" t="s">
+      <c r="A7" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="68"/>
+      <c r="B7" s="76"/>
       <c r="C7" s="46"/>
     </row>
     <row r="8" spans="1:3" ht="126" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="67"/>
-      <c r="B8" s="69"/>
+      <c r="A8" s="75"/>
+      <c r="B8" s="77"/>
       <c r="C8" s="46"/>
     </row>
     <row r="9" spans="1:3" ht="68" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="66"/>
+      <c r="A9" s="74"/>
       <c r="B9" s="51"/>
       <c r="C9" s="46"/>
     </row>
@@ -6064,10 +6067,10 @@
   <dimension ref="A1:V601"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="8" ySplit="1" topLeftCell="T61" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="8" ySplit="1" topLeftCell="T591" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B95" sqref="B95"/>
+      <selection pane="bottomRight" activeCell="E594" sqref="E594"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -18815,7 +18818,7 @@
       </c>
       <c r="U311" s="63"/>
     </row>
-    <row r="312" spans="1:21" ht="17" x14ac:dyDescent="0.2">
+    <row r="312" spans="1:21" ht="51" x14ac:dyDescent="0.2">
       <c r="A312" s="7">
         <v>304</v>
       </c>
@@ -18826,7 +18829,7 @@
         <v>595</v>
       </c>
       <c r="D312" s="7" t="s">
-        <v>32</v>
+        <v>87</v>
       </c>
       <c r="E312" s="7" t="s">
         <v>33</v>
@@ -18850,6 +18853,9 @@
         <f t="shared" si="16"/>
         <v/>
       </c>
+      <c r="T312" s="56" t="s">
+        <v>1069</v>
+      </c>
       <c r="U312" s="63"/>
     </row>
     <row r="313" spans="1:21" ht="102" x14ac:dyDescent="0.2">
@@ -29436,7 +29442,7 @@
       </c>
       <c r="U592" s="10"/>
     </row>
-    <row r="593" spans="1:22" ht="34" x14ac:dyDescent="0.2">
+    <row r="593" spans="1:22" ht="51" x14ac:dyDescent="0.2">
       <c r="A593" s="7">
         <v>585</v>
       </c>
@@ -29447,7 +29453,7 @@
         <v>1063</v>
       </c>
       <c r="D593" s="7" t="s">
-        <v>32</v>
+        <v>87</v>
       </c>
       <c r="E593" s="7" t="s">
         <v>33</v>
@@ -29471,10 +29477,12 @@
         <f t="shared" si="34"/>
         <v/>
       </c>
-      <c r="T593" s="10"/>
+      <c r="T593" s="56" t="s">
+        <v>1069</v>
+      </c>
       <c r="V593" s="13"/>
     </row>
-    <row r="594" spans="1:22" ht="34" x14ac:dyDescent="0.2">
+    <row r="594" spans="1:22" ht="51" x14ac:dyDescent="0.2">
       <c r="A594" s="7">
         <v>586</v>
       </c>
@@ -29485,7 +29493,7 @@
         <v>1064</v>
       </c>
       <c r="D594" s="7" t="s">
-        <v>32</v>
+        <v>87</v>
       </c>
       <c r="E594" s="7" t="s">
         <v>33</v>
@@ -29509,88 +29517,90 @@
         <f t="shared" si="34"/>
         <v/>
       </c>
-      <c r="T594" s="10"/>
+      <c r="T594" s="56" t="s">
+        <v>1069</v>
+      </c>
       <c r="V594" s="13"/>
     </row>
     <row r="595" spans="1:22" ht="34" x14ac:dyDescent="0.2">
       <c r="A595" s="7">
         <v>587</v>
       </c>
-      <c r="B595" s="72" t="s">
+      <c r="B595" s="66" t="s">
         <v>1062</v>
       </c>
-      <c r="C595" s="73" t="s">
+      <c r="C595" s="67" t="s">
         <v>1065</v>
       </c>
-      <c r="D595" s="74" t="s">
+      <c r="D595" s="68" t="s">
         <v>32</v>
       </c>
-      <c r="E595" s="74" t="s">
-        <v>33</v>
-      </c>
-      <c r="F595" s="75"/>
-      <c r="G595" s="74" t="b">
-        <v>0</v>
-      </c>
-      <c r="H595" s="76"/>
-      <c r="I595" s="77"/>
-      <c r="J595" s="77"/>
-      <c r="K595" s="77"/>
-      <c r="L595" s="77"/>
-      <c r="M595" s="78" t="s">
+      <c r="E595" s="68" t="s">
+        <v>33</v>
+      </c>
+      <c r="F595" s="69"/>
+      <c r="G595" s="68" t="b">
+        <v>0</v>
+      </c>
+      <c r="H595" s="70"/>
+      <c r="I595" s="71"/>
+      <c r="J595" s="71"/>
+      <c r="K595" s="71"/>
+      <c r="L595" s="71"/>
+      <c r="M595" s="72" t="s">
         <v>1066</v>
       </c>
-      <c r="N595" s="78" t="s">
+      <c r="N595" s="72" t="s">
         <v>1067</v>
       </c>
-      <c r="O595" s="79"/>
-      <c r="P595" s="79"/>
-      <c r="Q595" s="79"/>
-      <c r="R595" s="79"/>
-      <c r="S595" s="76"/>
-      <c r="T595" s="79"/>
-      <c r="U595" s="76"/>
-      <c r="V595" s="76"/>
+      <c r="O595" s="73"/>
+      <c r="P595" s="73"/>
+      <c r="Q595" s="73"/>
+      <c r="R595" s="73"/>
+      <c r="S595" s="70"/>
+      <c r="T595" s="73"/>
+      <c r="U595" s="70"/>
+      <c r="V595" s="70"/>
     </row>
     <row r="596" spans="1:22" ht="34" x14ac:dyDescent="0.2">
       <c r="A596" s="7">
         <v>588</v>
       </c>
-      <c r="B596" s="72" t="s">
+      <c r="B596" s="66" t="s">
         <v>1062</v>
       </c>
-      <c r="C596" s="73" t="s">
+      <c r="C596" s="67" t="s">
         <v>1068</v>
       </c>
-      <c r="D596" s="74" t="s">
+      <c r="D596" s="68" t="s">
         <v>32</v>
       </c>
-      <c r="E596" s="74" t="s">
-        <v>33</v>
-      </c>
-      <c r="F596" s="75"/>
-      <c r="G596" s="74" t="b">
-        <v>0</v>
-      </c>
-      <c r="H596" s="76"/>
-      <c r="I596" s="77"/>
-      <c r="J596" s="77"/>
-      <c r="K596" s="77"/>
-      <c r="L596" s="77"/>
-      <c r="M596" s="78" t="s">
+      <c r="E596" s="68" t="s">
+        <v>33</v>
+      </c>
+      <c r="F596" s="69"/>
+      <c r="G596" s="68" t="b">
+        <v>0</v>
+      </c>
+      <c r="H596" s="70"/>
+      <c r="I596" s="71"/>
+      <c r="J596" s="71"/>
+      <c r="K596" s="71"/>
+      <c r="L596" s="71"/>
+      <c r="M596" s="72" t="s">
         <v>1066</v>
       </c>
-      <c r="N596" s="78" t="s">
+      <c r="N596" s="72" t="s">
         <v>1067</v>
       </c>
-      <c r="O596" s="79"/>
-      <c r="P596" s="79"/>
-      <c r="Q596" s="79"/>
-      <c r="R596" s="79"/>
-      <c r="S596" s="76"/>
-      <c r="T596" s="79"/>
-      <c r="U596" s="76"/>
-      <c r="V596" s="76"/>
+      <c r="O596" s="73"/>
+      <c r="P596" s="73"/>
+      <c r="Q596" s="73"/>
+      <c r="R596" s="73"/>
+      <c r="S596" s="70"/>
+      <c r="T596" s="73"/>
+      <c r="U596" s="70"/>
+      <c r="V596" s="70"/>
     </row>
     <row r="597" spans="1:22" ht="136" x14ac:dyDescent="0.2">
       <c r="A597" s="7">
@@ -29807,14 +29817,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="409.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="70" t="s">
+      <c r="A1" s="78" t="s">
         <v>1018</v>
       </c>
-      <c r="B1" s="71"/>
+      <c r="B1" s="79"/>
     </row>
     <row r="2" spans="1:2" ht="82.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="71"/>
-      <c r="B2" s="71"/>
+      <c r="A2" s="79"/>
+      <c r="B2" s="79"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="15" t="s">
@@ -30065,6 +30075,28 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="b5a44311-ed64-4a72-909f-c9dc6973bde2" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="eebd8b74-b9de-41b2-9247-c010c4973c2b">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <Description xmlns="eebd8b74-b9de-41b2-9247-c010c4973c2b" xsi:nil="true"/>
+    <SortOrder xmlns="eebd8b74-b9de-41b2-9247-c010c4973c2b" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EC335ED7BB179244BF94A0DFE64544DC" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d3a0f66abe5d2a0564332877ab55d3f7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="eebd8b74-b9de-41b2-9247-c010c4973c2b" xmlns:ns3="b7009bbd-f938-489b-a530-f05273710fff" xmlns:ns4="b5a44311-ed64-4a72-909f-c9dc6973bde2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ec7ca2ee893ff8a0f61d4046c6461645" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="eebd8b74-b9de-41b2-9247-c010c4973c2b"/>
@@ -30318,44 +30350,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="b5a44311-ed64-4a72-909f-c9dc6973bde2" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="eebd8b74-b9de-41b2-9247-c010c4973c2b">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <Description xmlns="eebd8b74-b9de-41b2-9247-c010c4973c2b" xsi:nil="true"/>
-    <SortOrder xmlns="eebd8b74-b9de-41b2-9247-c010c4973c2b" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C0B0A19-6928-4F0B-831A-5B9FDDD3F6CE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA84097F-5807-4DCF-92C6-48C9EE26CFB8}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="eebd8b74-b9de-41b2-9247-c010c4973c2b"/>
-    <ds:schemaRef ds:uri="b7009bbd-f938-489b-a530-f05273710fff"/>
-    <ds:schemaRef ds:uri="b5a44311-ed64-4a72-909f-c9dc6973bde2"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -30379,9 +30377,21 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA84097F-5807-4DCF-92C6-48C9EE26CFB8}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C0B0A19-6928-4F0B-831A-5B9FDDD3F6CE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="eebd8b74-b9de-41b2-9247-c010c4973c2b"/>
+    <ds:schemaRef ds:uri="b7009bbd-f938-489b-a530-f05273710fff"/>
+    <ds:schemaRef ds:uri="b5a44311-ed64-4a72-909f-c9dc6973bde2"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Fi 4210 map v8 requirements (#267)
Mapped US Core v8 requirements. Addressed issues that arose with the underlying requirements spreadsheets and mappings for v6.1.0 and v7.0.0 requirements. Refactored how requirements are mapped to generated tests.
</commit_message>
<xml_diff>
--- a/lib/us_core_test_kit/requirements/hl7.fhir.us.core_6.1.0_reqs.xlsx
+++ b/lib/us_core_test_kit/requirements/hl7.fhir.us.core_6.1.0_reqs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/edeyoung/Documents/inferno/us-core-test-kit/lib/us_core_test_kit/requirements/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF5115A0-60B2-374F-97AE-A6FAC6940F09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B719ED2-74F4-5244-8A3F-99FB6C6180AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1780" yWindow="760" windowWidth="27360" windowHeight="18880" firstSheet="1" activeTab="1" xr2:uid="{D251129A-65BB-5042-909C-749E11B8C0B0}"/>
   </bookViews>
@@ -20,8 +20,8 @@
     <sheet name="Column Data" sheetId="7" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Requirements!$A$1:$U$597</definedName>
-    <definedName name="bottom" localSheetId="1">Requirements!$U$698</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Requirements!$A$1:$U$601</definedName>
+    <definedName name="bottom" localSheetId="1">Requirements!$U$702</definedName>
     <definedName name="EXPLODE" localSheetId="0">_xlfn.LAMBDA(_xlpm.string,_xlfn.MAKEARRAY(1,LEN(_xlpm.string),_xlfn.LAMBDA(_xlpm.r,_xlpm.c,MID(_xlpm.string,_xlpm.c,1))))</definedName>
     <definedName name="EXPLODE">_xlfn.LAMBDA(_xlpm.string,_xlfn.MAKEARRAY(1,LEN(_xlpm.string),_xlfn.LAMBDA(_xlpm.r,_xlpm.c,MID(_xlpm.string,_xlpm.c,1))))</definedName>
     <definedName name="FIND_DUPLICATES" localSheetId="0">_xlfn.LAMBDA(_xlpm.test_word,_xlpm.test_key,_xlpm.words,_xlpm.keys,_xlpm.threshold, _xlfn.LET(_xlpm.duplist,_xlfn._xlws.FILTER(_xlpm.keys,_xlfn.BYROW(_xlpm.words, _xlfn.LAMBDA(_xlpm.word, Info!HAMDIST(INDEX(_xlpm.word,1,1), _xlpm.test_word)&lt;_xlpm.threshold))),_xlfn.SINGLE(_xlfn._xlws.FILTER(_xlpm.duplist,_xlpm.duplist&lt;&gt;_xlpm.test_key,""))))</definedName>
@@ -40,21 +40,21 @@
     <definedName name="root" localSheetId="1">Requirements!$U$551</definedName>
     <definedName name="SECTION_NAME" localSheetId="0">_xlfn.LAMBDA(_xlpm.url,IFERROR(_xlfn.LET(_xlpm.rev_string, Info!STRREV(_xlpm.url), _xlpm.hash_index,FIND("#", _xlpm.rev_string),_xlpm.section, RIGHT(_xlpm.url, _xlpm.hash_index-1),_xlpm.section),""))</definedName>
     <definedName name="SECTION_NAME">_xlfn.LAMBDA(_xlpm.url,IFERROR(_xlfn.LET(_xlpm.rev_string, STRREV(_xlpm.url), _xlpm.hash_index,FIND("#", _xlpm.rev_string),_xlpm.section, RIGHT(_xlpm.url, _xlpm.hash_index-1),_xlpm.section),""))</definedName>
-    <definedName name="ServiceRequest" localSheetId="1">Requirements!$U$601</definedName>
-    <definedName name="ServiceRequest.authoredOn" localSheetId="1">Requirements!$U$616</definedName>
-    <definedName name="ServiceRequest.category" localSheetId="1">Requirements!$U$604</definedName>
-    <definedName name="ServiceRequest.code" localSheetId="1">Requirements!$U$609</definedName>
-    <definedName name="ServiceRequest.intent" localSheetId="1">Requirements!$U$603</definedName>
-    <definedName name="ServiceRequest.occurrence_x_" localSheetId="1">Requirements!$U$612</definedName>
-    <definedName name="ServiceRequest.reasonCode" localSheetId="1">Requirements!$U$618</definedName>
-    <definedName name="ServiceRequest.reasonReference" localSheetId="1">Requirements!$U$620</definedName>
-    <definedName name="ServiceRequest.requester" localSheetId="1">Requirements!$U$617</definedName>
-    <definedName name="ServiceRequest.status" localSheetId="1">Requirements!$U$602</definedName>
-    <definedName name="ServiceRequest.subject" localSheetId="1">Requirements!$U$611</definedName>
+    <definedName name="ServiceRequest" localSheetId="1">Requirements!$U$605</definedName>
+    <definedName name="ServiceRequest.authoredOn" localSheetId="1">Requirements!$U$620</definedName>
+    <definedName name="ServiceRequest.category" localSheetId="1">Requirements!$U$608</definedName>
+    <definedName name="ServiceRequest.code" localSheetId="1">Requirements!$U$613</definedName>
+    <definedName name="ServiceRequest.intent" localSheetId="1">Requirements!$U$607</definedName>
+    <definedName name="ServiceRequest.occurrence_x_" localSheetId="1">Requirements!$U$616</definedName>
+    <definedName name="ServiceRequest.reasonCode" localSheetId="1">Requirements!$U$622</definedName>
+    <definedName name="ServiceRequest.reasonReference" localSheetId="1">Requirements!$U$624</definedName>
+    <definedName name="ServiceRequest.requester" localSheetId="1">Requirements!$U$621</definedName>
+    <definedName name="ServiceRequest.status" localSheetId="1">Requirements!$U$606</definedName>
+    <definedName name="ServiceRequest.subject" localSheetId="1">Requirements!$U$615</definedName>
     <definedName name="STRREV" localSheetId="0">_xlfn.LAMBDA(_xlpm.word, _xlfn.CONCAT(MID(_xlpm.word,_xlfn.SEQUENCE(LEN(_xlpm.word),,LEN(_xlpm.word),-1),1)))</definedName>
     <definedName name="STRREV">_xlfn.LAMBDA(_xlpm.word, _xlfn.CONCAT(MID(_xlpm.word,_xlfn.SEQUENCE(LEN(_xlpm.word),,LEN(_xlpm.word),-1),1)))</definedName>
     <definedName name="top" localSheetId="1">Requirements!$U$543</definedName>
-    <definedName name="tx" localSheetId="1">Requirements!$U$622</definedName>
+    <definedName name="tx" localSheetId="1">Requirements!$U$626</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -99,7 +99,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3045" uniqueCount="1062">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3068" uniqueCount="1070">
   <si>
     <r>
       <rPr>
@@ -4878,6 +4878,30 @@
   <si>
     <t>Duplicate to req 1</t>
   </si>
+  <si>
+    <t>https://hl7.org/fhir/us/core/STU7/StructureDefinition-us-core-allergyintolerance.html#mandatory-and-must-support-data-elements</t>
+  </si>
+  <si>
+    <t>Each AllergyIntolerance Must Have: a clinical status of the allergy (e.g., active or resolved)</t>
+  </si>
+  <si>
+    <t>Each AllergyIntolerance Must Have: a code that tells you what the patient is allergic to</t>
+  </si>
+  <si>
+    <t>Each AllergyIntolerance Must Support: a verification status</t>
+  </si>
+  <si>
+    <t>StructureDefinition-us-core-allergyintolerance</t>
+  </si>
+  <si>
+    <t>mandatory-and-must-support-data-elements</t>
+  </si>
+  <si>
+    <t>Each AllergyIntolerance Must Support: a reaction manifestation</t>
+  </si>
+  <si>
+    <t>Deprecated because this is in the structured definition and unnecessary as a separate requirement.</t>
+  </si>
 </sst>
 </file>
 
@@ -5055,7 +5079,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -5122,8 +5146,26 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFF2CC"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFCE4D6"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDEBF7"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="23">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -5393,12 +5435,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFD0CECE"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFD0CECE"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFD0CECE"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5543,6 +5598,22 @@
     <xf numFmtId="0" fontId="24" fillId="11" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="13" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="14" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -5934,14 +6005,14 @@
       <c r="C3" s="28"/>
     </row>
     <row r="4" spans="1:3" ht="409.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="66" t="s">
+      <c r="A4" s="74" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="47"/>
       <c r="C4" s="29"/>
     </row>
     <row r="5" spans="1:3" ht="258" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="66"/>
+      <c r="A5" s="74"/>
       <c r="B5" s="48"/>
       <c r="C5" s="28"/>
     </row>
@@ -5953,19 +6024,19 @@
       <c r="C6" s="50"/>
     </row>
     <row r="7" spans="1:3" ht="98" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="67" t="s">
+      <c r="A7" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="68"/>
+      <c r="B7" s="76"/>
       <c r="C7" s="46"/>
     </row>
     <row r="8" spans="1:3" ht="126" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="67"/>
-      <c r="B8" s="69"/>
+      <c r="A8" s="75"/>
+      <c r="B8" s="77"/>
       <c r="C8" s="46"/>
     </row>
     <row r="9" spans="1:3" ht="68" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="66"/>
+      <c r="A9" s="74"/>
       <c r="B9" s="51"/>
       <c r="C9" s="46"/>
     </row>
@@ -5993,13 +6064,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0272D98A-080C-3945-A7E0-CB54FB3A65A9}">
-  <dimension ref="A1:V597"/>
+  <dimension ref="A1:V601"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="8" ySplit="1" topLeftCell="T278" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="8" ySplit="1" topLeftCell="T591" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E280" sqref="E280"/>
+      <selection pane="bottomRight" activeCell="E594" sqref="E594"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -18747,7 +18818,7 @@
       </c>
       <c r="U311" s="63"/>
     </row>
-    <row r="312" spans="1:21" ht="17" x14ac:dyDescent="0.2">
+    <row r="312" spans="1:21" ht="51" x14ac:dyDescent="0.2">
       <c r="A312" s="7">
         <v>304</v>
       </c>
@@ -18758,7 +18829,7 @@
         <v>595</v>
       </c>
       <c r="D312" s="7" t="s">
-        <v>32</v>
+        <v>87</v>
       </c>
       <c r="E312" s="7" t="s">
         <v>33</v>
@@ -18782,6 +18853,9 @@
         <f t="shared" si="16"/>
         <v/>
       </c>
+      <c r="T312" s="56" t="s">
+        <v>1069</v>
+      </c>
       <c r="U312" s="63"/>
     </row>
     <row r="313" spans="1:21" ht="102" x14ac:dyDescent="0.2">
@@ -29256,11 +29330,11 @@
         <v>patient-privacy-and-security</v>
       </c>
       <c r="O589" s="10" t="str">
-        <f t="shared" ref="O589:O597" si="31">IF(ISNUMBER(SEARCH("MAY", C589)), "MAY", IF(ISNUMBER(SEARCH("SHOULD", C589)), "SHOULD", IF(ISNUMBER(SEARCH("SHALL", C589)), "SHALL", IF(ISNUMBER(SEARCH("SHOULD NOT", C589)), "SHOULD NOT", IF(ISNUMBER(SEARCH("SHALL NOT", C589)), "SHALL NOT", "")))))</f>
+        <f t="shared" ref="O589:O601" si="31">IF(ISNUMBER(SEARCH("MAY", C589)), "MAY", IF(ISNUMBER(SEARCH("SHOULD", C589)), "SHOULD", IF(ISNUMBER(SEARCH("SHALL", C589)), "SHALL", IF(ISNUMBER(SEARCH("SHOULD NOT", C589)), "SHOULD NOT", IF(ISNUMBER(SEARCH("SHALL NOT", C589)), "SHALL NOT", "")))))</f>
         <v>MAY</v>
       </c>
       <c r="P589" s="10" t="str">
-        <f t="shared" ref="P589:P597" si="32">IF(ISNUMBER(SEARCH("server", C589)), "Server", IF(ISNUMBER(SEARCH("Server", C589)), "Server", IF(ISNUMBER(SEARCH("client", C589)), "Client", IF(ISNUMBER(SEARCH("Client", C589)), "Client", IF(ISNUMBER(SEARCH("US Core Responder", C589)), "Server", IF(ISNUMBER(SEARCH("US Core Requestor", C589)), "Client", ""))))))</f>
+        <f t="shared" ref="P589:P601" si="32">IF(ISNUMBER(SEARCH("server", C589)), "Server", IF(ISNUMBER(SEARCH("Server", C589)), "Server", IF(ISNUMBER(SEARCH("client", C589)), "Client", IF(ISNUMBER(SEARCH("Client", C589)), "Client", IF(ISNUMBER(SEARCH("US Core Responder", C589)), "Server", IF(ISNUMBER(SEARCH("US Core Requestor", C589)), "Client", ""))))))</f>
         <v/>
       </c>
     </row>
@@ -29359,27 +29433,27 @@
         <v>mandatory-and-must-support-data-elements</v>
       </c>
       <c r="O592" s="10" t="str">
-        <f t="shared" ref="O592" si="33">IF(ISNUMBER(SEARCH("MAY", C592)), "MAY", IF(ISNUMBER(SEARCH("SHOULD", C592)), "SHOULD", IF(ISNUMBER(SEARCH("SHALL", C592)), "SHALL", IF(ISNUMBER(SEARCH("SHOULD NOT", C592)), "SHOULD NOT", IF(ISNUMBER(SEARCH("SHALL NOT", C592)), "SHALL NOT", "")))))</f>
+        <f t="shared" ref="O592:O594" si="33">IF(ISNUMBER(SEARCH("MAY", C592)), "MAY", IF(ISNUMBER(SEARCH("SHOULD", C592)), "SHOULD", IF(ISNUMBER(SEARCH("SHALL", C592)), "SHALL", IF(ISNUMBER(SEARCH("SHOULD NOT", C592)), "SHOULD NOT", IF(ISNUMBER(SEARCH("SHALL NOT", C592)), "SHALL NOT", "")))))</f>
         <v/>
       </c>
       <c r="P592" s="10" t="str">
-        <f t="shared" ref="P592" si="34">IF(ISNUMBER(SEARCH("server", C592)), "Server", IF(ISNUMBER(SEARCH("Server", C592)), "Server", IF(ISNUMBER(SEARCH("client", C592)), "Client", IF(ISNUMBER(SEARCH("Client", C592)), "Client", IF(ISNUMBER(SEARCH("US Core Responder", C592)), "Server", IF(ISNUMBER(SEARCH("US Core Requestor", C592)), "Client", ""))))))</f>
+        <f t="shared" ref="P592:P594" si="34">IF(ISNUMBER(SEARCH("server", C592)), "Server", IF(ISNUMBER(SEARCH("Server", C592)), "Server", IF(ISNUMBER(SEARCH("client", C592)), "Client", IF(ISNUMBER(SEARCH("Client", C592)), "Client", IF(ISNUMBER(SEARCH("US Core Responder", C592)), "Server", IF(ISNUMBER(SEARCH("US Core Requestor", C592)), "Client", ""))))))</f>
         <v/>
       </c>
       <c r="U592" s="10"/>
     </row>
-    <row r="593" spans="1:21" ht="136" x14ac:dyDescent="0.2">
+    <row r="593" spans="1:22" ht="51" x14ac:dyDescent="0.2">
       <c r="A593" s="7">
-        <v>700</v>
+        <v>585</v>
       </c>
       <c r="B593" s="23" t="s">
-        <v>327</v>
+        <v>1062</v>
       </c>
       <c r="C593" s="8" t="s">
-        <v>1011</v>
+        <v>1063</v>
       </c>
       <c r="D593" s="7" t="s">
-        <v>41</v>
+        <v>87</v>
       </c>
       <c r="E593" s="7" t="s">
         <v>33</v>
@@ -29389,147 +29463,307 @@
       </c>
       <c r="M593" s="9" t="str" cm="1">
         <f t="array" ref="M593">PAGE_NAME(B593)</f>
-        <v>StructureDefinition-us-core-condition-encounter-diagnosis</v>
+        <v>StructureDefinition-us-core-allergyintolerance</v>
       </c>
       <c r="N593" s="9" t="str" cm="1">
         <f t="array" ref="N593">SECTION_NAME(B593)</f>
+        <v>mandatory-and-must-support-data-elements</v>
+      </c>
+      <c r="O593" s="10" t="str">
+        <f t="shared" si="33"/>
+        <v/>
+      </c>
+      <c r="P593" s="10" t="str">
+        <f t="shared" si="34"/>
+        <v/>
+      </c>
+      <c r="T593" s="56" t="s">
+        <v>1069</v>
+      </c>
+      <c r="V593" s="13"/>
+    </row>
+    <row r="594" spans="1:22" ht="51" x14ac:dyDescent="0.2">
+      <c r="A594" s="7">
+        <v>586</v>
+      </c>
+      <c r="B594" s="23" t="s">
+        <v>1062</v>
+      </c>
+      <c r="C594" s="8" t="s">
+        <v>1064</v>
+      </c>
+      <c r="D594" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="E594" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G594" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="M594" s="9" t="str" cm="1">
+        <f t="array" ref="M594">PAGE_NAME(B594)</f>
+        <v>StructureDefinition-us-core-allergyintolerance</v>
+      </c>
+      <c r="N594" s="9" t="str" cm="1">
+        <f t="array" ref="N594">SECTION_NAME(B594)</f>
+        <v>mandatory-and-must-support-data-elements</v>
+      </c>
+      <c r="O594" s="10" t="str">
+        <f t="shared" si="33"/>
+        <v/>
+      </c>
+      <c r="P594" s="10" t="str">
+        <f t="shared" si="34"/>
+        <v/>
+      </c>
+      <c r="T594" s="56" t="s">
+        <v>1069</v>
+      </c>
+      <c r="V594" s="13"/>
+    </row>
+    <row r="595" spans="1:22" ht="34" x14ac:dyDescent="0.2">
+      <c r="A595" s="7">
+        <v>587</v>
+      </c>
+      <c r="B595" s="66" t="s">
+        <v>1062</v>
+      </c>
+      <c r="C595" s="67" t="s">
+        <v>1065</v>
+      </c>
+      <c r="D595" s="68" t="s">
+        <v>32</v>
+      </c>
+      <c r="E595" s="68" t="s">
+        <v>33</v>
+      </c>
+      <c r="F595" s="69"/>
+      <c r="G595" s="68" t="b">
+        <v>0</v>
+      </c>
+      <c r="H595" s="70"/>
+      <c r="I595" s="71"/>
+      <c r="J595" s="71"/>
+      <c r="K595" s="71"/>
+      <c r="L595" s="71"/>
+      <c r="M595" s="72" t="s">
+        <v>1066</v>
+      </c>
+      <c r="N595" s="72" t="s">
+        <v>1067</v>
+      </c>
+      <c r="O595" s="73"/>
+      <c r="P595" s="73"/>
+      <c r="Q595" s="73"/>
+      <c r="R595" s="73"/>
+      <c r="S595" s="70"/>
+      <c r="T595" s="73"/>
+      <c r="U595" s="70"/>
+      <c r="V595" s="70"/>
+    </row>
+    <row r="596" spans="1:22" ht="34" x14ac:dyDescent="0.2">
+      <c r="A596" s="7">
+        <v>588</v>
+      </c>
+      <c r="B596" s="66" t="s">
+        <v>1062</v>
+      </c>
+      <c r="C596" s="67" t="s">
+        <v>1068</v>
+      </c>
+      <c r="D596" s="68" t="s">
+        <v>32</v>
+      </c>
+      <c r="E596" s="68" t="s">
+        <v>33</v>
+      </c>
+      <c r="F596" s="69"/>
+      <c r="G596" s="68" t="b">
+        <v>0</v>
+      </c>
+      <c r="H596" s="70"/>
+      <c r="I596" s="71"/>
+      <c r="J596" s="71"/>
+      <c r="K596" s="71"/>
+      <c r="L596" s="71"/>
+      <c r="M596" s="72" t="s">
+        <v>1066</v>
+      </c>
+      <c r="N596" s="72" t="s">
+        <v>1067</v>
+      </c>
+      <c r="O596" s="73"/>
+      <c r="P596" s="73"/>
+      <c r="Q596" s="73"/>
+      <c r="R596" s="73"/>
+      <c r="S596" s="70"/>
+      <c r="T596" s="73"/>
+      <c r="U596" s="70"/>
+      <c r="V596" s="70"/>
+    </row>
+    <row r="597" spans="1:22" ht="136" x14ac:dyDescent="0.2">
+      <c r="A597" s="7">
+        <v>700</v>
+      </c>
+      <c r="B597" s="23" t="s">
+        <v>327</v>
+      </c>
+      <c r="C597" s="8" t="s">
+        <v>1011</v>
+      </c>
+      <c r="D597" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E597" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G597" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="M597" s="9" t="str" cm="1">
+        <f t="array" ref="M597">PAGE_NAME(B597)</f>
+        <v>StructureDefinition-us-core-condition-encounter-diagnosis</v>
+      </c>
+      <c r="N597" s="9" t="str" cm="1">
+        <f t="array" ref="N597">SECTION_NAME(B597)</f>
         <v>notes</v>
       </c>
-      <c r="O593" s="10" t="str">
+      <c r="O597" s="10" t="str">
         <f t="shared" si="31"/>
         <v>MAY</v>
       </c>
-      <c r="P593" s="10" t="str">
+      <c r="P597" s="10" t="str">
         <f t="shared" si="32"/>
         <v>Server</v>
       </c>
     </row>
-    <row r="594" spans="1:21" ht="136" x14ac:dyDescent="0.2">
-      <c r="A594" s="7">
+    <row r="598" spans="1:22" ht="136" x14ac:dyDescent="0.2">
+      <c r="A598" s="7">
         <v>701</v>
       </c>
-      <c r="B594" s="23" t="s">
+      <c r="B598" s="23" t="s">
         <v>327</v>
       </c>
-      <c r="C594" s="8" t="s">
+      <c r="C598" s="8" t="s">
         <v>1012</v>
       </c>
-      <c r="D594" s="7" t="s">
+      <c r="D598" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="E594" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="G594" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="M594" s="9" t="str" cm="1">
-        <f t="array" ref="M594">PAGE_NAME(B594)</f>
+      <c r="E598" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G598" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="M598" s="9" t="str" cm="1">
+        <f t="array" ref="M598">PAGE_NAME(B598)</f>
         <v>StructureDefinition-us-core-condition-encounter-diagnosis</v>
       </c>
-      <c r="N594" s="9" t="str" cm="1">
-        <f t="array" ref="N594">SECTION_NAME(B594)</f>
+      <c r="N598" s="9" t="str" cm="1">
+        <f t="array" ref="N598">SECTION_NAME(B598)</f>
         <v>notes</v>
       </c>
-      <c r="O594" s="10" t="str">
+      <c r="O598" s="10" t="str">
         <f t="shared" si="31"/>
         <v>MAY</v>
       </c>
-      <c r="P594" s="10" t="str">
+      <c r="P598" s="10" t="str">
         <f t="shared" si="32"/>
         <v>Server</v>
       </c>
     </row>
-    <row r="595" spans="1:21" ht="51" x14ac:dyDescent="0.2">
-      <c r="A595" s="7">
+    <row r="599" spans="1:22" ht="51" x14ac:dyDescent="0.2">
+      <c r="A599" s="7">
         <v>702</v>
       </c>
-      <c r="B595" s="23" t="s">
+      <c r="B599" s="23" t="s">
         <v>1013</v>
       </c>
-      <c r="C595" s="8" t="s">
+      <c r="C599" s="8" t="s">
         <v>1014</v>
       </c>
-      <c r="D595" s="7" t="s">
+      <c r="D599" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="E595" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="G595" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="M595" s="9" t="str" cm="1">
-        <f t="array" ref="M595">PAGE_NAME(B595)</f>
+      <c r="E599" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G599" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="M599" s="9" t="str" cm="1">
+        <f t="array" ref="M599">PAGE_NAME(B599)</f>
         <v>StructureDefinition-us-core-practitionerrole</v>
       </c>
-      <c r="N595" s="9" t="str" cm="1">
-        <f t="array" ref="N595">SECTION_NAME(B595)</f>
+      <c r="N599" s="9" t="str" cm="1">
+        <f t="array" ref="N599">SECTION_NAME(B599)</f>
         <v>mandatory-and-must-support-data-elements</v>
       </c>
-      <c r="O595" s="10" t="str">
+      <c r="O599" s="10" t="str">
         <f t="shared" si="31"/>
         <v>SHOULD</v>
       </c>
-      <c r="P595" s="10" t="str">
+      <c r="P599" s="10" t="str">
         <f t="shared" si="32"/>
         <v/>
       </c>
-      <c r="U595" s="13" t="s">
+      <c r="U599" s="13" t="s">
         <v>1015</v>
       </c>
     </row>
-    <row r="596" spans="1:21" ht="51" x14ac:dyDescent="0.2">
-      <c r="A596" s="7">
+    <row r="600" spans="1:22" ht="51" x14ac:dyDescent="0.2">
+      <c r="A600" s="7">
         <v>703</v>
       </c>
-      <c r="B596" s="23" t="s">
+      <c r="B600" s="23" t="s">
         <v>1013</v>
       </c>
-      <c r="C596" s="8" t="s">
+      <c r="C600" s="8" t="s">
         <v>1016</v>
       </c>
-      <c r="D596" s="7" t="s">
+      <c r="D600" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="E596" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="G596" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="M596" s="9" t="str" cm="1">
-        <f t="array" ref="M596">PAGE_NAME(B596)</f>
+      <c r="E600" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G600" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="M600" s="9" t="str" cm="1">
+        <f t="array" ref="M600">PAGE_NAME(B600)</f>
         <v>StructureDefinition-us-core-practitionerrole</v>
       </c>
-      <c r="N596" s="9" t="str" cm="1">
-        <f t="array" ref="N596">SECTION_NAME(B596)</f>
+      <c r="N600" s="9" t="str" cm="1">
+        <f t="array" ref="N600">SECTION_NAME(B600)</f>
         <v>mandatory-and-must-support-data-elements</v>
       </c>
-      <c r="O596" s="10" t="str">
+      <c r="O600" s="10" t="str">
         <f t="shared" si="31"/>
         <v>SHOULD</v>
       </c>
-      <c r="P596" s="10" t="str">
+      <c r="P600" s="10" t="str">
         <f t="shared" si="32"/>
         <v/>
       </c>
-      <c r="U596" s="13" t="s">
+      <c r="U600" s="13" t="s">
         <v>1017</v>
       </c>
     </row>
-    <row r="597" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="O597" s="10" t="str">
+    <row r="601" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="O601" s="10" t="str">
         <f t="shared" si="31"/>
         <v/>
       </c>
-      <c r="P597" s="10" t="str">
+      <c r="P601" s="10" t="str">
         <f t="shared" si="32"/>
         <v/>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:U597" xr:uid="{0272D98A-080C-3945-A7E0-CB54FB3A65A9}"/>
+  <autoFilter ref="A1:U601" xr:uid="{0272D98A-080C-3945-A7E0-CB54FB3A65A9}"/>
   <phoneticPr fontId="19" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="B590" r:id="rId1" location="current-binding-for-coded-elements" display="https://www.hl7.org/fhir/us/core/general-requirements.html#current-binding-for-coded-elements" xr:uid="{C85EAD83-E2C6-4B4C-91F6-5EEB41B6CA95}"/>
@@ -29548,19 +29782,19 @@
           <x14:formula1>
             <xm:f>'Column Data'!$B$2:$B$3</xm:f>
           </x14:formula1>
-          <xm:sqref>G1:G257 G259:G589 G593:G1048576</xm:sqref>
+          <xm:sqref>G1:G257 G259:G589 G597:G1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F4FB27A2-804E-CB49-B85C-BBEE0C688B4F}">
           <x14:formula1>
             <xm:f>'Column Data'!$D$2:$D$4</xm:f>
           </x14:formula1>
-          <xm:sqref>I593:I1048576 I2:I589 K593:K1048576 K163:K398 K400:K412 K2:K138 K414:K418 K425:K589</xm:sqref>
+          <xm:sqref>I597:I1048576 I2:I589 K597:K1048576 K163:K398 K400:K412 K2:K138 K414:K418 K425:K589</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4866B9BF-5615-6646-965F-909D4D65F2A5}">
           <x14:formula1>
             <xm:f>'Column Data'!$A$2:$A$7</xm:f>
           </x14:formula1>
-          <xm:sqref>D2:D589 D593:D1048576</xm:sqref>
+          <xm:sqref>D2:D589 D597:D1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -29583,14 +29817,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="409.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="70" t="s">
+      <c r="A1" s="78" t="s">
         <v>1018</v>
       </c>
-      <c r="B1" s="71"/>
+      <c r="B1" s="79"/>
     </row>
     <row r="2" spans="1:2" ht="82.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="71"/>
-      <c r="B2" s="71"/>
+      <c r="A2" s="79"/>
+      <c r="B2" s="79"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="15" t="s">

</xml_diff>